<commit_message>
updates survey metadata with EB/95.1 (Mar-Apr 2021)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99D75DD-ACA9-41F4-94B0-C0BDE06A1882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E8BCEB-282D-4DD0-8BD4-CEC01495A6AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="905">
   <si>
     <t>archive_id</t>
   </si>
@@ -2723,6 +2723,18 @@
   </si>
   <si>
     <t>November-December 2020</t>
+  </si>
+  <si>
+    <t>ZA7781</t>
+  </si>
+  <si>
+    <t>95.1</t>
+  </si>
+  <si>
+    <t>March-April 2021</t>
+  </si>
+  <si>
+    <t>European Parliament Spring Survey, Climate Change, and EU Consumer Habits Regarding Fishery and Aquaculture Products</t>
   </si>
 </sst>
 </file>
@@ -3057,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D230"/>
+  <dimension ref="A1:D231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3081,2683 +3093,2683 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="C2" t="s">
-        <v>900</v>
+        <v>903</v>
+      </c>
+      <c r="D2" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>899</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
         <v>121</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C40" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B44" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C46" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D46" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C47" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D47" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C48" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D49" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D50" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C51" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D51" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C52" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D52" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C53" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C54" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D54" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B55" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C55" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D55" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B56" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C56" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D56" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C57" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D57" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B58" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C58" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D58" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B59" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C59" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D59" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B60" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C60" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D60" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B61" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C61" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D61" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B62" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C62" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D62" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B63" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C63" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D63" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B64" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C64" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B65" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C65" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D65" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B66" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C66" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D66" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B67" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C67" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D67" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C68" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D68" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B69" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D69" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B70" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C70" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D70" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B71" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C71" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D71" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B72" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C72" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D72" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B73" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C73" t="s">
         <v>276</v>
       </c>
       <c r="D73" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B74" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C74" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D74" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B75" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C75" t="s">
         <v>283</v>
       </c>
       <c r="D75" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B76" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C76" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D76" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B77" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C77" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D77" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B78" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C78" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D78" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B79" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C79" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D79" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B80" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C80" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D80" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B81" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C81" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D81" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B82" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C82" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D82" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B83" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C83" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D83" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B84" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C84" t="s">
         <v>318</v>
       </c>
       <c r="D84" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B85" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C85" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D85" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B86" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C86" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D86" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B87" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C87" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D87" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B88" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C88" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D88" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B89" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C89" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D89" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B90" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C90" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D90" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B91" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C91" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D91" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B92" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C92" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D92" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B93" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C93" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D93" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B94" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C94" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D94" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B95" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C95" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D95" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B96" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C96" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D96" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B97" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C97" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D97" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B98" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C98" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D98" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B99" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C99" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D99" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B100" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C100" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D100" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B101" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C101" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D101" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B102" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C102" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D102" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B103" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C103" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D103" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B104" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C104" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D104" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B105" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C105" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D105" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B106" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C106" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D106" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B107" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C107" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D107" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B108" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C108" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D108" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B109" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C109" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D109" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B110" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C110" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D110" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B111" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C111" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D111" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B112" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C112" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D112" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B113" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C113" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D113" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B114" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C114" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D114" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B115" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C115" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D115" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B116" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C116" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D116" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B117" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C117" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D117" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B118" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C118" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D118" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B119" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C119" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D119" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B120" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C120" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D120" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B121" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C121" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D121" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B122" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C122" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D122" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B123" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C123" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D123" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B124" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C124" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D124" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B125" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C125" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D125" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B126" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C126" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D126" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B127" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C127" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D127" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B128" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C128" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D128" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B129" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C129" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D129" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B130" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C130" t="s">
         <v>501</v>
       </c>
       <c r="D130" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B131" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C131" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D131" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B132" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C132" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D132" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B133" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C133" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D133" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B134" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C134" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D134" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B135" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C135" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D135" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B136" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C136" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D136" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B137" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C137" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D137" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B138" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C138" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D138" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B139" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C139" t="s">
         <v>536</v>
       </c>
       <c r="D139" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B140" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C140" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D140" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B141" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C141" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D141" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B142" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C142" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D142" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B143" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C143" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D143" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B144" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C144" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D144" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B145" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C145" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D145" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B146" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C146" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D146" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B147" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C147" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D147" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B148" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C148" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D148" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B149" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C149" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D149" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B150" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C150" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D150" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B151" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C151" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D151" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B152" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C152" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D152" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B153" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C153" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D153" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B154" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C154" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D154" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B155" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C155" t="s">
         <v>599</v>
       </c>
       <c r="D155" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B156" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C156" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D156" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B157" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C157" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D157" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B158" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C158" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D158" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B159" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C159" t="s">
         <v>614</v>
       </c>
       <c r="D159" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B160" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C160" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D160" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B161" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C161" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D161" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B162" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C162" t="s">
         <v>625</v>
       </c>
       <c r="D162" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B163" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C163" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D163" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B164" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C164" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D164" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B165" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C165" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D165" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B166" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C166" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D166" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B167" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C167" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D167" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B168" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C168" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D168" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B169" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C169" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D169" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B170" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C170" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D170" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B171" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C171" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D171" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B172" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C172" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D172" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B173" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C173" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D173" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B174" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C174" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D174" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B175" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C175" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D175" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B176" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C176" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D176" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B177" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C177" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D177" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B178" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C178" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D178" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B179" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C179" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D179" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B180" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C180" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D180" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B181" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C181" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D181" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B182" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C182" t="s">
         <v>704</v>
       </c>
       <c r="D182" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B183" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C183" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D183" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B184" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C184" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D184" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B185" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C185" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D185" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B186" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C186" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D186" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B187" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C187" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D187" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B188" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C188" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D188" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B189" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C189" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D189" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B190" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C190" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D190" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B191" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C191" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D191" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B192" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C192" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D192" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B193" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C193" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D193" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B194" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C194" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D194" t="s">
         <v>752</v>
@@ -5765,505 +5777,519 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="B195" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C195" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D195" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B196" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C196" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D196" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B197" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C197" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D197" t="s">
-        <v>600</v>
+        <v>763</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B198" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C198" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D198" t="s">
-        <v>770</v>
+        <v>600</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B199" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C199" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D199" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B200" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C200" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D200" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B201" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C201" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D201" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B202" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C202" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D202" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B203" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C203" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D203" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B204" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C204" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D204" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B205" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C205" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D205" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B206" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C206" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D206" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B207" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C207" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D207" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B208" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C208" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D208" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B209" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C209" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D209" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B210" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C210" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D210" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B211" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C211" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D211" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B212" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C212" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D212" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B213" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C213" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D213" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B214" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="C214" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D214" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B215" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C215" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D215" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B216" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C216" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D216" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B217" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C217" t="s">
         <v>841</v>
       </c>
       <c r="D217" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B218" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C218" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D218" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B219" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C219" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D219" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B220" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C220" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D220" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B221" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C221" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D221" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B222" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C222" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D222" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B223" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C223" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D223" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B224" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C224" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D224" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B225" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C225" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D225" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B226" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C226" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D226" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B227" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C227" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D227" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B228" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C228" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="D228" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B229" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C229" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D229" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>890</v>
+      </c>
+      <c r="B230" t="s">
+        <v>891</v>
+      </c>
+      <c r="C230" t="s">
+        <v>892</v>
+      </c>
+      <c r="D230" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
         <v>894</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>895</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C231" t="s">
         <v>896</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D231" t="s">
         <v>897</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates survey metadata with EB/94.3 (Feb-Mar 2021)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E8BCEB-282D-4DD0-8BD4-CEC01495A6AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14A7059-5420-447F-A62E-F54F069AD161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="909">
   <si>
     <t>archive_id</t>
   </si>
@@ -2735,6 +2735,18 @@
   </si>
   <si>
     <t>European Parliament Spring Survey, Climate Change, and EU Consumer Habits Regarding Fishery and Aquaculture Products</t>
+  </si>
+  <si>
+    <t>ZA7780</t>
+  </si>
+  <si>
+    <t>94.3</t>
+  </si>
+  <si>
+    <t>February - March 2021</t>
+  </si>
+  <si>
+    <t>COVID-19 Pandemic</t>
   </si>
 </sst>
 </file>
@@ -3069,10 +3081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D231"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3107,2683 +3119,2683 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="C3" t="s">
-        <v>900</v>
+        <v>907</v>
+      </c>
+      <c r="D3" t="s">
+        <v>908</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>899</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
         <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C41" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C44" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D44" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D45" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C46" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D46" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D47" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B49" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C49" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C50" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D50" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B51" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C51" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D51" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B52" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D53" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C54" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D54" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B55" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C55" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D55" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C56" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D56" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B57" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C57" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D57" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C58" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D58" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B59" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C59" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D59" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B60" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D60" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C61" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D61" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B62" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C62" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D62" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B63" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C63" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D63" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B64" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C64" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D64" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B65" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C65" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D65" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B66" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D66" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B67" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C67" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D67" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B68" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C68" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D68" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B69" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C69" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D69" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B70" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C70" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D70" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B71" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C71" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D71" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B72" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C72" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D72" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B73" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C73" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D73" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B74" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C74" t="s">
         <v>276</v>
       </c>
       <c r="D74" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B75" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C75" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D75" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B76" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C76" t="s">
         <v>283</v>
       </c>
       <c r="D76" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B77" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C77" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D77" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B78" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C78" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D78" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B79" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C79" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D79" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B80" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C80" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D80" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B81" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C81" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D81" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B82" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C82" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D82" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B83" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C83" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D83" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B84" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C84" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D84" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B85" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C85" t="s">
         <v>318</v>
       </c>
       <c r="D85" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B86" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C86" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D86" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B87" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C87" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D87" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B88" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C88" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D88" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B89" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C89" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D89" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B90" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C90" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D90" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B91" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C91" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D91" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B92" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C92" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D92" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B93" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C93" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D93" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B94" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C94" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D94" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B95" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C95" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D95" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B96" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C96" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D96" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B97" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C97" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D97" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B98" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C98" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D98" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B99" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C99" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D99" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B100" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C100" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D100" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B101" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C101" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D101" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B102" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C102" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D102" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B103" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C103" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D103" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B104" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C104" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D104" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B105" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C105" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D105" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B106" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C106" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D106" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B107" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C107" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D107" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B108" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C108" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D108" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B109" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C109" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D109" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B110" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C110" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D110" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B111" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C111" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D111" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B112" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C112" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D112" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B113" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C113" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D113" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B114" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C114" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D114" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B115" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C115" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D115" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B116" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C116" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D116" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B117" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D117" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B118" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C118" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D118" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B119" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C119" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D119" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B120" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C120" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D120" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B121" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C121" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D121" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B122" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C122" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D122" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B123" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C123" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D123" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B124" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C124" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D124" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B125" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C125" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D125" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B126" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C126" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D126" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B127" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C127" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D127" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B128" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C128" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D128" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B129" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C129" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D129" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B130" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C130" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D130" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B131" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C131" t="s">
         <v>501</v>
       </c>
       <c r="D131" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B132" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C132" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D132" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B133" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C133" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D133" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B134" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C134" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D134" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B135" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C135" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D135" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B136" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C136" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D136" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B137" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C137" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D137" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B138" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C138" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D138" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B139" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C139" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D139" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B140" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C140" t="s">
         <v>536</v>
       </c>
       <c r="D140" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B141" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C141" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D141" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B142" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C142" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D142" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B143" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C143" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D143" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B144" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C144" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D144" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B145" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C145" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D145" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B146" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C146" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D146" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B147" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C147" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D147" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B148" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C148" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D148" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B149" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C149" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D149" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B150" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C150" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D150" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B151" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C151" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D151" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B152" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C152" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D152" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B153" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C153" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D153" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B154" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C154" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D154" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B155" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C155" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D155" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B156" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C156" t="s">
         <v>599</v>
       </c>
       <c r="D156" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B157" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C157" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D157" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B158" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C158" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D158" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B159" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C159" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D159" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B160" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C160" t="s">
         <v>614</v>
       </c>
       <c r="D160" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B161" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C161" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D161" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B162" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C162" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D162" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B163" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C163" t="s">
         <v>625</v>
       </c>
       <c r="D163" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B164" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C164" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D164" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B165" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C165" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D165" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B166" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C166" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D166" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B167" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C167" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D167" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B168" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C168" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D168" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B169" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C169" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D169" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B170" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C170" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D170" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B171" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C171" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D171" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B172" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C172" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D172" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B173" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C173" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D173" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B174" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C174" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D174" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B175" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C175" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D175" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B176" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C176" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D176" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B177" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C177" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D177" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B178" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C178" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D178" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B179" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C179" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D179" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B180" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C180" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D180" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B181" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C181" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D181" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B182" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C182" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D182" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B183" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C183" t="s">
         <v>704</v>
       </c>
       <c r="D183" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B184" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C184" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D184" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B185" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C185" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D185" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B186" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C186" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D186" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B187" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C187" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D187" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B188" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C188" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D188" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B189" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C189" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D189" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B190" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C190" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D190" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B191" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C191" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D191" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B192" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C192" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D192" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B193" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C193" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D193" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B194" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C194" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D194" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B195" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C195" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D195" t="s">
         <v>752</v>
@@ -5791,510 +5803,524 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="B196" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C196" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D196" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B197" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C197" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D197" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B198" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C198" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D198" t="s">
-        <v>600</v>
+        <v>763</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B199" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C199" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D199" t="s">
-        <v>770</v>
+        <v>600</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B200" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C200" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D200" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B201" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C201" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D201" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B202" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C202" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D202" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B203" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C203" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D203" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B204" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C204" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D204" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B205" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C205" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D205" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B206" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C206" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D206" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B207" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C207" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D207" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B208" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C208" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D208" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B209" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C209" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D209" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B210" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C210" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D210" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B211" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C211" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D211" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B212" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C212" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D212" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B213" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C213" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D213" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B214" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C214" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D214" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B215" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="C215" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D215" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B216" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C216" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D216" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B217" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C217" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D217" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B218" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C218" t="s">
         <v>841</v>
       </c>
       <c r="D218" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B219" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C219" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D219" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B220" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C220" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D220" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B221" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C221" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D221" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B222" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C222" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D222" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B223" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C223" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D223" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B224" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C224" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D224" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B225" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C225" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D225" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B226" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C226" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D226" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B227" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C227" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D227" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B228" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C228" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D228" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B229" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C229" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="D229" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B230" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C230" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D230" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>890</v>
+      </c>
+      <c r="B231" t="s">
+        <v>891</v>
+      </c>
+      <c r="C231" t="s">
+        <v>892</v>
+      </c>
+      <c r="D231" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
         <v>894</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>895</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C232" t="s">
         <v>896</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D232" t="s">
         <v>897</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates survey metadata with EB/95.3 (June-July 2021)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14A7059-5420-447F-A62E-F54F069AD161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF1C50E-7CC3-49DF-B941-A7C213CB50EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="912">
   <si>
     <t>archive_id</t>
   </si>
@@ -2743,10 +2743,19 @@
     <t>94.3</t>
   </si>
   <si>
-    <t>February - March 2021</t>
-  </si>
-  <si>
     <t>COVID-19 Pandemic</t>
+  </si>
+  <si>
+    <t>February-March 2021</t>
+  </si>
+  <si>
+    <t>ZA7783</t>
+  </si>
+  <si>
+    <t>95.3</t>
+  </si>
+  <si>
+    <t>June-July 2021</t>
   </si>
 </sst>
 </file>
@@ -3081,13 +3090,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D232"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3105,2711 +3118,2711 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>901</v>
+        <v>909</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="C2" t="s">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="D2" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C3" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="D3" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="C4" t="s">
-        <v>900</v>
+        <v>908</v>
+      </c>
+      <c r="D4" t="s">
+        <v>907</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>899</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
         <v>121</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C45" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D45" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C50" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D50" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B51" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D51" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C52" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D52" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B53" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C53" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D53" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D54" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C55" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D55" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B56" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C56" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B57" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C57" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D57" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D58" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C59" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D59" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B60" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C60" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D60" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B61" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C61" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D61" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B62" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C62" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D62" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B63" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C63" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D63" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B64" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C64" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D64" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B65" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C65" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B66" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C66" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D66" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C67" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D67" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B68" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C68" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D68" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B69" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C69" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D69" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B70" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C70" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D70" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B71" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C71" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D71" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B72" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C72" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D72" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B73" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C73" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D73" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B74" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C74" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D74" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B75" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C75" t="s">
         <v>276</v>
       </c>
       <c r="D75" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B76" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C76" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D76" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B77" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C77" t="s">
         <v>283</v>
       </c>
       <c r="D77" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B78" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C78" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D78" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B79" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C79" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D79" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B80" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C80" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D80" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B81" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C81" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D81" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B82" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C82" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D82" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B83" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C83" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D83" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B84" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C84" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D84" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B85" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C85" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D85" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B86" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C86" t="s">
         <v>318</v>
       </c>
       <c r="D86" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B87" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C87" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D87" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B88" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C88" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D88" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B89" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C89" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D89" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B90" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C90" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D90" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B91" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C91" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D91" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B92" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C92" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D92" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B93" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C93" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D93" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B94" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C94" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D94" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B95" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C95" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D95" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B96" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C96" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D96" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B97" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C97" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D97" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B98" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C98" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D98" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B99" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C99" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D99" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B100" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C100" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D100" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B101" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C101" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D101" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B102" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C102" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D102" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B103" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C103" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D103" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B104" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C104" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D104" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B105" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C105" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D105" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B106" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C106" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D106" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B107" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C107" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D107" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B108" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C108" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D108" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B109" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C109" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D109" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B110" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C110" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D110" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B111" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C111" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D111" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B112" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C112" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D112" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B113" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C113" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D113" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B114" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C114" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D114" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B115" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C115" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D115" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B116" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C116" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D116" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B117" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C117" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D117" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B118" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C118" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D118" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B119" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C119" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D119" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B120" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C120" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D120" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B121" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C121" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D121" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B122" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C122" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D122" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B123" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C123" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D123" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B124" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C124" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D124" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B125" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C125" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D125" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B126" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C126" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D126" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B127" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C127" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D127" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B128" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C128" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D128" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B129" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C129" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D129" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B130" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C130" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D130" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B131" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C131" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D131" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B132" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C132" t="s">
         <v>501</v>
       </c>
       <c r="D132" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B133" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C133" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D133" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B134" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C134" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D134" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B135" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C135" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D135" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B136" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C136" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D136" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B137" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C137" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D137" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B138" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C138" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D138" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B139" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C139" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D139" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B140" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C140" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D140" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B141" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C141" t="s">
         <v>536</v>
       </c>
       <c r="D141" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B142" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C142" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D142" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B143" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C143" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D143" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B144" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C144" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D144" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B145" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C145" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D145" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B146" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C146" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D146" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B147" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C147" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D147" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B148" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C148" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D148" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B149" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C149" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D149" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B150" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C150" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D150" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B151" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C151" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D151" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B152" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C152" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D152" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B153" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C153" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D153" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B154" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C154" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D154" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B155" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C155" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D155" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B156" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C156" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D156" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B157" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C157" t="s">
         <v>599</v>
       </c>
       <c r="D157" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B158" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C158" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D158" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B159" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C159" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D159" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B160" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C160" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D160" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B161" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C161" t="s">
         <v>614</v>
       </c>
       <c r="D161" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B162" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C162" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D162" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B163" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C163" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D163" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B164" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C164" t="s">
         <v>625</v>
       </c>
       <c r="D164" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B165" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C165" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D165" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B166" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C166" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D166" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B167" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C167" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D167" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B168" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C168" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D168" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B169" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C169" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D169" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B170" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C170" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D170" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B171" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C171" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D171" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B172" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C172" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D172" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B173" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C173" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D173" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B174" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C174" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D174" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B175" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C175" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D175" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B176" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C176" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D176" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B177" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C177" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D177" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B178" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C178" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D178" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B179" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C179" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D179" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B180" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C180" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D180" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B181" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C181" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D181" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B182" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C182" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D182" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B183" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C183" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D183" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B184" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C184" t="s">
         <v>704</v>
       </c>
       <c r="D184" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B185" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C185" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D185" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B186" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C186" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D186" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B187" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C187" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D187" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B188" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C188" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D188" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B189" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C189" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D189" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B190" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C190" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D190" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B191" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C191" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D191" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B192" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C192" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D192" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B193" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C193" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D193" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B194" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C194" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D194" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B195" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C195" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D195" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B196" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C196" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D196" t="s">
         <v>752</v>
@@ -5817,505 +5830,519 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="B197" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C197" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D197" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B198" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C198" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D198" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B199" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C199" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D199" t="s">
-        <v>600</v>
+        <v>763</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B200" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C200" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D200" t="s">
-        <v>770</v>
+        <v>600</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B201" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C201" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D201" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B202" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C202" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D202" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B203" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C203" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D203" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B204" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C204" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D204" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B205" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C205" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D205" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B206" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C206" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D206" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B207" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C207" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D207" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B208" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C208" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D208" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B209" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C209" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D209" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B210" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C210" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D210" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B211" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C211" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D211" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B212" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C212" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D212" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B213" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C213" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D213" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B214" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C214" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D214" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B215" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C215" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D215" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B216" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="C216" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D216" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B217" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C217" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D217" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B218" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C218" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D218" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B219" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C219" t="s">
         <v>841</v>
       </c>
       <c r="D219" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B220" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C220" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D220" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B221" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C221" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D221" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B222" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C222" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D222" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B223" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C223" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D223" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B224" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C224" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D224" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B225" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C225" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D225" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B226" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C226" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D226" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B227" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C227" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D227" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B228" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C228" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D228" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B229" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C229" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D229" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B230" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C230" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="D230" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B231" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C231" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D231" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>890</v>
+      </c>
+      <c r="B232" t="s">
+        <v>891</v>
+      </c>
+      <c r="C232" t="s">
+        <v>892</v>
+      </c>
+      <c r="D232" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
         <v>894</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>895</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C233" t="s">
         <v>896</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D233" t="s">
         <v>897</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 92.2 (ZA 7580)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF1C50E-7CC3-49DF-B941-A7C213CB50EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B286D1-9126-44CB-8EC3-7D0BAC9ED389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="917">
   <si>
     <t>archive_id</t>
   </si>
@@ -2756,6 +2756,21 @@
   </si>
   <si>
     <t>June-July 2021</t>
+  </si>
+  <si>
+    <t>ZA7580</t>
+  </si>
+  <si>
+    <t>92.2</t>
+  </si>
+  <si>
+    <t>October 2019</t>
+  </si>
+  <si>
+    <t>Parlemeter 2019, Europeans attitudes towards cyber security</t>
+  </si>
+  <si>
+    <t>Parlemeter 2020, and Social Issues</t>
   </si>
 </sst>
 </file>
@@ -3090,10 +3105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3168,6 +3183,9 @@
       <c r="C5" t="s">
         <v>900</v>
       </c>
+      <c r="D5" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -3227,2616 +3245,2616 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
+        <v>912</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>914</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>915</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D32" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
         <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D46" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B49" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C49" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D50" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D51" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D52" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C53" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D53" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B54" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C54" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D54" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C55" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D55" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C56" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D56" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B57" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D57" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B58" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C58" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C59" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D59" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C60" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D60" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B61" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C61" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D61" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B62" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C62" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D62" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C63" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D63" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B64" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C64" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D64" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B65" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C65" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D65" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B66" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C66" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D66" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B67" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C67" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D67" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B68" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C68" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D68" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B69" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C69" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D69" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B70" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C70" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D70" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B71" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C71" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D71" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B72" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C72" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D72" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B73" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C73" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D73" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B74" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C74" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D74" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B75" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C75" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D75" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B76" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C76" t="s">
         <v>276</v>
       </c>
       <c r="D76" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B77" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C77" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D77" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B78" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C78" t="s">
         <v>283</v>
       </c>
       <c r="D78" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B79" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C79" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D79" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B80" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C80" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D80" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B81" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C81" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D81" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B82" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C82" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D82" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B83" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C83" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D83" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B84" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C84" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D84" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B85" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C85" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D85" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B86" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C86" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D86" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B87" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C87" t="s">
         <v>318</v>
       </c>
       <c r="D87" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B88" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C88" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D88" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B89" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C89" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D89" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B90" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C90" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D90" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B91" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C91" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D91" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B92" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C92" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D92" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B93" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C93" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D93" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B94" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C94" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D94" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B95" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C95" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D95" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B96" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C96" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D96" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B97" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C97" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D97" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B98" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C98" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D98" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B99" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C99" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D99" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B100" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C100" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D100" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B101" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C101" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D101" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B102" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C102" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D102" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B103" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C103" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D103" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B104" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C104" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D104" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B105" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C105" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D105" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B106" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C106" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D106" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B107" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C107" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D107" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B108" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C108" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D108" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B109" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C109" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D109" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B110" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C110" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D110" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B111" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C111" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D111" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B112" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C112" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D112" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B113" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C113" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D113" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B114" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C114" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D114" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B115" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C115" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D115" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B116" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C116" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D116" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B117" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C117" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D117" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B118" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C118" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D118" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B119" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C119" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D119" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B120" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C120" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D120" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B121" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C121" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D121" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B122" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C122" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D122" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B123" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C123" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D123" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B124" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C124" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D124" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B125" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C125" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D125" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B126" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C126" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D126" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B127" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C127" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D127" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B128" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C128" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D128" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B129" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C129" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D129" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B130" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C130" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D130" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B131" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C131" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D131" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B132" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C132" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D132" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B133" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C133" t="s">
         <v>501</v>
       </c>
       <c r="D133" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B134" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C134" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D134" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B135" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C135" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D135" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B136" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C136" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D136" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B137" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C137" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D137" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B138" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C138" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D138" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B139" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C139" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D139" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B140" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C140" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D140" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B141" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C141" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D141" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B142" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C142" t="s">
         <v>536</v>
       </c>
       <c r="D142" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B143" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C143" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D143" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B144" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C144" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D144" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B145" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C145" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D145" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B146" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C146" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D146" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B147" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C147" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D147" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B148" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C148" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D148" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B149" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C149" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D149" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B150" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C150" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D150" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B151" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C151" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D151" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B152" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C152" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D152" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B153" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C153" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D153" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B154" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C154" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D154" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B155" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C155" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D155" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B156" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C156" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D156" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B157" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C157" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D157" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B158" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C158" t="s">
         <v>599</v>
       </c>
       <c r="D158" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B159" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C159" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D159" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B160" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C160" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D160" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B161" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C161" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D161" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B162" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C162" t="s">
         <v>614</v>
       </c>
       <c r="D162" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B163" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C163" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D163" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B164" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C164" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D164" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B165" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C165" t="s">
         <v>625</v>
       </c>
       <c r="D165" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B166" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C166" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D166" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B167" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C167" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D167" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B168" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C168" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D168" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B169" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C169" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D169" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B170" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C170" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D170" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B171" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C171" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D171" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B172" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C172" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D172" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B173" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C173" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D173" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B174" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C174" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D174" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B175" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C175" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D175" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B176" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C176" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D176" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B177" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C177" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D177" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B178" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C178" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D178" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B179" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C179" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D179" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B180" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C180" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D180" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B181" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C181" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D181" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B182" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C182" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D182" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B183" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C183" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D183" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B184" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C184" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D184" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B185" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C185" t="s">
         <v>704</v>
       </c>
       <c r="D185" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B186" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C186" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D186" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B187" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C187" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D187" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B188" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C188" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D188" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B189" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C189" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D189" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B190" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C190" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D190" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B191" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C191" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D191" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B192" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C192" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D192" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B193" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C193" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D193" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B194" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C194" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D194" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B195" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C195" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D195" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B196" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C196" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D196" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B197" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C197" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D197" t="s">
         <v>752</v>
@@ -5844,505 +5862,519 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="B198" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C198" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D198" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B199" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C199" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D199" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B200" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C200" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D200" t="s">
-        <v>600</v>
+        <v>763</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B201" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C201" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D201" t="s">
-        <v>770</v>
+        <v>600</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B202" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C202" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D202" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B203" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C203" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D203" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B204" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C204" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D204" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B205" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C205" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D205" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B206" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C206" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D206" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B207" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C207" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D207" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B208" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C208" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D208" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B209" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C209" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D209" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B210" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C210" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D210" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B211" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C211" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D211" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B212" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C212" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D212" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B213" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C213" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D213" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B214" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C214" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D214" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B215" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C215" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D215" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B216" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C216" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D216" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B217" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="C217" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D217" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B218" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C218" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D218" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B219" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C219" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D219" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B220" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C220" t="s">
         <v>841</v>
       </c>
       <c r="D220" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B221" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C221" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D221" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B222" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C222" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D222" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B223" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C223" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D223" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B224" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C224" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D224" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B225" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C225" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D225" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B226" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C226" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D226" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B227" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C227" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D227" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B228" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C228" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D228" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B229" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C229" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D229" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B230" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C230" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D230" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B231" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C231" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="D231" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B232" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C232" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D232" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>890</v>
+      </c>
+      <c r="B233" t="s">
+        <v>891</v>
+      </c>
+      <c r="C233" t="s">
+        <v>892</v>
+      </c>
+      <c r="D233" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
         <v>894</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>895</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C234" t="s">
         <v>896</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D234" t="s">
         <v>897</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 95.2 (ZA 7782)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B286D1-9126-44CB-8EC3-7D0BAC9ED389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15B291D-0DED-40BA-A28A-CC6D41513BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="921">
   <si>
     <t>archive_id</t>
   </si>
@@ -2771,6 +2771,18 @@
   </si>
   <si>
     <t>Parlemeter 2020, and Social Issues</t>
+  </si>
+  <si>
+    <t>ZA7782</t>
+  </si>
+  <si>
+    <t>95.2</t>
+  </si>
+  <si>
+    <t>April-May 2021</t>
+  </si>
+  <si>
+    <t>European citizens’ knowledge and attitudes towards science and technology</t>
   </si>
 </sst>
 </file>
@@ -3105,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D234"/>
+  <dimension ref="A1:D235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="A10:D10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3147,2728 +3159,2728 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="C3" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
       <c r="D3" t="s">
-        <v>904</v>
+        <v>920</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C4" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="D4" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="C5" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="D5" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>899</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>900</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>916</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>912</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>913</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>914</v>
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>915</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
+        <v>912</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>914</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>915</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C38" t="s">
         <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B48" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C50" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C51" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D52" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C53" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D53" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B54" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C54" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D54" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B55" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C55" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D55" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D56" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B57" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D57" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B58" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D58" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B59" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C59" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B60" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C60" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D60" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B61" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C61" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D61" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B62" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C62" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D62" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B63" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C63" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D63" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B64" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C64" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D64" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B65" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C65" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D65" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B66" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C66" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D66" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B67" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C67" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D67" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B68" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C68" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D68" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B69" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C69" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D69" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B70" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C70" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D70" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B71" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C71" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D71" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B72" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C72" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D72" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B73" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C73" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D73" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B74" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C74" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D74" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D75" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B76" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C76" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D76" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B77" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C77" t="s">
         <v>276</v>
       </c>
       <c r="D77" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B78" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C78" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D78" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B79" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C79" t="s">
         <v>283</v>
       </c>
       <c r="D79" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B80" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C80" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D80" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B81" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C81" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D81" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B82" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C82" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D82" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B83" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C83" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D83" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B84" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C84" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D84" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B85" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C85" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D85" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B86" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C86" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D86" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B87" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C87" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D87" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B88" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C88" t="s">
         <v>318</v>
       </c>
       <c r="D88" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B89" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C89" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D89" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B90" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C90" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D90" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B91" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C91" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D91" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B92" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C92" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D92" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B93" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C93" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D93" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B94" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C94" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D94" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B95" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C95" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D95" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B96" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C96" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D96" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B97" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C97" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D97" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B98" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C98" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D98" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B99" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C99" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D99" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C100" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D100" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B101" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C101" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D101" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B102" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C102" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D102" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B103" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C103" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D103" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B104" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C104" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D104" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B105" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C105" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D105" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B106" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C106" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D106" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B107" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C107" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D107" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B108" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C108" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D108" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B109" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C109" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D109" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B110" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C110" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D110" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B111" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C111" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D111" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B112" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C112" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D112" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B113" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C113" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D113" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B114" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C114" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D114" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B115" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C115" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D115" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B116" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C116" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D116" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B117" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C117" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D117" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B118" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C118" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D118" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B119" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C119" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D119" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B120" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C120" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D120" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B121" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C121" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D121" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B122" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C122" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D122" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B123" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C123" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D123" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B124" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C124" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D124" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B125" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C125" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D125" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B126" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C126" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D126" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B127" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C127" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D127" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B128" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C128" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D128" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B129" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C129" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D129" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B130" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C130" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D130" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B131" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C131" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D131" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B132" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C132" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D132" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B133" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C133" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D133" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B134" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C134" t="s">
         <v>501</v>
       </c>
       <c r="D134" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B135" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C135" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D135" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B136" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C136" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D136" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B137" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C137" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D137" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B138" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C138" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D138" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B139" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C139" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D139" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B140" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C140" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D140" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B141" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C141" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D141" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B142" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C142" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D142" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B143" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C143" t="s">
         <v>536</v>
       </c>
       <c r="D143" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B144" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C144" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D144" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B145" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C145" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D145" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B146" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C146" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D146" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B147" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C147" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D147" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B148" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C148" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D148" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B149" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C149" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D149" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B150" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C150" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D150" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B151" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C151" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D151" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B152" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C152" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D152" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B153" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C153" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D153" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B154" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C154" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D154" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B155" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C155" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D155" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B156" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C156" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D156" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B157" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C157" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D157" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B158" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C158" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D158" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B159" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C159" t="s">
         <v>599</v>
       </c>
       <c r="D159" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B160" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C160" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D160" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B161" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C161" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D161" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B162" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C162" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D162" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B163" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C163" t="s">
         <v>614</v>
       </c>
       <c r="D163" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B164" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C164" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D164" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B165" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C165" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D165" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B166" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C166" t="s">
         <v>625</v>
       </c>
       <c r="D166" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B167" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C167" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D167" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B168" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C168" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D168" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B169" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C169" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D169" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B170" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C170" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D170" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B171" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C171" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D171" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B172" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C172" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D172" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B173" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C173" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D173" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B174" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C174" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D174" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B175" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C175" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D175" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B176" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C176" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D176" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B177" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C177" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D177" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B178" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C178" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D178" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B179" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C179" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D179" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B180" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C180" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D180" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B181" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C181" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D181" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B182" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C182" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D182" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B183" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C183" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D183" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B184" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C184" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D184" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B185" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C185" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D185" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B186" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C186" t="s">
         <v>704</v>
       </c>
       <c r="D186" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B187" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C187" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D187" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B188" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C188" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D188" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B189" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C189" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D189" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B190" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C190" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D190" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B191" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C191" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D191" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B192" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C192" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D192" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B193" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C193" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D193" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B194" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C194" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D194" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B195" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C195" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D195" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B196" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C196" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D196" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B197" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C197" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D197" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B198" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C198" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D198" t="s">
         <v>752</v>
@@ -5876,505 +5888,519 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="B199" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C199" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D199" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B200" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C200" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D200" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B201" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C201" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D201" t="s">
-        <v>600</v>
+        <v>763</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B202" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C202" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D202" t="s">
-        <v>770</v>
+        <v>600</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B203" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C203" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D203" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B204" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C204" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D204" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B205" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C205" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D205" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B206" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C206" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D206" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B207" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C207" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D207" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B208" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C208" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D208" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B209" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C209" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D209" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B210" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C210" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D210" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B211" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C211" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D211" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B212" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C212" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D212" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B213" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C213" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D213" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B214" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C214" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D214" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B215" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C215" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D215" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B216" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C216" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D216" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B217" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C217" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D217" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B218" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="C218" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D218" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B219" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C219" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D219" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B220" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C220" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D220" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B221" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C221" t="s">
         <v>841</v>
       </c>
       <c r="D221" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B222" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C222" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D222" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B223" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C223" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D223" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B224" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C224" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D224" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B225" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C225" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D225" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B226" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C226" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D226" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B227" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C227" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D227" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B228" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C228" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D228" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B229" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C229" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D229" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B230" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C230" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D230" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B231" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C231" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D231" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B232" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C232" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="D232" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B233" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C233" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D233" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>890</v>
+      </c>
+      <c r="B234" t="s">
+        <v>891</v>
+      </c>
+      <c r="C234" t="s">
+        <v>892</v>
+      </c>
+      <c r="D234" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
         <v>894</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>895</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C235" t="s">
         <v>896</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D235" t="s">
         <v>897</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 96.1 (ZA 7846)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15B291D-0DED-40BA-A28A-CC6D41513BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39F2CAA-9CB6-419C-8193-B3B062EC98DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="925">
   <si>
     <t>archive_id</t>
   </si>
@@ -2783,6 +2783,18 @@
   </si>
   <si>
     <t>European citizens’ knowledge and attitudes towards science and technology</t>
+  </si>
+  <si>
+    <t>ZA7846</t>
+  </si>
+  <si>
+    <t>96.1</t>
+  </si>
+  <si>
+    <t>September-October 2021</t>
+  </si>
+  <si>
+    <t>Future of Europe, and Digital rights and principles (COVID-19 Pandemic)</t>
   </si>
 </sst>
 </file>
@@ -3117,10 +3129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D235"/>
+  <dimension ref="A1:D236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3145,2756 +3157,2756 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="C2" t="s">
-        <v>911</v>
+        <v>923</v>
       </c>
       <c r="D2" t="s">
-        <v>907</v>
+        <v>924</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C3" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="D3" t="s">
-        <v>920</v>
+        <v>907</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="C4" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
       <c r="D4" t="s">
-        <v>904</v>
+        <v>920</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C5" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="D5" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="C6" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="D6" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>899</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>900</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>916</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>912</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>913</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>914</v>
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>915</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
+        <v>912</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>914</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>915</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
         <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B44" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D46" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B49" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B54" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C54" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D54" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C55" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D55" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B56" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D56" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B57" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C57" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D57" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B58" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C58" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D58" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B59" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C59" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D59" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B60" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C60" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D60" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B62" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C62" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D62" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C63" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B64" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C64" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D64" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C65" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D65" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B66" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C66" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D66" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C67" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D67" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B68" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C68" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D68" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B69" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C69" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D69" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B70" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C70" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D70" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C71" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D71" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B72" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C72" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D72" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B73" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C73" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D73" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B74" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C74" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D74" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B75" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C75" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D75" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B76" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C76" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D76" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B77" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C77" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D77" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B78" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C78" t="s">
         <v>276</v>
       </c>
       <c r="D78" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B79" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C79" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D79" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B80" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C80" t="s">
         <v>283</v>
       </c>
       <c r="D80" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B81" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C81" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D81" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B82" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C82" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D82" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B83" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C83" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D83" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B84" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C84" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D84" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B85" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C85" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D85" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B86" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C86" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D86" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B87" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C87" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D87" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B88" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C88" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D88" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B89" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C89" t="s">
         <v>318</v>
       </c>
       <c r="D89" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B90" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C90" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D90" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B91" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C91" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D91" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B92" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C92" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D92" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B93" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C93" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D93" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B94" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C94" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D94" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B95" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C95" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D95" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B96" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C96" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D96" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B97" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C97" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D97" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B98" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C98" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D98" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B99" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C99" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D99" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B100" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C100" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D100" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B101" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C101" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D101" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B102" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C102" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D102" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B103" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C103" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D103" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B104" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C104" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D104" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B105" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C105" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D105" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B106" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C106" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D106" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B107" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C107" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D107" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B108" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C108" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D108" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B109" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C109" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D109" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B110" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C110" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D110" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B111" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C111" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D111" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B112" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C112" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D112" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B113" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C113" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D113" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B114" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C114" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D114" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B115" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C115" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D115" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B116" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C116" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D116" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B117" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C117" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D117" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B118" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C118" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D118" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B119" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C119" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D119" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B120" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C120" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D120" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B121" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C121" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D121" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B122" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C122" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D122" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B123" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C123" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D123" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B124" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C124" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D124" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B125" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C125" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D125" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B126" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C126" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D126" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B127" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C127" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D127" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B128" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C128" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D128" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B129" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C129" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D129" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B130" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C130" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D130" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B131" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C131" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D131" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B132" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C132" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D132" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B133" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C133" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D133" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B134" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C134" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D134" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B135" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C135" t="s">
         <v>501</v>
       </c>
       <c r="D135" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B136" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C136" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D136" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B137" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C137" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D137" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B138" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C138" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D138" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B139" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C139" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D139" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B140" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C140" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D140" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B141" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C141" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D141" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B142" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C142" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D142" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B143" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C143" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D143" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B144" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C144" t="s">
         <v>536</v>
       </c>
       <c r="D144" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B145" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C145" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D145" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B146" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C146" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D146" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B147" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C147" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D147" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B148" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C148" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D148" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B149" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C149" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D149" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B150" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C150" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D150" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B151" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C151" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D151" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B152" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C152" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D152" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B153" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C153" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D153" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B154" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C154" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D154" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B155" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C155" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D155" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B156" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C156" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D156" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B157" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C157" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D157" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B158" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C158" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D158" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B159" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C159" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D159" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B160" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C160" t="s">
         <v>599</v>
       </c>
       <c r="D160" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B161" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C161" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D161" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B162" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C162" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D162" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B163" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C163" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D163" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B164" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C164" t="s">
         <v>614</v>
       </c>
       <c r="D164" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B165" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C165" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D165" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B166" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C166" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D166" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B167" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C167" t="s">
         <v>625</v>
       </c>
       <c r="D167" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B168" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C168" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D168" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B169" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C169" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D169" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B170" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C170" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D170" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B171" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C171" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D171" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B172" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C172" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D172" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B173" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C173" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D173" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B174" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C174" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D174" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B175" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C175" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D175" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B176" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C176" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D176" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B177" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C177" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D177" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B178" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C178" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D178" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B179" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C179" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D179" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B180" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C180" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D180" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B181" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C181" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D181" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B182" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C182" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D182" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B183" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C183" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D183" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B184" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C184" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D184" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B185" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C185" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D185" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B186" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C186" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D186" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B187" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C187" t="s">
         <v>704</v>
       </c>
       <c r="D187" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B188" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C188" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D188" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B189" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C189" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D189" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B190" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C190" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D190" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B191" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C191" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D191" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B192" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C192" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D192" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B193" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C193" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D193" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B194" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C194" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D194" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B195" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C195" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D195" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B196" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C196" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D196" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B197" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C197" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D197" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B198" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C198" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D198" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B199" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C199" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D199" t="s">
         <v>752</v>
@@ -5902,505 +5914,519 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="B200" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C200" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D200" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B201" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C201" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D201" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B202" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C202" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D202" t="s">
-        <v>600</v>
+        <v>763</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B203" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C203" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D203" t="s">
-        <v>770</v>
+        <v>600</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B204" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C204" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D204" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B205" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C205" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D205" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B206" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C206" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D206" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B207" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C207" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D207" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B208" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C208" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D208" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B209" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C209" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D209" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B210" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C210" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D210" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B211" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C211" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D211" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B212" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C212" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D212" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B213" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C213" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D213" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B214" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C214" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D214" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B215" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C215" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D215" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B216" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C216" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D216" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B217" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C217" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D217" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B218" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C218" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D218" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B219" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="C219" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D219" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B220" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C220" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D220" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B221" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C221" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D221" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B222" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C222" t="s">
         <v>841</v>
       </c>
       <c r="D222" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B223" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C223" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D223" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B224" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C224" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D224" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B225" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C225" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D225" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B226" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C226" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D226" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B227" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C227" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D227" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B228" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C228" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D228" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B229" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C229" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D229" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B230" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C230" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D230" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B231" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C231" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D231" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B232" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C232" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D232" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B233" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C233" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="D233" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B234" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C234" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D234" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
+        <v>890</v>
+      </c>
+      <c r="B235" t="s">
+        <v>891</v>
+      </c>
+      <c r="C235" t="s">
+        <v>892</v>
+      </c>
+      <c r="D235" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
         <v>894</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B236" t="s">
         <v>895</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C236" t="s">
         <v>896</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D236" t="s">
         <v>897</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB94.1 (ZA7749) and EB96.3 (ZA7848)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39F2CAA-9CB6-419C-8193-B3B062EC98DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DA3A94-8820-422E-8B77-11F5B72BF9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="932">
   <si>
     <t>archive_id</t>
   </si>
@@ -2795,6 +2795,27 @@
   </si>
   <si>
     <t>Future of Europe, and Digital rights and principles (COVID-19 Pandemic)</t>
+  </si>
+  <si>
+    <t>ZA7848</t>
+  </si>
+  <si>
+    <t>96.3</t>
+  </si>
+  <si>
+    <t>January-February 2022</t>
+  </si>
+  <si>
+    <t>ZA7749</t>
+  </si>
+  <si>
+    <t>94.1</t>
+  </si>
+  <si>
+    <t>October-November 2020</t>
+  </si>
+  <si>
+    <t>Future of Europe, Democracy in the EU, and Values and Identities of EU citizens</t>
   </si>
 </sst>
 </file>
@@ -3129,10 +3150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D236"/>
+  <dimension ref="A1:D238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3157,3276 +3178,3304 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="C2" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="D2" t="s">
-        <v>924</v>
+        <v>907</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="C3" t="s">
-        <v>911</v>
+        <v>923</v>
       </c>
       <c r="D3" t="s">
-        <v>907</v>
+        <v>924</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C4" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="D4" t="s">
-        <v>920</v>
+        <v>907</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="C5" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
       <c r="D5" t="s">
-        <v>904</v>
+        <v>920</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C6" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="D6" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="C7" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="D7" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>899</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>900</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>916</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
+        <v>928</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>929</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>930</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>931</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>912</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>913</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>914</v>
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>915</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
+        <v>912</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>914</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>915</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D43" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D45" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D47" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C50" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D50" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B51" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D51" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D53" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C54" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B55" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D55" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D56" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D58" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C59" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D59" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B60" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C60" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D60" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C61" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D61" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C62" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D62" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C63" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D63" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B64" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C64" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D64" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C65" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D65" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B66" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C66" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D66" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B67" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C67" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D67" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C68" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D68" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B69" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C69" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D69" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C70" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D70" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B71" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C71" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D71" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B72" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C72" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D72" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B73" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C73" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D73" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B74" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C74" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D74" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B75" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C75" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D75" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B76" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C76" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D76" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B77" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C77" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D77" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B78" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C78" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D78" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B79" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C79" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D79" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B80" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C80" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D80" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B81" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C81" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D81" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B82" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C82" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D82" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B83" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C83" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D83" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B84" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C84" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D84" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B85" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C85" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D85" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B86" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C86" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D86" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B87" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C87" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D87" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B88" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C88" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D88" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B89" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C89" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D89" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B90" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C90" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D90" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B91" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C91" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D91" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B92" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C92" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D92" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B93" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C93" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D93" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B94" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C94" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D94" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B95" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C95" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D95" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B96" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C96" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D96" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B97" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C97" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D97" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B98" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C98" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D98" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B99" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C99" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D99" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B100" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C100" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D100" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B101" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C101" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D101" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B102" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C102" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D102" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B103" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C103" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D103" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B104" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C104" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D104" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B105" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C105" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D105" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B106" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C106" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D106" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B107" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C107" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D107" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B108" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C108" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D108" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B109" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C109" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D109" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B110" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C110" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D110" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B111" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C111" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D111" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B112" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C112" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="D112" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B113" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C113" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="D113" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B114" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C114" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="D114" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B115" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C115" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="D115" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B116" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C116" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="D116" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B117" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C117" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="D117" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="B118" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="C118" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="D118" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="B119" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="C119" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="D119" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B120" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="C120" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="D120" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B121" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="C121" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="D121" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B122" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C122" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="D122" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B123" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="C123" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="D123" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B124" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C124" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="D124" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="B125" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="C125" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D125" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B126" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="C126" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="D126" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="B127" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="C127" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="D127" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B128" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="C128" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="D128" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B129" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="C129" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="D129" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B130" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="C130" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D130" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B131" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="C131" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="D131" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B132" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="C132" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="D132" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B133" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C133" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="D133" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="B134" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="C134" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="D134" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B135" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="C135" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="D135" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B136" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="C136" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D136" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B137" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="C137" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D137" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="B138" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="C138" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="D138" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B139" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="C139" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="D139" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="B140" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="C140" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="D140" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B141" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="C141" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D141" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="B142" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="C142" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="D142" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="B143" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C143" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="D143" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B144" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="C144" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="D144" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="B145" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="C145" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D145" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="B146" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C146" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D146" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="B147" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="C147" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="D147" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="B148" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="C148" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="D148" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="B149" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="C149" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="D149" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="B150" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="C150" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="D150" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="B151" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="C151" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="D151" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="B152" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="C152" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="D152" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="B153" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="C153" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="D153" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="B154" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="C154" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="D154" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="B155" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="C155" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="D155" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="B156" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="C156" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="D156" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="B157" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="C157" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="D157" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="B158" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="C158" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="D158" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="B159" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="C159" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="D159" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="B160" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="C160" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="D160" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="B161" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="C161" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D161" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="B162" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="C162" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D162" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="B163" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="C163" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="D163" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="B164" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="C164" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="D164" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="B165" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C165" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D165" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B166" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="C166" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="D166" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="B167" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="C167" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="D167" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="B168" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="C168" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D168" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="B169" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="C169" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D169" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="B170" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="C170" t="s">
-        <v>636</v>
+        <v>625</v>
       </c>
       <c r="D170" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="B171" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="C171" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="D171" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="B172" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="C172" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="D172" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="B173" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C173" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="D173" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="B174" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="C174" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="D174" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="B175" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="C175" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="D175" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="B176" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="C176" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="D176" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="B177" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="C177" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="D177" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="B178" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="C178" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="D178" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B179" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="C179" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="D179" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="B180" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="C180" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="D180" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="B181" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="C181" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="D181" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="B182" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="C182" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="D182" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="B183" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C183" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="D183" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="B184" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="C184" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="D184" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="B185" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="C185" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="D185" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="B186" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="C186" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="D186" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="B187" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="C187" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="D187" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="B188" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="C188" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D188" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="B189" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="C189" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D189" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="B190" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="C190" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
       <c r="D190" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="B191" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C191" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="D191" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="B192" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="C192" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="D192" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="B193" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="C193" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="D193" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="B194" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="C194" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="D194" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="B195" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="C195" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="D195" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="B196" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="C196" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="D196" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="B197" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="C197" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="D197" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B198" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="C198" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="D198" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="B199" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="C199" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="D199" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="B200" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="C200" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="D200" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
       <c r="B201" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="C201" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="D201" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="B202" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="C202" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="D202" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="B203" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="C203" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="D203" t="s">
-        <v>600</v>
+        <v>759</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="B204" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
       <c r="C204" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="D204" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>771</v>
+        <v>764</v>
       </c>
       <c r="B205" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
       <c r="C205" t="s">
-        <v>773</v>
+        <v>766</v>
       </c>
       <c r="D205" t="s">
-        <v>774</v>
+        <v>600</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="B206" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="C206" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="D206" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="B207" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="C207" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="D207" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="B208" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="C208" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="D208" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="B209" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="C209" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="D209" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="B210" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="C210" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="D210" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="B211" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="C211" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="D211" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="B212" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="C212" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="D212" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="B213" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="C213" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="D213" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="B214" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="C214" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="D214" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="B215" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="C215" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="D215" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="B216" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="C216" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="D216" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="B217" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="C217" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="D217" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="B218" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="C218" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="D218" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="B219" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="C219" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="D219" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="B220" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="C220" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="D220" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="B221" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="C221" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="D221" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="B222" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="C222" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="D222" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="B223" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="C223" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D223" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="B224" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="C224" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D224" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="B225" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="C225" t="s">
-        <v>852</v>
+        <v>841</v>
       </c>
       <c r="D225" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="B226" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="C226" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="D226" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="B227" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="C227" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="D227" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="B228" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="C228" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="D228" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="B229" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="C229" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="D229" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="B230" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="C230" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="D230" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="B231" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="C231" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="D231" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="B232" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="C232" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="D232" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="B233" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="C233" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="D233" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="B234" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="C234" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="D234" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="B235" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="C235" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="D235" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>886</v>
+      </c>
+      <c r="B236" t="s">
+        <v>887</v>
+      </c>
+      <c r="C236" t="s">
+        <v>888</v>
+      </c>
+      <c r="D236" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>890</v>
+      </c>
+      <c r="B237" t="s">
+        <v>891</v>
+      </c>
+      <c r="C237" t="s">
+        <v>892</v>
+      </c>
+      <c r="D237" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
         <v>894</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B238" t="s">
         <v>895</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C238" t="s">
         <v>896</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D238" t="s">
         <v>897</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add workflow for left-right scale from EB
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DA3A94-8820-422E-8B77-11F5B72BF9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ED4661-1155-425F-8ED3-361A3A2A3957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1237,9 +1237,6 @@
     <t>65.1</t>
   </si>
   <si>
-    <t>February-March 206</t>
-  </si>
-  <si>
     <t>The Future of Europe, Transborder Purchases in the European Union, and Family Planning</t>
   </si>
   <si>
@@ -2816,6 +2813,9 @@
   </si>
   <si>
     <t>Future of Europe, Democracy in the EU, and Values and Identities of EU citizens</t>
+  </si>
+  <si>
+    <t>February-March 2006</t>
   </si>
 </sst>
 </file>
@@ -3152,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C113" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3178,114 +3178,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>925</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>926</v>
       </c>
-      <c r="C2" t="s">
-        <v>927</v>
-      </c>
       <c r="D2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>920</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>922</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>923</v>
-      </c>
-      <c r="D3" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>908</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>910</v>
       </c>
-      <c r="C4" t="s">
-        <v>911</v>
-      </c>
       <c r="D4" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>916</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>918</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>919</v>
-      </c>
-      <c r="D5" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>900</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
         <v>902</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>903</v>
-      </c>
-      <c r="D6" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>904</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>905</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>907</v>
+      </c>
+      <c r="D7" t="s">
         <v>906</v>
-      </c>
-      <c r="C7" t="s">
-        <v>908</v>
-      </c>
-      <c r="D7" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>897</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>898</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
         <v>899</v>
       </c>
-      <c r="C8" t="s">
-        <v>900</v>
-      </c>
       <c r="D8" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>927</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>928</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" t="s">
         <v>929</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>930</v>
-      </c>
-      <c r="D9" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3346,16 +3346,16 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>911</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>912</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>913</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" t="s">
         <v>914</v>
-      </c>
-      <c r="D14" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -4723,1760 +4723,1760 @@
         <v>404</v>
       </c>
       <c r="C113" t="s">
+        <v>931</v>
+      </c>
+      <c r="D113" t="s">
         <v>405</v>
-      </c>
-      <c r="D113" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>406</v>
+      </c>
+      <c r="B114" t="s">
         <v>407</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>408</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>409</v>
-      </c>
-      <c r="D114" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
+        <v>410</v>
+      </c>
+      <c r="B115" t="s">
         <v>411</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>412</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>413</v>
-      </c>
-      <c r="D115" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>414</v>
+      </c>
+      <c r="B116" t="s">
         <v>415</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>416</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>417</v>
-      </c>
-      <c r="D116" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>418</v>
+      </c>
+      <c r="B117" t="s">
         <v>419</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>420</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>421</v>
-      </c>
-      <c r="D117" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>422</v>
+      </c>
+      <c r="B118" t="s">
         <v>423</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>424</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>425</v>
-      </c>
-      <c r="D118" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>426</v>
+      </c>
+      <c r="B119" t="s">
         <v>427</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>428</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>429</v>
-      </c>
-      <c r="D119" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>430</v>
+      </c>
+      <c r="B120" t="s">
         <v>431</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>432</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>433</v>
-      </c>
-      <c r="D120" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>434</v>
+      </c>
+      <c r="B121" t="s">
         <v>435</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>436</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
         <v>437</v>
-      </c>
-      <c r="D121" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>438</v>
+      </c>
+      <c r="B122" t="s">
         <v>439</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>440</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>441</v>
-      </c>
-      <c r="D122" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>442</v>
+      </c>
+      <c r="B123" t="s">
         <v>443</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>444</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>445</v>
-      </c>
-      <c r="D123" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>446</v>
+      </c>
+      <c r="B124" t="s">
         <v>447</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>448</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>449</v>
-      </c>
-      <c r="D124" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>450</v>
+      </c>
+      <c r="B125" t="s">
         <v>451</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>452</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D125" t="s">
         <v>453</v>
-      </c>
-      <c r="D125" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>454</v>
+      </c>
+      <c r="B126" t="s">
         <v>455</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>456</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>457</v>
-      </c>
-      <c r="D126" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>458</v>
+      </c>
+      <c r="B127" t="s">
         <v>459</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>460</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>461</v>
-      </c>
-      <c r="D127" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>462</v>
+      </c>
+      <c r="B128" t="s">
         <v>463</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>464</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>465</v>
-      </c>
-      <c r="D128" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>466</v>
+      </c>
+      <c r="B129" t="s">
         <v>467</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>468</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
         <v>469</v>
-      </c>
-      <c r="D129" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>470</v>
+      </c>
+      <c r="B130" t="s">
         <v>471</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>472</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>473</v>
-      </c>
-      <c r="D130" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>474</v>
+      </c>
+      <c r="B131" t="s">
         <v>475</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>476</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>477</v>
-      </c>
-      <c r="D131" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
+        <v>478</v>
+      </c>
+      <c r="B132" t="s">
         <v>479</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>480</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>481</v>
-      </c>
-      <c r="D132" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
+        <v>482</v>
+      </c>
+      <c r="B133" t="s">
         <v>483</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>484</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>485</v>
-      </c>
-      <c r="D133" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>486</v>
+      </c>
+      <c r="B134" t="s">
         <v>487</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>488</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>489</v>
-      </c>
-      <c r="D134" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
+        <v>490</v>
+      </c>
+      <c r="B135" t="s">
         <v>491</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>492</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" t="s">
         <v>493</v>
-      </c>
-      <c r="D135" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>494</v>
+      </c>
+      <c r="B136" t="s">
         <v>495</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>496</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>497</v>
-      </c>
-      <c r="D136" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>498</v>
+      </c>
+      <c r="B137" t="s">
         <v>499</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>500</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>501</v>
-      </c>
-      <c r="D137" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>502</v>
+      </c>
+      <c r="B138" t="s">
         <v>503</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
+        <v>500</v>
+      </c>
+      <c r="D138" t="s">
         <v>504</v>
-      </c>
-      <c r="C138" t="s">
-        <v>501</v>
-      </c>
-      <c r="D138" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>505</v>
+      </c>
+      <c r="B139" t="s">
         <v>506</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>507</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
         <v>508</v>
-      </c>
-      <c r="D139" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>509</v>
+      </c>
+      <c r="B140" t="s">
         <v>510</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>511</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
         <v>512</v>
-      </c>
-      <c r="D140" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>513</v>
+      </c>
+      <c r="B141" t="s">
         <v>514</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>515</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>516</v>
-      </c>
-      <c r="D141" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
+        <v>517</v>
+      </c>
+      <c r="B142" t="s">
         <v>518</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>519</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>520</v>
-      </c>
-      <c r="D142" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
+        <v>521</v>
+      </c>
+      <c r="B143" t="s">
         <v>522</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>523</v>
       </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
         <v>524</v>
-      </c>
-      <c r="D143" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>525</v>
+      </c>
+      <c r="B144" t="s">
         <v>526</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>527</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>528</v>
-      </c>
-      <c r="D144" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>529</v>
+      </c>
+      <c r="B145" t="s">
         <v>530</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
         <v>531</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>532</v>
-      </c>
-      <c r="D145" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>533</v>
+      </c>
+      <c r="B146" t="s">
         <v>534</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
         <v>535</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>536</v>
-      </c>
-      <c r="D146" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>537</v>
+      </c>
+      <c r="B147" t="s">
         <v>538</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" t="s">
+        <v>535</v>
+      </c>
+      <c r="D147" t="s">
         <v>539</v>
-      </c>
-      <c r="C147" t="s">
-        <v>536</v>
-      </c>
-      <c r="D147" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
+        <v>540</v>
+      </c>
+      <c r="B148" t="s">
         <v>541</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
         <v>542</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>543</v>
-      </c>
-      <c r="D148" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>544</v>
+      </c>
+      <c r="B149" t="s">
         <v>545</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>546</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>547</v>
-      </c>
-      <c r="D149" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>548</v>
+      </c>
+      <c r="B150" t="s">
         <v>549</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" t="s">
         <v>550</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>551</v>
-      </c>
-      <c r="D150" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
+        <v>552</v>
+      </c>
+      <c r="B151" t="s">
         <v>553</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" t="s">
         <v>554</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" t="s">
         <v>555</v>
-      </c>
-      <c r="D151" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
+        <v>556</v>
+      </c>
+      <c r="B152" t="s">
         <v>557</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" t="s">
         <v>558</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" t="s">
         <v>559</v>
-      </c>
-      <c r="D152" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
+        <v>560</v>
+      </c>
+      <c r="B153" t="s">
         <v>561</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153" t="s">
         <v>562</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>563</v>
-      </c>
-      <c r="D153" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>564</v>
+      </c>
+      <c r="B154" t="s">
         <v>565</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>566</v>
       </c>
-      <c r="C154" t="s">
+      <c r="D154" t="s">
         <v>567</v>
-      </c>
-      <c r="D154" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
+        <v>568</v>
+      </c>
+      <c r="B155" t="s">
         <v>569</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" t="s">
         <v>570</v>
       </c>
-      <c r="C155" t="s">
+      <c r="D155" t="s">
         <v>571</v>
-      </c>
-      <c r="D155" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
+        <v>572</v>
+      </c>
+      <c r="B156" t="s">
         <v>573</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" t="s">
         <v>574</v>
       </c>
-      <c r="C156" t="s">
+      <c r="D156" t="s">
         <v>575</v>
-      </c>
-      <c r="D156" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>576</v>
+      </c>
+      <c r="B157" t="s">
         <v>577</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>578</v>
       </c>
-      <c r="C157" t="s">
+      <c r="D157" t="s">
         <v>579</v>
-      </c>
-      <c r="D157" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>580</v>
+      </c>
+      <c r="B158" t="s">
         <v>581</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>582</v>
       </c>
-      <c r="C158" t="s">
+      <c r="D158" t="s">
         <v>583</v>
-      </c>
-      <c r="D158" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>584</v>
+      </c>
+      <c r="B159" t="s">
         <v>585</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" t="s">
         <v>586</v>
       </c>
-      <c r="C159" t="s">
+      <c r="D159" t="s">
         <v>587</v>
-      </c>
-      <c r="D159" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>588</v>
+      </c>
+      <c r="B160" t="s">
         <v>589</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
         <v>590</v>
       </c>
-      <c r="C160" t="s">
+      <c r="D160" t="s">
         <v>591</v>
-      </c>
-      <c r="D160" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
+        <v>592</v>
+      </c>
+      <c r="B161" t="s">
         <v>593</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
         <v>594</v>
       </c>
-      <c r="C161" t="s">
+      <c r="D161" t="s">
         <v>595</v>
-      </c>
-      <c r="D161" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>596</v>
+      </c>
+      <c r="B162" t="s">
         <v>597</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>598</v>
       </c>
-      <c r="C162" t="s">
+      <c r="D162" t="s">
         <v>599</v>
-      </c>
-      <c r="D162" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>600</v>
+      </c>
+      <c r="B163" t="s">
         <v>601</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" t="s">
+        <v>598</v>
+      </c>
+      <c r="D163" t="s">
         <v>602</v>
-      </c>
-      <c r="C163" t="s">
-        <v>599</v>
-      </c>
-      <c r="D163" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>603</v>
+      </c>
+      <c r="B164" t="s">
         <v>604</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>605</v>
       </c>
-      <c r="C164" t="s">
+      <c r="D164" t="s">
         <v>606</v>
-      </c>
-      <c r="D164" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>607</v>
+      </c>
+      <c r="B165" t="s">
         <v>608</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
         <v>609</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" t="s">
         <v>610</v>
-      </c>
-      <c r="D165" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>611</v>
+      </c>
+      <c r="B166" t="s">
         <v>612</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
         <v>613</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D166" t="s">
         <v>614</v>
-      </c>
-      <c r="D166" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>615</v>
+      </c>
+      <c r="B167" t="s">
         <v>616</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
+        <v>613</v>
+      </c>
+      <c r="D167" t="s">
         <v>617</v>
-      </c>
-      <c r="C167" t="s">
-        <v>614</v>
-      </c>
-      <c r="D167" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
+        <v>618</v>
+      </c>
+      <c r="B168" t="s">
         <v>619</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>620</v>
       </c>
-      <c r="C168" t="s">
+      <c r="D168" t="s">
         <v>621</v>
-      </c>
-      <c r="D168" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>622</v>
+      </c>
+      <c r="B169" t="s">
         <v>623</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>624</v>
       </c>
-      <c r="C169" t="s">
+      <c r="D169" t="s">
         <v>625</v>
-      </c>
-      <c r="D169" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
+        <v>626</v>
+      </c>
+      <c r="B170" t="s">
         <v>627</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
+        <v>624</v>
+      </c>
+      <c r="D170" t="s">
         <v>628</v>
-      </c>
-      <c r="C170" t="s">
-        <v>625</v>
-      </c>
-      <c r="D170" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
+        <v>629</v>
+      </c>
+      <c r="B171" t="s">
         <v>630</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
         <v>631</v>
       </c>
-      <c r="C171" t="s">
+      <c r="D171" t="s">
         <v>632</v>
-      </c>
-      <c r="D171" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
+        <v>633</v>
+      </c>
+      <c r="B172" t="s">
         <v>634</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>635</v>
       </c>
-      <c r="C172" t="s">
+      <c r="D172" t="s">
         <v>636</v>
-      </c>
-      <c r="D172" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>637</v>
+      </c>
+      <c r="B173" t="s">
         <v>638</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
         <v>639</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D173" t="s">
         <v>640</v>
-      </c>
-      <c r="D173" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>641</v>
+      </c>
+      <c r="B174" t="s">
         <v>642</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>643</v>
       </c>
-      <c r="C174" t="s">
+      <c r="D174" t="s">
         <v>644</v>
-      </c>
-      <c r="D174" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>645</v>
+      </c>
+      <c r="B175" t="s">
         <v>646</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
         <v>647</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D175" t="s">
         <v>648</v>
-      </c>
-      <c r="D175" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
+        <v>649</v>
+      </c>
+      <c r="B176" t="s">
         <v>650</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>651</v>
       </c>
-      <c r="C176" t="s">
+      <c r="D176" t="s">
         <v>652</v>
-      </c>
-      <c r="D176" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>653</v>
+      </c>
+      <c r="B177" t="s">
         <v>654</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" t="s">
         <v>655</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>656</v>
-      </c>
-      <c r="D177" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
+        <v>657</v>
+      </c>
+      <c r="B178" t="s">
         <v>658</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C178" t="s">
         <v>659</v>
       </c>
-      <c r="C178" t="s">
+      <c r="D178" t="s">
         <v>660</v>
-      </c>
-      <c r="D178" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>661</v>
+      </c>
+      <c r="B179" t="s">
         <v>662</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" t="s">
         <v>663</v>
       </c>
-      <c r="C179" t="s">
+      <c r="D179" t="s">
         <v>664</v>
-      </c>
-      <c r="D179" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
+        <v>665</v>
+      </c>
+      <c r="B180" t="s">
         <v>666</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" t="s">
         <v>667</v>
       </c>
-      <c r="C180" t="s">
+      <c r="D180" t="s">
         <v>668</v>
-      </c>
-      <c r="D180" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>669</v>
+      </c>
+      <c r="B181" t="s">
         <v>670</v>
       </c>
-      <c r="B181" t="s">
+      <c r="C181" t="s">
         <v>671</v>
       </c>
-      <c r="C181" t="s">
+      <c r="D181" t="s">
         <v>672</v>
-      </c>
-      <c r="D181" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
+        <v>673</v>
+      </c>
+      <c r="B182" t="s">
         <v>674</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>675</v>
       </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>676</v>
-      </c>
-      <c r="D182" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>677</v>
+      </c>
+      <c r="B183" t="s">
         <v>678</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C183" t="s">
         <v>679</v>
       </c>
-      <c r="C183" t="s">
+      <c r="D183" t="s">
         <v>680</v>
-      </c>
-      <c r="D183" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>681</v>
+      </c>
+      <c r="B184" t="s">
         <v>682</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>683</v>
       </c>
-      <c r="C184" t="s">
+      <c r="D184" t="s">
         <v>684</v>
-      </c>
-      <c r="D184" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>685</v>
+      </c>
+      <c r="B185" t="s">
         <v>686</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>687</v>
       </c>
-      <c r="C185" t="s">
+      <c r="D185" t="s">
         <v>688</v>
-      </c>
-      <c r="D185" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
+        <v>689</v>
+      </c>
+      <c r="B186" t="s">
         <v>690</v>
       </c>
-      <c r="B186" t="s">
+      <c r="C186" t="s">
         <v>691</v>
       </c>
-      <c r="C186" t="s">
+      <c r="D186" t="s">
         <v>692</v>
-      </c>
-      <c r="D186" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
+        <v>693</v>
+      </c>
+      <c r="B187" t="s">
         <v>694</v>
       </c>
-      <c r="B187" t="s">
+      <c r="C187" t="s">
         <v>695</v>
       </c>
-      <c r="C187" t="s">
+      <c r="D187" t="s">
         <v>696</v>
-      </c>
-      <c r="D187" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
+        <v>697</v>
+      </c>
+      <c r="B188" t="s">
         <v>698</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
         <v>699</v>
       </c>
-      <c r="C188" t="s">
+      <c r="D188" t="s">
         <v>700</v>
-      </c>
-      <c r="D188" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
+        <v>701</v>
+      </c>
+      <c r="B189" t="s">
         <v>702</v>
       </c>
-      <c r="B189" t="s">
+      <c r="C189" t="s">
         <v>703</v>
       </c>
-      <c r="C189" t="s">
+      <c r="D189" t="s">
         <v>704</v>
-      </c>
-      <c r="D189" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>705</v>
+      </c>
+      <c r="B190" t="s">
         <v>706</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" t="s">
+        <v>703</v>
+      </c>
+      <c r="D190" t="s">
         <v>707</v>
-      </c>
-      <c r="C190" t="s">
-        <v>704</v>
-      </c>
-      <c r="D190" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
+        <v>708</v>
+      </c>
+      <c r="B191" t="s">
         <v>709</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
         <v>710</v>
       </c>
-      <c r="C191" t="s">
+      <c r="D191" t="s">
         <v>711</v>
-      </c>
-      <c r="D191" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>712</v>
+      </c>
+      <c r="B192" t="s">
         <v>713</v>
       </c>
-      <c r="B192" t="s">
+      <c r="C192" t="s">
         <v>714</v>
       </c>
-      <c r="C192" t="s">
+      <c r="D192" t="s">
         <v>715</v>
-      </c>
-      <c r="D192" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>716</v>
+      </c>
+      <c r="B193" t="s">
         <v>717</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
         <v>718</v>
       </c>
-      <c r="C193" t="s">
+      <c r="D193" t="s">
         <v>719</v>
-      </c>
-      <c r="D193" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
+        <v>720</v>
+      </c>
+      <c r="B194" t="s">
         <v>721</v>
       </c>
-      <c r="B194" t="s">
+      <c r="C194" t="s">
         <v>722</v>
       </c>
-      <c r="C194" t="s">
+      <c r="D194" t="s">
         <v>723</v>
-      </c>
-      <c r="D194" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>724</v>
+      </c>
+      <c r="B195" t="s">
         <v>725</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195" t="s">
         <v>726</v>
       </c>
-      <c r="C195" t="s">
+      <c r="D195" t="s">
         <v>727</v>
-      </c>
-      <c r="D195" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
+        <v>728</v>
+      </c>
+      <c r="B196" t="s">
         <v>729</v>
       </c>
-      <c r="B196" t="s">
+      <c r="C196" t="s">
         <v>730</v>
       </c>
-      <c r="C196" t="s">
+      <c r="D196" t="s">
         <v>731</v>
-      </c>
-      <c r="D196" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>732</v>
+      </c>
+      <c r="B197" t="s">
         <v>733</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>734</v>
       </c>
-      <c r="C197" t="s">
+      <c r="D197" t="s">
         <v>735</v>
-      </c>
-      <c r="D197" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
+        <v>736</v>
+      </c>
+      <c r="B198" t="s">
         <v>737</v>
       </c>
-      <c r="B198" t="s">
+      <c r="C198" t="s">
         <v>738</v>
       </c>
-      <c r="C198" t="s">
+      <c r="D198" t="s">
         <v>739</v>
-      </c>
-      <c r="D198" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>740</v>
+      </c>
+      <c r="B199" t="s">
         <v>741</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>742</v>
       </c>
-      <c r="C199" t="s">
+      <c r="D199" t="s">
         <v>743</v>
-      </c>
-      <c r="D199" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
+        <v>744</v>
+      </c>
+      <c r="B200" t="s">
         <v>745</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
         <v>746</v>
       </c>
-      <c r="C200" t="s">
+      <c r="D200" t="s">
         <v>747</v>
-      </c>
-      <c r="D200" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>748</v>
+      </c>
+      <c r="B201" t="s">
         <v>749</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
         <v>750</v>
       </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>751</v>
-      </c>
-      <c r="D201" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>752</v>
+      </c>
+      <c r="B202" t="s">
         <v>753</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>754</v>
       </c>
-      <c r="C202" t="s">
-        <v>755</v>
-      </c>
       <c r="D202" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
+        <v>755</v>
+      </c>
+      <c r="B203" t="s">
         <v>756</v>
       </c>
-      <c r="B203" t="s">
+      <c r="C203" t="s">
         <v>757</v>
       </c>
-      <c r="C203" t="s">
+      <c r="D203" t="s">
         <v>758</v>
-      </c>
-      <c r="D203" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>759</v>
+      </c>
+      <c r="B204" t="s">
         <v>760</v>
       </c>
-      <c r="B204" t="s">
+      <c r="C204" t="s">
         <v>761</v>
       </c>
-      <c r="C204" t="s">
+      <c r="D204" t="s">
         <v>762</v>
-      </c>
-      <c r="D204" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>763</v>
+      </c>
+      <c r="B205" t="s">
         <v>764</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>765</v>
       </c>
-      <c r="C205" t="s">
-        <v>766</v>
-      </c>
       <c r="D205" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>766</v>
+      </c>
+      <c r="B206" t="s">
         <v>767</v>
       </c>
-      <c r="B206" t="s">
+      <c r="C206" t="s">
         <v>768</v>
       </c>
-      <c r="C206" t="s">
+      <c r="D206" t="s">
         <v>769</v>
-      </c>
-      <c r="D206" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>770</v>
+      </c>
+      <c r="B207" t="s">
         <v>771</v>
       </c>
-      <c r="B207" t="s">
+      <c r="C207" t="s">
         <v>772</v>
       </c>
-      <c r="C207" t="s">
+      <c r="D207" t="s">
         <v>773</v>
-      </c>
-      <c r="D207" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>774</v>
+      </c>
+      <c r="B208" t="s">
         <v>775</v>
       </c>
-      <c r="B208" t="s">
+      <c r="C208" t="s">
         <v>776</v>
       </c>
-      <c r="C208" t="s">
+      <c r="D208" t="s">
         <v>777</v>
-      </c>
-      <c r="D208" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>778</v>
+      </c>
+      <c r="B209" t="s">
         <v>779</v>
       </c>
-      <c r="B209" t="s">
+      <c r="C209" t="s">
         <v>780</v>
       </c>
-      <c r="C209" t="s">
+      <c r="D209" t="s">
         <v>781</v>
-      </c>
-      <c r="D209" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>782</v>
+      </c>
+      <c r="B210" t="s">
         <v>783</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>784</v>
       </c>
-      <c r="C210" t="s">
+      <c r="D210" t="s">
         <v>785</v>
-      </c>
-      <c r="D210" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>786</v>
+      </c>
+      <c r="B211" t="s">
         <v>787</v>
       </c>
-      <c r="B211" t="s">
+      <c r="C211" t="s">
         <v>788</v>
       </c>
-      <c r="C211" t="s">
+      <c r="D211" t="s">
         <v>789</v>
-      </c>
-      <c r="D211" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
+        <v>790</v>
+      </c>
+      <c r="B212" t="s">
         <v>791</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>792</v>
       </c>
-      <c r="C212" t="s">
+      <c r="D212" t="s">
         <v>793</v>
-      </c>
-      <c r="D212" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
+        <v>794</v>
+      </c>
+      <c r="B213" t="s">
         <v>795</v>
       </c>
-      <c r="B213" t="s">
+      <c r="C213" t="s">
         <v>796</v>
       </c>
-      <c r="C213" t="s">
+      <c r="D213" t="s">
         <v>797</v>
-      </c>
-      <c r="D213" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
+        <v>798</v>
+      </c>
+      <c r="B214" t="s">
         <v>799</v>
       </c>
-      <c r="B214" t="s">
+      <c r="C214" t="s">
         <v>800</v>
       </c>
-      <c r="C214" t="s">
+      <c r="D214" t="s">
         <v>801</v>
-      </c>
-      <c r="D214" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
+        <v>802</v>
+      </c>
+      <c r="B215" t="s">
         <v>803</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
         <v>804</v>
       </c>
-      <c r="C215" t="s">
+      <c r="D215" t="s">
         <v>805</v>
-      </c>
-      <c r="D215" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>806</v>
+      </c>
+      <c r="B216" t="s">
         <v>807</v>
       </c>
-      <c r="B216" t="s">
+      <c r="C216" t="s">
         <v>808</v>
       </c>
-      <c r="C216" t="s">
+      <c r="D216" t="s">
         <v>809</v>
-      </c>
-      <c r="D216" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
+        <v>810</v>
+      </c>
+      <c r="B217" t="s">
         <v>811</v>
       </c>
-      <c r="B217" t="s">
+      <c r="C217" t="s">
         <v>812</v>
       </c>
-      <c r="C217" t="s">
+      <c r="D217" t="s">
         <v>813</v>
-      </c>
-      <c r="D217" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
+        <v>814</v>
+      </c>
+      <c r="B218" t="s">
         <v>815</v>
       </c>
-      <c r="B218" t="s">
+      <c r="C218" t="s">
         <v>816</v>
       </c>
-      <c r="C218" t="s">
+      <c r="D218" t="s">
         <v>817</v>
-      </c>
-      <c r="D218" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
+        <v>818</v>
+      </c>
+      <c r="B219" t="s">
         <v>819</v>
       </c>
-      <c r="B219" t="s">
+      <c r="C219" t="s">
         <v>820</v>
       </c>
-      <c r="C219" t="s">
+      <c r="D219" t="s">
         <v>821</v>
-      </c>
-      <c r="D219" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
+        <v>822</v>
+      </c>
+      <c r="B220" t="s">
         <v>823</v>
       </c>
-      <c r="B220" t="s">
+      <c r="C220" t="s">
         <v>824</v>
       </c>
-      <c r="C220" t="s">
+      <c r="D220" t="s">
         <v>825</v>
-      </c>
-      <c r="D220" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
+        <v>826</v>
+      </c>
+      <c r="B221" t="s">
         <v>827</v>
       </c>
-      <c r="B221" t="s">
+      <c r="C221" t="s">
         <v>828</v>
       </c>
-      <c r="C221" t="s">
+      <c r="D221" t="s">
         <v>829</v>
-      </c>
-      <c r="D221" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
+        <v>830</v>
+      </c>
+      <c r="B222" t="s">
         <v>831</v>
       </c>
-      <c r="B222" t="s">
+      <c r="C222" t="s">
         <v>832</v>
       </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>833</v>
-      </c>
-      <c r="D222" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>834</v>
+      </c>
+      <c r="B223" t="s">
         <v>835</v>
       </c>
-      <c r="B223" t="s">
+      <c r="C223" t="s">
         <v>836</v>
       </c>
-      <c r="C223" t="s">
+      <c r="D223" t="s">
         <v>837</v>
-      </c>
-      <c r="D223" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>838</v>
+      </c>
+      <c r="B224" t="s">
         <v>839</v>
       </c>
-      <c r="B224" t="s">
+      <c r="C224" t="s">
         <v>840</v>
       </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>841</v>
-      </c>
-      <c r="D224" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
+        <v>842</v>
+      </c>
+      <c r="B225" t="s">
         <v>843</v>
       </c>
-      <c r="B225" t="s">
+      <c r="C225" t="s">
+        <v>840</v>
+      </c>
+      <c r="D225" t="s">
         <v>844</v>
-      </c>
-      <c r="C225" t="s">
-        <v>841</v>
-      </c>
-      <c r="D225" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>845</v>
+      </c>
+      <c r="B226" t="s">
         <v>846</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
         <v>847</v>
       </c>
-      <c r="C226" t="s">
+      <c r="D226" t="s">
         <v>848</v>
-      </c>
-      <c r="D226" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>849</v>
+      </c>
+      <c r="B227" t="s">
         <v>850</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
         <v>851</v>
       </c>
-      <c r="C227" t="s">
+      <c r="D227" t="s">
         <v>852</v>
-      </c>
-      <c r="D227" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>853</v>
+      </c>
+      <c r="B228" t="s">
         <v>854</v>
       </c>
-      <c r="B228" t="s">
+      <c r="C228" t="s">
         <v>855</v>
       </c>
-      <c r="C228" t="s">
+      <c r="D228" t="s">
         <v>856</v>
-      </c>
-      <c r="D228" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>857</v>
+      </c>
+      <c r="B229" t="s">
         <v>858</v>
       </c>
-      <c r="B229" t="s">
+      <c r="C229" t="s">
         <v>859</v>
       </c>
-      <c r="C229" t="s">
+      <c r="D229" t="s">
         <v>860</v>
-      </c>
-      <c r="D229" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>861</v>
+      </c>
+      <c r="B230" t="s">
         <v>862</v>
       </c>
-      <c r="B230" t="s">
+      <c r="C230" t="s">
         <v>863</v>
       </c>
-      <c r="C230" t="s">
+      <c r="D230" t="s">
         <v>864</v>
-      </c>
-      <c r="D230" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>865</v>
+      </c>
+      <c r="B231" t="s">
         <v>866</v>
       </c>
-      <c r="B231" t="s">
+      <c r="C231" t="s">
         <v>867</v>
       </c>
-      <c r="C231" t="s">
+      <c r="D231" t="s">
         <v>868</v>
-      </c>
-      <c r="D231" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>869</v>
+      </c>
+      <c r="B232" t="s">
         <v>870</v>
       </c>
-      <c r="B232" t="s">
+      <c r="C232" t="s">
         <v>871</v>
       </c>
-      <c r="C232" t="s">
+      <c r="D232" t="s">
         <v>872</v>
-      </c>
-      <c r="D232" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>873</v>
+      </c>
+      <c r="B233" t="s">
         <v>874</v>
       </c>
-      <c r="B233" t="s">
+      <c r="C233" t="s">
         <v>875</v>
       </c>
-      <c r="C233" t="s">
+      <c r="D233" t="s">
         <v>876</v>
-      </c>
-      <c r="D233" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>877</v>
+      </c>
+      <c r="B234" t="s">
         <v>878</v>
       </c>
-      <c r="B234" t="s">
+      <c r="C234" t="s">
         <v>879</v>
       </c>
-      <c r="C234" t="s">
+      <c r="D234" t="s">
         <v>880</v>
-      </c>
-      <c r="D234" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
+        <v>881</v>
+      </c>
+      <c r="B235" t="s">
         <v>882</v>
       </c>
-      <c r="B235" t="s">
+      <c r="C235" t="s">
         <v>883</v>
       </c>
-      <c r="C235" t="s">
+      <c r="D235" t="s">
         <v>884</v>
-      </c>
-      <c r="D235" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>885</v>
+      </c>
+      <c r="B236" t="s">
         <v>886</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
         <v>887</v>
       </c>
-      <c r="C236" t="s">
+      <c r="D236" t="s">
         <v>888</v>
-      </c>
-      <c r="D236" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
+        <v>889</v>
+      </c>
+      <c r="B237" t="s">
         <v>890</v>
       </c>
-      <c r="B237" t="s">
+      <c r="C237" t="s">
         <v>891</v>
       </c>
-      <c r="C237" t="s">
+      <c r="D237" t="s">
         <v>892</v>
-      </c>
-      <c r="D237" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>893</v>
+      </c>
+      <c r="B238" t="s">
         <v>894</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>895</v>
       </c>
-      <c r="C238" t="s">
+      <c r="D238" t="s">
         <v>896</v>
-      </c>
-      <c r="D238" t="s">
-        <v>897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add EB 97.1 (ZA7886)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ED4661-1155-425F-8ED3-361A3A2A3957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D6899-B660-4180-AC15-3862DCC0BA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="936">
   <si>
     <t>archive_id</t>
   </si>
@@ -2816,6 +2816,18 @@
   </si>
   <si>
     <t>February-March 2006</t>
+  </si>
+  <si>
+    <t>ZA7886</t>
+  </si>
+  <si>
+    <t>97.1</t>
+  </si>
+  <si>
+    <t>Europeans, Agriculture and the CAP (COVID-19 Pandemic)</t>
+  </si>
+  <si>
+    <t>February-March 2022</t>
   </si>
 </sst>
 </file>
@@ -3150,10 +3162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D238"/>
+  <dimension ref="A1:D239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C113" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3178,2798 +3190,2798 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C2" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D2" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C3" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D3" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C4" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D4" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C5" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D5" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C6" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D6" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C7" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D7" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C8" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D8" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C9" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D9" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>911</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D37" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
         <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D50" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D51" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D55" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C56" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D57" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B58" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D58" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B59" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D59" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C60" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D60" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B61" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D61" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B62" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C62" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D62" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B63" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C63" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D63" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D64" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C65" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D65" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B66" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C66" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D66" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B67" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C67" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D67" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B68" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C68" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D68" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B69" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C69" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D69" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B70" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C70" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D70" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B71" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C71" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D71" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B72" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C72" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D72" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B73" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C73" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D73" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B74" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C74" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D74" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B75" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C75" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D75" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B76" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C76" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D76" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B77" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C77" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D77" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B78" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C78" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D78" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B79" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C79" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D79" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B80" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C80" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D80" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B81" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C81" t="s">
         <v>276</v>
       </c>
       <c r="D81" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B82" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C82" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D82" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B83" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C83" t="s">
         <v>283</v>
       </c>
       <c r="D83" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B84" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C84" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D84" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B85" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C85" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D85" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B86" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C86" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D86" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B87" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C87" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D87" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B88" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C88" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D88" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B89" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C89" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D89" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B90" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C90" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D90" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B91" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C91" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D91" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B92" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C92" t="s">
         <v>318</v>
       </c>
       <c r="D92" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B93" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C93" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D93" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B94" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C94" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D94" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B95" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C95" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D95" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B96" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C96" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D96" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B97" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C97" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D97" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B98" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C98" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D98" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B99" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C99" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D99" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B100" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C100" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D100" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B101" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C101" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D101" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B102" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C102" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D102" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B103" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C103" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D103" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B104" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C104" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D104" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B105" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C105" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D105" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B106" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C106" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D106" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B107" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C107" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D107" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B108" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C108" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D108" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B109" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C109" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D109" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B110" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C110" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D110" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B111" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C111" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D111" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B112" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C112" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D112" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B113" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C113" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D113" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B114" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C114" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D114" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B115" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C115" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D115" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B116" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C116" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D116" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B117" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C117" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D117" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B118" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C118" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D118" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B119" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C119" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D119" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B120" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C120" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D120" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B121" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C121" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D121" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B122" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C122" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D122" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B123" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C123" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D123" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B124" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C124" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D124" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B125" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C125" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D125" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B126" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C126" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D126" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B127" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C127" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D127" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B128" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C128" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D128" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B129" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C129" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D129" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B130" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C130" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D130" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B131" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C131" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D131" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B132" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C132" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D132" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B133" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C133" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D133" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B134" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C134" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D134" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B135" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C135" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D135" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B136" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C136" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D136" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B137" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C137" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D137" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B138" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C138" t="s">
         <v>500</v>
       </c>
       <c r="D138" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B139" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C139" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D139" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B140" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C140" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D140" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B141" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C141" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D141" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B142" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C142" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D142" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B143" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C143" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D143" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B144" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C144" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D144" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B145" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C145" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D145" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B146" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C146" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D146" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B147" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C147" t="s">
         <v>535</v>
       </c>
       <c r="D147" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B148" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C148" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D148" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B149" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C149" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D149" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B150" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C150" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D150" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B151" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C151" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D151" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B152" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C152" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D152" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B153" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C153" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D153" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B154" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C154" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D154" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B155" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C155" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D155" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B156" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C156" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D156" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B157" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C157" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D157" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B158" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C158" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D158" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B159" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C159" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D159" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B160" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C160" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D160" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B161" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C161" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D161" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B162" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C162" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D162" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B163" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C163" t="s">
         <v>598</v>
       </c>
       <c r="D163" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B164" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C164" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D164" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B165" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C165" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D165" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B166" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C166" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D166" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B167" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C167" t="s">
         <v>613</v>
       </c>
       <c r="D167" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B168" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C168" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D168" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B169" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C169" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D169" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B170" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C170" t="s">
         <v>624</v>
       </c>
       <c r="D170" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B171" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C171" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D171" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B172" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C172" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D172" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B173" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C173" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D173" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B174" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C174" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D174" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B175" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C175" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D175" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B176" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C176" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D176" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B177" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C177" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D177" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B178" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C178" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D178" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B179" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C179" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D179" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B180" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C180" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D180" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B181" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C181" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D181" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B182" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C182" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D182" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B183" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C183" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D183" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B184" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C184" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D184" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B185" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C185" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D185" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B186" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C186" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D186" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B187" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C187" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D187" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B188" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C188" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D188" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B189" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C189" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D189" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B190" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C190" t="s">
         <v>703</v>
       </c>
       <c r="D190" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B191" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C191" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D191" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B192" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C192" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D192" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B193" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C193" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D193" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B194" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C194" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D194" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B195" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C195" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D195" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B196" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C196" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D196" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B197" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C197" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D197" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B198" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C198" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D198" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B199" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C199" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D199" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B200" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C200" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D200" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B201" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C201" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D201" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B202" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C202" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D202" t="s">
         <v>751</v>
@@ -5977,505 +5989,519 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B203" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C203" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D203" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B204" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C204" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D204" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B205" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C205" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D205" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B206" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C206" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D206" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B207" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C207" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D207" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B208" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C208" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D208" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B209" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C209" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D209" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B210" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C210" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D210" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B211" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C211" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D211" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B212" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C212" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D212" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B213" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C213" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D213" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B214" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C214" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D214" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B215" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C215" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D215" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B216" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C216" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D216" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B217" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C217" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D217" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B218" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C218" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D218" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B219" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C219" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D219" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B220" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C220" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D220" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B221" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C221" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D221" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B222" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C222" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D222" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B223" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C223" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D223" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B224" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C224" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D224" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B225" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C225" t="s">
         <v>840</v>
       </c>
       <c r="D225" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B226" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C226" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D226" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B227" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C227" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D227" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B228" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C228" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D228" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B229" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C229" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D229" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B230" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C230" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D230" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B231" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C231" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D231" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B232" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C232" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D232" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B233" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C233" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D233" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B234" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C234" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D234" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B235" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C235" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D235" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B236" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C236" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D236" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B237" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C237" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D237" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>889</v>
+      </c>
+      <c r="B238" t="s">
+        <v>890</v>
+      </c>
+      <c r="C238" t="s">
+        <v>891</v>
+      </c>
+      <c r="D238" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
         <v>893</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B239" t="s">
         <v>894</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C239" t="s">
         <v>895</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D239" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 97.2 (ZA7887) and EB 97.3 (ZA7888)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D6899-B660-4180-AC15-3862DCC0BA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF02B97-A741-4162-AB48-C222A230CCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="944">
   <si>
     <t>archive_id</t>
   </si>
@@ -2828,6 +2828,30 @@
   </si>
   <si>
     <t>February-March 2022</t>
+  </si>
+  <si>
+    <t>ZA7887</t>
+  </si>
+  <si>
+    <t>97.2</t>
+  </si>
+  <si>
+    <t>ZA7888</t>
+  </si>
+  <si>
+    <t>97.3</t>
+  </si>
+  <si>
+    <t>March-April 2022</t>
+  </si>
+  <si>
+    <t>Corruption and Attitudes of Europeans towards Air Quality</t>
+  </si>
+  <si>
+    <t>April-May 2022</t>
+  </si>
+  <si>
+    <t>European Parliament Spring Survey, Sport and Physical Activity, and Key Challenges of our Times - The EU in 2022</t>
   </si>
 </sst>
 </file>
@@ -3162,10 +3186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D239"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3190,55 +3214,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>932</v>
+        <v>938</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>933</v>
+        <v>939</v>
       </c>
       <c r="C2" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="D2" t="s">
-        <v>934</v>
+        <v>943</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>924</v>
+        <v>936</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>925</v>
+        <v>937</v>
       </c>
       <c r="C3" t="s">
-        <v>926</v>
+        <v>940</v>
       </c>
       <c r="D3" t="s">
-        <v>906</v>
+        <v>941</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>920</v>
+        <v>932</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>921</v>
+        <v>933</v>
       </c>
       <c r="C4" t="s">
-        <v>922</v>
+        <v>935</v>
       </c>
       <c r="D4" t="s">
-        <v>923</v>
+        <v>934</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>908</v>
+        <v>924</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>909</v>
+        <v>925</v>
       </c>
       <c r="C5" t="s">
-        <v>910</v>
+        <v>926</v>
       </c>
       <c r="D5" t="s">
         <v>906</v>
@@ -3246,3262 +3270,3290 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="C6" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="D6" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>901</v>
+        <v>909</v>
       </c>
       <c r="C7" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="D7" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>904</v>
+        <v>916</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>905</v>
+        <v>917</v>
       </c>
       <c r="C8" t="s">
-        <v>907</v>
+        <v>918</v>
       </c>
       <c r="D8" t="s">
-        <v>906</v>
+        <v>919</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="C9" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="D9" t="s">
-        <v>915</v>
+        <v>903</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>927</v>
+        <v>904</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>928</v>
+        <v>905</v>
       </c>
       <c r="C10" t="s">
-        <v>929</v>
+        <v>907</v>
       </c>
       <c r="D10" t="s">
-        <v>930</v>
+        <v>906</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
+        <v>897</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>898</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>899</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>915</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
+        <v>927</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>929</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>930</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>911</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>913</v>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>914</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
+        <v>911</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>914</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="D38" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D41" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C46" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D51" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C52" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C53" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D54" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C55" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D55" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D56" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C57" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D57" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C58" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D58" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C59" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C61" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D61" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C62" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C63" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D64" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C65" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D65" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B66" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C66" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D66" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B67" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C67" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D67" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B68" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C68" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D68" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B69" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C69" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D69" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B70" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C70" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D70" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B71" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C71" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D71" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B72" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C72" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D72" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C73" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D73" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B74" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C74" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D74" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B75" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C75" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D75" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B76" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C76" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D76" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C77" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D77" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B78" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C78" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D78" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B79" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C79" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D79" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B80" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C80" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D80" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B81" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C81" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D81" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B82" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C82" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D82" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B83" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C83" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D83" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B84" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C84" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D84" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B85" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C85" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D85" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B86" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C86" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D86" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B87" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C87" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D87" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B88" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C88" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D88" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B89" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C89" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D89" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B90" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C90" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D90" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B91" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C91" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D91" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B92" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C92" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D92" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B93" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C93" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D93" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B94" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C94" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D94" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B95" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C95" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D95" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B96" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C96" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D96" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B97" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C97" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D97" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B98" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C98" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D98" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B99" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C99" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D99" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B100" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C100" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D100" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B101" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C101" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D101" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B102" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C102" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D102" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B103" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C103" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D103" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B104" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C104" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D104" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B105" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C105" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D105" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B106" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C106" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D106" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B107" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C107" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D107" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B108" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C108" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D108" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B109" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C109" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D109" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B110" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C110" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D110" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B111" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C111" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D111" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B112" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C112" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D112" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B113" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C113" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D113" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B114" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C114" t="s">
-        <v>931</v>
+        <v>397</v>
       </c>
       <c r="D114" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B115" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C115" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D115" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B116" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C116" t="s">
-        <v>412</v>
+        <v>931</v>
       </c>
       <c r="D116" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B117" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C117" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="D117" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B118" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C118" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="D118" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B119" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C119" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="D119" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B120" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C120" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="D120" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B121" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C121" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="D121" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B122" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C122" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="D122" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B123" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C123" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="D123" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B124" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C124" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D124" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B125" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C125" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D125" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B126" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C126" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="D126" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B127" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C127" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D127" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B128" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C128" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D128" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B129" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="C129" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="D129" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B130" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="C130" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="D130" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B131" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C131" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D131" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B132" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C132" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="D132" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B133" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C133" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D133" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B134" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C134" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D134" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B135" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C135" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D135" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B136" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C136" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D136" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B137" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C137" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D137" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B138" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C138" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D138" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B139" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="C139" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D139" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B140" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C140" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D140" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="B141" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="C141" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="D141" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B142" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C142" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="D142" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B143" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C143" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="D143" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B144" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C144" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D144" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B145" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C145" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="D145" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="B146" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C146" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="D146" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B147" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C147" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="D147" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="B148" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C148" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D148" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B149" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C149" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D149" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="B150" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C150" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="D150" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="B151" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C151" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="D151" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="B152" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="C152" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="D152" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="B153" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="C153" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="D153" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B154" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="C154" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D154" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B155" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C155" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D155" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B156" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C156" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="D156" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="B157" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="C157" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="D157" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B158" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C158" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D158" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B159" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="C159" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="D159" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B160" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="C160" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="D160" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B161" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C161" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D161" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B162" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="C162" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D162" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B163" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C163" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="D163" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="B164" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C164" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D164" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="B165" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="C165" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D165" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="B166" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="C166" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="D166" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="B167" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="C167" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="D167" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="B168" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="C168" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D168" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="B169" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="C169" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D169" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="B170" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="C170" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="D170" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="B171" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="C171" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D171" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="B172" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="C172" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D172" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="B173" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="C173" t="s">
-        <v>635</v>
+        <v>624</v>
       </c>
       <c r="D173" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="B174" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="C174" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="D174" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="B175" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="C175" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="D175" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="B176" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="C176" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="D176" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="B177" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="C177" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="D177" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="B178" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="C178" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="D178" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="B179" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="C179" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="D179" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="B180" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="C180" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="D180" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="B181" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="C181" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="D181" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="B182" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="C182" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="D182" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="B183" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="C183" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="D183" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="B184" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="C184" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="D184" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="B185" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="C185" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D185" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="B186" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="C186" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="D186" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B187" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="C187" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="D187" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="B188" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="C188" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="D188" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="B189" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C189" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="D189" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="B190" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="C190" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="D190" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="B191" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="C191" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D191" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="B192" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="C192" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D192" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="B193" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="C193" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="D193" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="B194" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="C194" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="D194" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="B195" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="C195" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="D195" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="B196" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="C196" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="D196" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="B197" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="C197" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="D197" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="B198" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="C198" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="D198" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="B199" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="C199" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="D199" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="B200" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="C200" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="D200" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="B201" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="C201" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="D201" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="B202" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="C202" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="D202" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="B203" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="C203" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="D203" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>755</v>
+        <v>748</v>
       </c>
       <c r="B204" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
       <c r="C204" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="D204" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="B205" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="C205" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="D205" t="s">
-        <v>762</v>
+        <v>751</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="B206" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="C206" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D206" t="s">
-        <v>599</v>
+        <v>758</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="B207" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="C207" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
       <c r="D207" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="B208" t="s">
-        <v>771</v>
+        <v>764</v>
       </c>
       <c r="C208" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
       <c r="D208" t="s">
-        <v>773</v>
+        <v>599</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="B209" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="C209" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="D209" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="B210" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="C210" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="D210" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="B211" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="C211" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D211" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="B212" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="C212" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="D212" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="B213" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="C213" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="D213" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="B214" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="C214" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="D214" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="B215" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="C215" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="D215" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="B216" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="C216" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="D216" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="B217" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="C217" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="D217" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="B218" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="C218" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="D218" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B219" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="C219" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="D219" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="B220" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="C220" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="D220" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="B221" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="C221" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="D221" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="B222" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="C222" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="D222" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="B223" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="C223" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="D223" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="B224" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="C224" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="D224" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="B225" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="C225" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="D225" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="B226" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="C226" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D226" t="s">
-        <v>844</v>
+        <v>837</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
       <c r="B227" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="C227" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D227" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="B228" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="C228" t="s">
-        <v>851</v>
+        <v>840</v>
       </c>
       <c r="D228" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="B229" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="C229" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="D229" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="B230" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="C230" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="D230" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="B231" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="C231" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="D231" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="B232" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="C232" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="D232" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="B233" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="C233" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="D233" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="B234" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="C234" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="D234" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="B235" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="C235" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="D235" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="B236" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="C236" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="D236" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="B237" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="C237" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="D237" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="B238" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="C238" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="D238" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>885</v>
+      </c>
+      <c r="B239" t="s">
+        <v>886</v>
+      </c>
+      <c r="C239" t="s">
+        <v>887</v>
+      </c>
+      <c r="D239" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>889</v>
+      </c>
+      <c r="B240" t="s">
+        <v>890</v>
+      </c>
+      <c r="C240" t="s">
+        <v>891</v>
+      </c>
+      <c r="D240" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
         <v>893</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B241" t="s">
         <v>894</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C241" t="s">
         <v>895</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D241" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 97.5 (ZA7902)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF02B97-A741-4162-AB48-C222A230CCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A438B18B-49E0-432B-BAE3-0DB475CE8D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="948">
   <si>
     <t>archive_id</t>
   </si>
@@ -2852,6 +2852,18 @@
   </si>
   <si>
     <t>European Parliament Spring Survey, Sport and Physical Activity, and Key Challenges of our Times - The EU in 2022</t>
+  </si>
+  <si>
+    <t>ZA7902</t>
+  </si>
+  <si>
+    <t>97.5</t>
+  </si>
+  <si>
+    <t>Standard Eurobarometer 97 (COVID-19 Pandemic)</t>
+  </si>
+  <si>
+    <t>June-July 2022</t>
   </si>
 </sst>
 </file>
@@ -3186,10 +3198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3214,2840 +3226,2840 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>938</v>
+        <v>944</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>939</v>
+        <v>945</v>
       </c>
       <c r="C2" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
       <c r="D2" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C3" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D3" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C4" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D4" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C5" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D5" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C6" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D6" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C7" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D7" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C8" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D8" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C9" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D9" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C10" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D10" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C11" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D11" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C12" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D12" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>911</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D36" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D40" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
         <v>121</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D46" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D52" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B54" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D55" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D58" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D59" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C60" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D60" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C61" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D61" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D62" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C63" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C64" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D64" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C65" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D65" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B66" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C66" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D66" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C67" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D67" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C68" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D68" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C69" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D69" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B71" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C71" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D71" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B72" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C72" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D72" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B73" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C73" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D73" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B74" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C74" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D74" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C75" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D75" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B76" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C76" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B77" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C77" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D77" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C78" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D78" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B79" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C79" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D79" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B80" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C80" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D80" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B81" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C81" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D81" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B82" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C82" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D82" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B83" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C83" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D83" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B84" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C84" t="s">
         <v>276</v>
       </c>
       <c r="D84" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B85" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C85" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D85" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B86" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C86" t="s">
         <v>283</v>
       </c>
       <c r="D86" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B87" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C87" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D87" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B88" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C88" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D88" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B89" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C89" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D89" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B90" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C90" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D90" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B91" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C91" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D91" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B92" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C92" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D92" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B93" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C93" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D93" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B94" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C94" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D94" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B95" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C95" t="s">
         <v>318</v>
       </c>
       <c r="D95" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B96" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C96" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D96" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B97" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C97" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D97" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B98" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C98" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D98" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B99" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C99" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D99" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B100" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C100" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D100" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B101" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C101" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D101" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B102" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C102" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D102" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B103" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C103" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D103" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B104" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C104" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D104" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B105" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C105" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D105" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B106" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C106" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D106" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B107" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C107" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D107" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B108" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C108" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D108" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B109" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C109" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D109" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B110" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C110" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D110" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B111" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C111" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D111" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B112" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C112" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D112" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B113" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C113" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D113" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B114" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C114" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D114" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B115" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C115" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D115" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B116" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C116" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D116" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B117" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C117" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D117" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B118" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C118" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D118" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B119" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C119" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D119" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B120" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C120" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D120" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B121" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C121" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D121" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B122" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C122" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D122" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B123" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C123" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D123" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B124" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C124" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D124" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B125" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C125" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D125" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B126" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C126" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D126" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B127" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C127" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D127" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B128" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C128" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D128" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B129" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C129" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D129" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B130" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C130" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D130" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B131" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C131" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D131" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B132" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C132" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D132" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B133" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C133" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D133" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B134" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C134" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D134" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B135" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C135" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D135" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B136" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C136" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D136" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B137" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C137" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D137" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B138" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C138" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D138" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B139" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C139" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D139" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B140" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C140" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D140" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B141" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C141" t="s">
         <v>500</v>
       </c>
       <c r="D141" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B142" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C142" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D142" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B143" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C143" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D143" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B144" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C144" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D144" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B145" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C145" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D145" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B146" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C146" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D146" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B147" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C147" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D147" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B148" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C148" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D148" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B149" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C149" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D149" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B150" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C150" t="s">
         <v>535</v>
       </c>
       <c r="D150" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B151" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C151" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D151" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B152" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C152" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D152" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B153" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C153" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D153" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B154" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C154" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D154" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B155" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C155" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D155" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B156" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C156" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D156" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B157" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C157" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D157" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B158" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C158" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D158" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B159" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C159" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D159" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B160" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C160" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D160" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B161" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C161" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D161" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B162" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C162" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D162" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B163" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C163" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D163" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B164" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C164" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D164" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B165" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C165" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D165" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B166" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C166" t="s">
         <v>598</v>
       </c>
       <c r="D166" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B167" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C167" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D167" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B168" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C168" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D168" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B169" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C169" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D169" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B170" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C170" t="s">
         <v>613</v>
       </c>
       <c r="D170" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B171" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C171" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D171" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B172" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C172" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D172" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B173" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C173" t="s">
         <v>624</v>
       </c>
       <c r="D173" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B174" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C174" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D174" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B175" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C175" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D175" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B176" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C176" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D176" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B177" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C177" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D177" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B178" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C178" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D178" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B179" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C179" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D179" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B180" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C180" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D180" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B181" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C181" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D181" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B182" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C182" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D182" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B183" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C183" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D183" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B184" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C184" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D184" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B185" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C185" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D185" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B186" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C186" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D186" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B187" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C187" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D187" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B188" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C188" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D188" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B189" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C189" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D189" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B190" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C190" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D190" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B191" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C191" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D191" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B192" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C192" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D192" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B193" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C193" t="s">
         <v>703</v>
       </c>
       <c r="D193" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B194" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C194" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D194" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B195" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C195" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D195" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B196" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C196" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D196" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B197" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C197" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D197" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B198" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C198" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D198" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B199" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C199" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D199" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B200" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C200" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D200" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B201" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C201" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D201" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B202" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C202" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D202" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B203" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C203" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D203" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B204" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C204" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D204" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B205" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C205" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D205" t="s">
         <v>751</v>
@@ -6055,505 +6067,519 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B206" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C206" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D206" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B207" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C207" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D207" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B208" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C208" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D208" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B209" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C209" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D209" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B210" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C210" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D210" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B211" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C211" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D211" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B212" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C212" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D212" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B213" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C213" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D213" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B214" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C214" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D214" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B215" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C215" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D215" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B216" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C216" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D216" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B217" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C217" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D217" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B218" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C218" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D218" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B219" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C219" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D219" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B220" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C220" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D220" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B221" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C221" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D221" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B222" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C222" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D222" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B223" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C223" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D223" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B224" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C224" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D224" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B225" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C225" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D225" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B226" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C226" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D226" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B227" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C227" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D227" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B228" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C228" t="s">
         <v>840</v>
       </c>
       <c r="D228" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B229" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C229" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D229" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B230" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C230" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D230" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B231" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C231" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D231" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B232" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C232" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D232" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B233" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C233" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D233" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B234" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C234" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D234" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B235" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C235" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D235" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B236" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C236" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D236" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B237" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C237" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D237" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B238" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C238" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D238" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B239" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C239" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D239" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B240" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C240" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D240" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
+        <v>889</v>
+      </c>
+      <c r="B241" t="s">
+        <v>890</v>
+      </c>
+      <c r="C241" t="s">
+        <v>891</v>
+      </c>
+      <c r="D241" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
         <v>893</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B242" t="s">
         <v>894</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C242" t="s">
         <v>895</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D242" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 98.2 (add EB 97.5 ZA7953)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A438B18B-49E0-432B-BAE3-0DB475CE8D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D626F2-ECFA-463E-BB48-9C3BCD543E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="952">
   <si>
     <t>archive_id</t>
   </si>
@@ -2864,6 +2864,18 @@
   </si>
   <si>
     <t>June-July 2022</t>
+  </si>
+  <si>
+    <t>ZA7953</t>
+  </si>
+  <si>
+    <t>98.2</t>
+  </si>
+  <si>
+    <t>Standard Eurobarometer 98 (COVID-19 Pandemic)</t>
+  </si>
+  <si>
+    <t>January-February 2023</t>
   </si>
 </sst>
 </file>
@@ -3198,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D242"/>
+  <dimension ref="A1:D243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3226,2854 +3238,2854 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="C2" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="D2" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>938</v>
+        <v>944</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>939</v>
+        <v>945</v>
       </c>
       <c r="C3" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
       <c r="D3" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C4" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D4" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C5" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D5" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C6" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D6" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C7" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D7" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C8" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D8" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C9" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D9" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C10" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D10" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C11" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D11" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C12" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D12" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C13" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D13" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>911</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D43" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
         <v>121</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D55" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B56" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D56" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D57" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D58" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D59" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D61" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D62" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B64" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C64" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D64" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B65" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D65" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B66" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C66" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D66" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D67" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C68" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B69" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C69" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C70" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D70" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B71" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D71" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C72" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D72" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B73" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C73" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D73" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B74" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C74" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D74" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B75" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C75" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B76" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C76" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D76" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C77" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D77" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B78" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C78" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D78" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B79" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C79" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D79" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B80" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C80" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D80" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B81" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C81" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B82" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C82" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D82" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B83" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C83" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D83" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B84" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C84" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D84" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B85" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C85" t="s">
         <v>276</v>
       </c>
       <c r="D85" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B86" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C86" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D86" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B87" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C87" t="s">
         <v>283</v>
       </c>
       <c r="D87" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B88" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C88" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D88" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B89" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C89" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D89" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B90" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D90" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B91" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C91" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D91" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B92" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C92" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D92" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B93" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C93" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D93" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B94" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C94" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D94" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B95" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C95" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D95" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B96" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C96" t="s">
         <v>318</v>
       </c>
       <c r="D96" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B97" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C97" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D97" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B98" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C98" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D98" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B99" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C99" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D99" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B100" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C100" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D100" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B101" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C101" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D101" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B102" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C102" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D102" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B103" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C103" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D103" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B104" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C104" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D104" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B105" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C105" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D105" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B106" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C106" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D106" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B107" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C107" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D107" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B108" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C108" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D108" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B109" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C109" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D109" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B110" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C110" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D110" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B111" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C111" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D111" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B112" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C112" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D112" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B113" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C113" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D113" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B114" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C114" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D114" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B115" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C115" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D115" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B116" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C116" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D116" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B117" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C117" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D117" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B118" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C118" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D118" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B119" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C119" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D119" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B120" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C120" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D120" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B121" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C121" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D121" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B122" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C122" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D122" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B123" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C123" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D123" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B124" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C124" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D124" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B125" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C125" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D125" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B126" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C126" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D126" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B127" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C127" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D127" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B128" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C128" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D128" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B129" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C129" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D129" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B130" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C130" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D130" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B131" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C131" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D131" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B132" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C132" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D132" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B133" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C133" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D133" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B134" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C134" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D134" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B135" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C135" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D135" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B136" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C136" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D136" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B137" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C137" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D137" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B138" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C138" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D138" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B139" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C139" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D139" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B140" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C140" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D140" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B141" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C141" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D141" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B142" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C142" t="s">
         <v>500</v>
       </c>
       <c r="D142" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B143" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C143" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D143" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B144" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C144" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D144" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B145" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C145" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D145" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B146" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C146" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D146" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B147" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C147" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D147" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B148" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C148" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D148" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B149" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C149" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D149" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B150" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C150" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D150" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B151" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C151" t="s">
         <v>535</v>
       </c>
       <c r="D151" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B152" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C152" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D152" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B153" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C153" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D153" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B154" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C154" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D154" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B155" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C155" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D155" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B156" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C156" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D156" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B157" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C157" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D157" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B158" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C158" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D158" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B159" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C159" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D159" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B160" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C160" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D160" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B161" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C161" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D161" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B162" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C162" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D162" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B163" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C163" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D163" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B164" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C164" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D164" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B165" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C165" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D165" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B166" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C166" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D166" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B167" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C167" t="s">
         <v>598</v>
       </c>
       <c r="D167" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B168" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C168" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D168" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B169" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C169" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D169" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B170" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C170" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D170" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B171" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C171" t="s">
         <v>613</v>
       </c>
       <c r="D171" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B172" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C172" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D172" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B173" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C173" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D173" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B174" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C174" t="s">
         <v>624</v>
       </c>
       <c r="D174" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B175" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C175" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D175" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B176" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C176" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D176" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B177" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C177" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D177" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B178" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C178" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D178" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B179" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C179" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D179" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B180" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C180" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D180" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B181" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C181" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D181" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B182" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C182" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D182" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B183" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C183" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D183" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B184" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C184" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D184" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B185" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C185" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D185" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B186" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C186" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D186" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B187" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C187" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D187" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B188" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C188" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D188" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B189" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C189" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D189" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B190" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C190" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D190" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B191" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C191" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D191" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B192" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C192" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D192" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B193" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C193" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D193" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B194" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C194" t="s">
         <v>703</v>
       </c>
       <c r="D194" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B195" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C195" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D195" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B196" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C196" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D196" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B197" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C197" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D197" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B198" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C198" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D198" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B199" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C199" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D199" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B200" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C200" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D200" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B201" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C201" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D201" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B202" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C202" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D202" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B203" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C203" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D203" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B204" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C204" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D204" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B205" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C205" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D205" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B206" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C206" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D206" t="s">
         <v>751</v>
@@ -6081,505 +6093,519 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B207" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C207" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D207" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B208" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C208" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D208" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B209" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C209" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D209" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B210" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C210" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D210" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B211" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C211" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D211" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B212" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C212" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D212" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B213" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C213" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D213" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B214" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C214" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D214" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B215" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C215" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D215" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B216" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C216" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D216" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B217" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C217" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D217" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B218" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C218" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D218" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B219" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C219" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D219" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B220" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C220" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D220" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B221" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C221" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D221" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B222" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C222" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D222" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B223" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C223" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D223" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B224" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C224" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D224" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B225" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C225" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D225" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B226" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C226" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D226" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B227" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C227" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D227" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B228" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C228" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D228" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B229" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C229" t="s">
         <v>840</v>
       </c>
       <c r="D229" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B230" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C230" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D230" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B231" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C231" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D231" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B232" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C232" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D232" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B233" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C233" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D233" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B234" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C234" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D234" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B235" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C235" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D235" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B236" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C236" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D236" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B237" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C237" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D237" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B238" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C238" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D238" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B239" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C239" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D239" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B240" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C240" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D240" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B241" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C241" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D241" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>889</v>
+      </c>
+      <c r="B242" t="s">
+        <v>890</v>
+      </c>
+      <c r="C242" t="s">
+        <v>891</v>
+      </c>
+      <c r="D242" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
         <v>893</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>894</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C243" t="s">
         <v>895</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D243" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 97.4 (ZA7901)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D626F2-ECFA-463E-BB48-9C3BCD543E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1755BD9B-504C-4048-81AE-67AB099822F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="956">
   <si>
     <t>archive_id</t>
   </si>
@@ -2876,6 +2876,18 @@
   </si>
   <si>
     <t>January-February 2023</t>
+  </si>
+  <si>
+    <t>ZA7901</t>
+  </si>
+  <si>
+    <t>97.4</t>
+  </si>
+  <si>
+    <t>May-June 2022</t>
+  </si>
+  <si>
+    <t>Fairness perceptions of the green transition</t>
   </si>
 </sst>
 </file>
@@ -3210,10 +3222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D243"/>
+  <dimension ref="A1:D244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3266,2840 +3278,2840 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>938</v>
+        <v>952</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>939</v>
+        <v>953</v>
       </c>
       <c r="C4" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="D4" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C5" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D5" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C6" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D6" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C7" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D7" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C8" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D8" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C9" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D9" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C10" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D10" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C11" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D11" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C12" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D12" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C13" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D13" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C14" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D14" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>911</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D42" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D44" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D46" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
         <v>121</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D57" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C58" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D59" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C60" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D60" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B61" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D62" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C63" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B64" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C65" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C66" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D66" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B67" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D67" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D68" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C70" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C71" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D71" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B72" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D72" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C73" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D73" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B74" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C74" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D74" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B75" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C75" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D75" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B76" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C76" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D76" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B77" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C77" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B78" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C78" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D78" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B79" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C79" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D79" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B80" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C80" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D80" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B81" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C81" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D81" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B82" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C82" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D82" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B83" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C83" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D83" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B84" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C84" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D84" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B85" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C85" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D85" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B86" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C86" t="s">
         <v>276</v>
       </c>
       <c r="D86" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B87" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C87" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D87" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B88" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C88" t="s">
         <v>283</v>
       </c>
       <c r="D88" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B89" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C89" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D89" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B90" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C90" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D90" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B91" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C91" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D91" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B92" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C92" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D92" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B93" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C93" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D93" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B94" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C94" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D94" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B95" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C95" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D95" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B96" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C96" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D96" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B97" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C97" t="s">
         <v>318</v>
       </c>
       <c r="D97" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B98" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C98" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D98" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B99" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C99" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D99" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B100" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C100" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D100" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B101" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C101" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D101" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B102" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C102" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D102" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B103" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C103" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D103" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B104" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C104" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D104" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B105" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C105" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D105" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B106" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C106" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D106" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B107" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C107" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D107" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B108" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C108" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D108" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B109" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C109" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D109" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B110" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C110" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D110" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B111" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C111" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D111" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B112" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C112" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D112" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B113" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C113" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D113" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B114" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C114" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D114" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B115" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C115" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D115" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B116" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C116" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D116" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B117" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C117" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D117" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B118" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C118" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D118" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B119" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C119" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D119" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B120" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C120" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D120" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B121" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C121" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D121" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B122" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C122" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D122" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B123" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C123" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D123" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B124" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C124" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D124" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B125" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C125" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D125" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B126" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C126" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D126" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B127" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C127" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D127" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B128" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C128" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D128" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B129" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C129" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D129" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B130" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C130" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D130" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B131" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C131" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D131" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B132" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C132" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D132" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B133" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C133" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D133" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B134" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C134" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D134" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B135" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C135" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D135" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B136" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C136" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D136" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B137" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C137" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D137" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B138" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C138" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D138" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B139" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C139" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D139" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B140" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C140" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D140" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B141" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C141" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D141" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B142" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C142" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D142" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B143" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C143" t="s">
         <v>500</v>
       </c>
       <c r="D143" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B144" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C144" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D144" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B145" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C145" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D145" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B146" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C146" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D146" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B147" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C147" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D147" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B148" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C148" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D148" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B149" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C149" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D149" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B150" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C150" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D150" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B151" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C151" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D151" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B152" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C152" t="s">
         <v>535</v>
       </c>
       <c r="D152" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B153" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C153" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D153" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B154" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C154" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D154" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B155" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C155" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D155" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B156" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C156" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D156" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B157" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C157" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D157" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B158" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C158" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D158" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B159" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C159" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D159" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B160" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C160" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D160" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B161" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C161" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D161" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B162" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C162" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D162" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B163" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C163" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D163" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B164" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C164" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D164" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B165" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C165" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D165" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B166" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C166" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D166" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B167" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C167" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D167" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B168" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C168" t="s">
         <v>598</v>
       </c>
       <c r="D168" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B169" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C169" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D169" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B170" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C170" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D170" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B171" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C171" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D171" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B172" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C172" t="s">
         <v>613</v>
       </c>
       <c r="D172" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B173" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C173" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D173" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B174" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C174" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D174" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B175" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C175" t="s">
         <v>624</v>
       </c>
       <c r="D175" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B176" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C176" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D176" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B177" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C177" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D177" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B178" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C178" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D178" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B179" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C179" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D179" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B180" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C180" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D180" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B181" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C181" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D181" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B182" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C182" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D182" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B183" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C183" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D183" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B184" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C184" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D184" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B185" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C185" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D185" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B186" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C186" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D186" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B187" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C187" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D187" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B188" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C188" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D188" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B189" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C189" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D189" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B190" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C190" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D190" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B191" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C191" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D191" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B192" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C192" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D192" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B193" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C193" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D193" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B194" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C194" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D194" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B195" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C195" t="s">
         <v>703</v>
       </c>
       <c r="D195" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B196" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C196" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D196" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B197" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C197" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D197" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B198" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C198" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D198" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B199" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C199" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D199" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B200" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C200" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D200" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B201" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C201" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D201" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B202" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C202" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D202" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B203" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C203" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D203" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B204" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C204" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D204" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B205" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C205" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D205" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B206" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C206" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D206" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B207" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C207" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D207" t="s">
         <v>751</v>
@@ -6107,505 +6119,519 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B208" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C208" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D208" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B209" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C209" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D209" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B210" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C210" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D210" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B211" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C211" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D211" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B212" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C212" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D212" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B213" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C213" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D213" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B214" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C214" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D214" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B215" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C215" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D215" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B216" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C216" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D216" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B217" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C217" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D217" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B218" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C218" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D218" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B219" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C219" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D219" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B220" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C220" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D220" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B221" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C221" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D221" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B222" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C222" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D222" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B223" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C223" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D223" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B224" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C224" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D224" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B225" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C225" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D225" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B226" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C226" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D226" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B227" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C227" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D227" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B228" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C228" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D228" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B229" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C229" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D229" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B230" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C230" t="s">
         <v>840</v>
       </c>
       <c r="D230" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B231" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C231" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D231" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B232" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C232" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D232" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B233" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C233" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D233" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B234" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C234" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D234" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B235" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C235" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D235" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B236" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C236" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D236" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B237" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C237" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D237" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B238" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C238" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D238" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B239" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C239" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D239" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B240" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C240" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D240" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B241" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C241" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D241" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B242" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C242" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D242" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
+        <v>889</v>
+      </c>
+      <c r="B243" t="s">
+        <v>890</v>
+      </c>
+      <c r="C243" t="s">
+        <v>891</v>
+      </c>
+      <c r="D243" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
         <v>893</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B244" t="s">
         <v>894</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C244" t="s">
         <v>895</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D244" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 99.4 (ZA7997)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1755BD9B-504C-4048-81AE-67AB099822F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9219E61F-7386-48CD-8F4B-1D40CA4E75CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="960">
   <si>
     <t>archive_id</t>
   </si>
@@ -2888,6 +2888,18 @@
   </si>
   <si>
     <t>Fairness perceptions of the green transition</t>
+  </si>
+  <si>
+    <t>ZA7997</t>
+  </si>
+  <si>
+    <t>99.4</t>
+  </si>
+  <si>
+    <t>May-June 2023</t>
+  </si>
+  <si>
+    <t>Standard Eurobarometer 99</t>
   </si>
 </sst>
 </file>
@@ -3222,10 +3234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D244"/>
+  <dimension ref="A1:D245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3250,2882 +3262,2882 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>948</v>
+        <v>956</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>949</v>
+        <v>957</v>
       </c>
       <c r="C2" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="D2" t="s">
-        <v>950</v>
+        <v>959</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="C3" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="D3" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C4" t="s">
-        <v>954</v>
+        <v>947</v>
       </c>
       <c r="D4" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>938</v>
+        <v>952</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>939</v>
+        <v>953</v>
       </c>
       <c r="C5" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="D5" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C6" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D6" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C7" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D7" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C8" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D8" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C9" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D9" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C10" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D10" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C11" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D11" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C12" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D12" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C13" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D13" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C14" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D14" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C15" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D15" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>911</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D39" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D43" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
         <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C57" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B59" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C59" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D59" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C60" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D60" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D61" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D62" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C63" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D63" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D64" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D65" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B66" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C66" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D68" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B69" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C69" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D69" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D70" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C71" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D71" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B72" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C72" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D72" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B73" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D73" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C74" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D74" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C75" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D75" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C76" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D76" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B77" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C77" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D77" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B78" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C78" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D78" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B79" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C79" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D79" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B80" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C80" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D80" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B81" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C81" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D81" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B82" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C82" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D82" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B83" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C83" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B84" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C84" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D84" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B85" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C85" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D85" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B86" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C86" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D86" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B87" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C87" t="s">
         <v>276</v>
       </c>
       <c r="D87" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B88" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C88" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D88" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B89" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C89" t="s">
         <v>283</v>
       </c>
       <c r="D89" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B90" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C90" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D90" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B91" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C91" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D91" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B92" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C92" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D92" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B93" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C93" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D93" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B94" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C94" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D94" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B95" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C95" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D95" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B96" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C96" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D96" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B97" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C97" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D97" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B98" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C98" t="s">
         <v>318</v>
       </c>
       <c r="D98" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B99" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C99" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D99" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B100" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C100" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D100" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B101" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C101" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D101" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B102" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C102" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D102" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B103" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C103" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D103" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B104" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C104" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D104" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B105" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C105" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D105" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B106" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C106" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D106" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B107" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C107" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D107" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B108" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C108" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D108" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B109" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C109" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D109" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B110" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C110" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D110" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B111" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C111" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D111" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B112" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C112" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D112" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B113" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C113" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D113" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B114" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C114" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D114" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B115" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C115" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D115" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B116" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C116" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D116" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B117" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C117" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D117" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B118" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C118" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D118" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B119" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C119" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D119" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B120" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C120" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D120" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B121" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C121" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D121" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B122" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C122" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D122" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B123" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C123" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D123" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B124" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C124" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D124" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B125" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C125" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D125" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B126" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C126" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D126" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B127" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C127" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D127" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B128" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C128" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D128" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B129" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C129" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D129" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B130" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C130" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D130" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B131" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C131" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D131" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B132" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C132" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D132" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B133" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C133" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D133" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B134" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C134" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D134" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B135" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C135" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D135" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B136" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C136" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D136" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B137" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C137" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D137" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B138" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C138" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D138" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B139" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C139" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D139" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B140" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C140" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D140" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B141" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C141" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D141" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B142" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C142" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D142" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B143" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C143" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D143" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B144" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C144" t="s">
         <v>500</v>
       </c>
       <c r="D144" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B145" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C145" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D145" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B146" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C146" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D146" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B147" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C147" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D147" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B148" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C148" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D148" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B149" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C149" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D149" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B150" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C150" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D150" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B151" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C151" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D151" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B152" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C152" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D152" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B153" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C153" t="s">
         <v>535</v>
       </c>
       <c r="D153" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B154" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C154" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D154" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B155" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C155" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D155" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B156" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C156" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D156" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B157" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C157" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D157" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B158" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C158" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D158" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B159" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C159" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D159" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B160" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C160" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D160" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B161" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D161" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B162" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C162" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D162" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B163" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C163" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D163" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B164" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C164" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D164" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B165" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C165" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D165" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B166" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C166" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D166" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B167" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C167" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D167" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B168" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C168" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D168" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B169" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C169" t="s">
         <v>598</v>
       </c>
       <c r="D169" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B170" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C170" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D170" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B171" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C171" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D171" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B172" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C172" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D172" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B173" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C173" t="s">
         <v>613</v>
       </c>
       <c r="D173" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B174" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C174" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D174" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B175" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C175" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D175" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B176" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C176" t="s">
         <v>624</v>
       </c>
       <c r="D176" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B177" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C177" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D177" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B178" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C178" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D178" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B179" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C179" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D179" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B180" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C180" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D180" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B181" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C181" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D181" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B182" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C182" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D182" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B183" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C183" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D183" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B184" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C184" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D184" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B185" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C185" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D185" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B186" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C186" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D186" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B187" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C187" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D187" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B188" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C188" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D188" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B189" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C189" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D189" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B190" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C190" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D190" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B191" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C191" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D191" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B192" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C192" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D192" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B193" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C193" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D193" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B194" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C194" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D194" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B195" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C195" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D195" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B196" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C196" t="s">
         <v>703</v>
       </c>
       <c r="D196" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B197" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C197" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D197" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B198" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C198" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D198" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B199" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C199" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D199" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B200" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C200" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D200" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B201" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C201" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D201" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B202" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C202" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D202" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B203" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C203" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D203" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B204" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C204" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D204" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B205" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C205" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D205" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B206" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C206" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D206" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B207" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C207" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D207" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B208" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C208" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D208" t="s">
         <v>751</v>
@@ -6133,505 +6145,519 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B209" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C209" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D209" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B210" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C210" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D210" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B211" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C211" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D211" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B212" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C212" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D212" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B213" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C213" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D213" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B214" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C214" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D214" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B215" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C215" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D215" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B216" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C216" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D216" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B217" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C217" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D217" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B218" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C218" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D218" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B219" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C219" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D219" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B220" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C220" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D220" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B221" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C221" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D221" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B222" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C222" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D222" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B223" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C223" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D223" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B224" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C224" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D224" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B225" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C225" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D225" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B226" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C226" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D226" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B227" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C227" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D227" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B228" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C228" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D228" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B229" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C229" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D229" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B230" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C230" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D230" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B231" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C231" t="s">
         <v>840</v>
       </c>
       <c r="D231" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B232" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C232" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D232" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B233" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C233" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D233" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B234" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C234" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D234" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B235" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C235" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D235" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B236" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C236" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D236" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B237" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C237" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D237" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B238" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C238" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D238" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B239" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C239" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D239" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B240" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C240" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D240" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B241" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C241" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D241" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B242" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C242" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D242" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B243" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C243" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D243" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
+        <v>889</v>
+      </c>
+      <c r="B244" t="s">
+        <v>890</v>
+      </c>
+      <c r="C244" t="s">
+        <v>891</v>
+      </c>
+      <c r="D244" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
         <v>893</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B245" t="s">
         <v>894</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C245" t="s">
         <v>895</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D245" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 100.2 (ZA8779)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9219E61F-7386-48CD-8F4B-1D40CA4E75CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5888FB-FB88-40DC-AAA7-5D36BDF105D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="964">
   <si>
     <t>archive_id</t>
   </si>
@@ -2900,6 +2900,18 @@
   </si>
   <si>
     <t>Standard Eurobarometer 99</t>
+  </si>
+  <si>
+    <t>ZA8779</t>
+  </si>
+  <si>
+    <t>100.2</t>
+  </si>
+  <si>
+    <t>October-November 2023</t>
+  </si>
+  <si>
+    <t>Standard Eurobarometer 100</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3246,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D245"/>
+  <dimension ref="A1:D246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -3262,2896 +3274,2896 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="C2" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="D2" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>948</v>
+        <v>956</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>949</v>
+        <v>957</v>
       </c>
       <c r="C3" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="D3" t="s">
-        <v>950</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="C4" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="D4" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C5" t="s">
-        <v>954</v>
+        <v>947</v>
       </c>
       <c r="D5" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>938</v>
+        <v>952</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>939</v>
+        <v>953</v>
       </c>
       <c r="C6" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="D6" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C7" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D7" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C8" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D8" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C9" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D9" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C10" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D10" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C11" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D11" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C12" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D12" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C13" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D13" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C14" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D14" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C15" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D15" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C16" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D16" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>911</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D40" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D43" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D44" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
         <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D51" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D54" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D55" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D57" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D58" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D59" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C60" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D60" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C61" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D61" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C62" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D62" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C63" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D63" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C64" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D64" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B65" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C65" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D65" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D66" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C67" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D67" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C68" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D68" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B69" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C69" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D69" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B70" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C70" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C71" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D71" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B72" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C72" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D72" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B73" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C73" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D73" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B74" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D74" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C75" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D75" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D76" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B77" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D77" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B78" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C78" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D78" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C79" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D79" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C80" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D80" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B81" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C81" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D81" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D82" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C83" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D83" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B84" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C84" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D84" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B85" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C85" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D85" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B86" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C86" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D86" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B87" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C87" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D87" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B88" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C88" t="s">
         <v>276</v>
       </c>
       <c r="D88" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B89" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C89" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D89" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B90" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C90" t="s">
         <v>283</v>
       </c>
       <c r="D90" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B91" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C91" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D91" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B92" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C92" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D92" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B93" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C93" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D93" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B94" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C94" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D94" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B95" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C95" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D95" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B96" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C96" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D96" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B97" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C97" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D97" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B98" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C98" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D98" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B99" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C99" t="s">
         <v>318</v>
       </c>
       <c r="D99" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B100" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C100" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D100" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B101" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C101" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D101" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B102" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C102" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D102" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B103" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C103" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D103" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B104" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C104" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D104" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B105" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C105" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D105" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B106" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C106" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D106" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B107" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C107" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D107" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B108" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C108" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D108" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B109" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C109" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D109" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B110" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C110" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D110" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B111" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C111" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D111" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B112" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C112" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D112" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B113" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C113" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D113" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B114" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C114" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D114" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B115" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C115" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D115" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B116" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C116" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D116" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B117" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C117" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D117" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B118" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C118" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D118" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B119" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C119" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D119" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B120" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C120" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D120" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B121" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C121" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D121" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B122" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C122" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D122" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B123" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C123" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D123" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B124" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C124" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D124" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B125" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C125" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D125" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B126" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C126" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D126" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B127" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C127" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D127" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B128" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C128" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D128" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B129" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C129" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D129" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B130" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C130" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D130" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B131" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C131" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D131" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B132" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C132" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D132" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B133" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C133" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D133" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B134" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C134" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D134" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B135" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C135" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D135" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B136" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C136" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D136" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B137" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C137" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D137" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B138" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C138" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D138" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B139" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C139" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D139" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B140" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C140" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D140" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B141" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C141" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D141" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B142" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C142" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D142" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B143" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C143" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D143" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B144" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C144" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D144" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B145" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C145" t="s">
         <v>500</v>
       </c>
       <c r="D145" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B146" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C146" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D146" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B147" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C147" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D147" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B148" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C148" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D148" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B149" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C149" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D149" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B150" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C150" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D150" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B151" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C151" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D151" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B152" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C152" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D152" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B153" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C153" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D153" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B154" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C154" t="s">
         <v>535</v>
       </c>
       <c r="D154" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B155" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C155" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D155" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B156" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C156" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D156" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B157" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C157" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D157" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B158" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C158" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D158" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B159" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C159" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D159" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B160" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C160" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D160" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B161" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C161" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D161" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B162" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C162" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D162" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B163" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C163" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D163" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B164" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C164" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D164" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B165" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C165" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D165" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B166" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C166" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D166" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B167" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C167" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D167" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B168" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C168" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D168" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B169" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C169" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D169" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B170" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C170" t="s">
         <v>598</v>
       </c>
       <c r="D170" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B171" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C171" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D171" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B172" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C172" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D172" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B173" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C173" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D173" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B174" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C174" t="s">
         <v>613</v>
       </c>
       <c r="D174" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B175" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C175" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D175" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B176" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C176" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D176" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B177" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C177" t="s">
         <v>624</v>
       </c>
       <c r="D177" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B178" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C178" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D178" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B179" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C179" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D179" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B180" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C180" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D180" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B181" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C181" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D181" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B182" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C182" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D182" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B183" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C183" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D183" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B184" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C184" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D184" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B185" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C185" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D185" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B186" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C186" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D186" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B187" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C187" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D187" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B188" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C188" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D188" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B189" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C189" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D189" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B190" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C190" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D190" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B191" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C191" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D191" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B192" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C192" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D192" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B193" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C193" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D193" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B194" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C194" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D194" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B195" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C195" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D195" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B196" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C196" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D196" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B197" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C197" t="s">
         <v>703</v>
       </c>
       <c r="D197" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B198" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C198" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D198" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B199" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C199" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D199" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B200" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C200" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D200" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B201" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C201" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D201" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B202" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C202" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D202" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B203" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C203" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D203" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B204" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C204" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D204" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B205" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C205" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D205" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B206" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C206" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D206" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B207" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C207" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D207" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B208" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C208" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D208" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B209" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C209" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D209" t="s">
         <v>751</v>
@@ -6159,505 +6171,519 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B210" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C210" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D210" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B211" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C211" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D211" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B212" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C212" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D212" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B213" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C213" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D213" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B214" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C214" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D214" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B215" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C215" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D215" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B216" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C216" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D216" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B217" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C217" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D217" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B218" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C218" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D218" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B219" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C219" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D219" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B220" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C220" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D220" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B221" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C221" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D221" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B222" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C222" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D222" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B223" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C223" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D223" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B224" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C224" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D224" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B225" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C225" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D225" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B226" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C226" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D226" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B227" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C227" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D227" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B228" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C228" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D228" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B229" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C229" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D229" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B230" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C230" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D230" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B231" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C231" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D231" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B232" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C232" t="s">
         <v>840</v>
       </c>
       <c r="D232" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B233" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C233" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D233" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B234" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C234" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D234" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B235" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C235" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D235" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B236" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C236" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D236" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B237" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C237" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D237" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B238" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C238" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D238" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B239" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C239" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D239" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B240" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C240" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D240" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B241" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C241" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D241" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B242" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C242" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D242" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B243" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C243" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D243" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B244" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C244" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D244" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
+        <v>889</v>
+      </c>
+      <c r="B245" t="s">
+        <v>890</v>
+      </c>
+      <c r="C245" t="s">
+        <v>891</v>
+      </c>
+      <c r="D245" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
         <v>893</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B246" t="s">
         <v>894</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C246" t="s">
         <v>895</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D246" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 98.1 (ZA7952)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5888FB-FB88-40DC-AAA7-5D36BDF105D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A23752-9658-426C-A74D-3D2A982C4D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="968">
   <si>
     <t>archive_id</t>
   </si>
@@ -2912,6 +2912,18 @@
   </si>
   <si>
     <t>Standard Eurobarometer 100</t>
+  </si>
+  <si>
+    <t>ZA7952</t>
+  </si>
+  <si>
+    <t>98.1</t>
+  </si>
+  <si>
+    <t>Parlemeter 2022, International communications within the EU, and Key Challenges of our Times - Autumn 2022</t>
+  </si>
+  <si>
+    <t>October-November 2022</t>
   </si>
 </sst>
 </file>
@@ -3246,10 +3258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D246"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3316,2868 +3328,2868 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>944</v>
+        <v>964</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>945</v>
+        <v>965</v>
       </c>
       <c r="C5" t="s">
-        <v>947</v>
+        <v>967</v>
       </c>
       <c r="D5" t="s">
-        <v>946</v>
+        <v>966</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C6" t="s">
-        <v>954</v>
+        <v>947</v>
       </c>
       <c r="D6" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>938</v>
+        <v>952</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>939</v>
+        <v>953</v>
       </c>
       <c r="C7" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="D7" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C8" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D8" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C9" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D9" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C10" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D10" t="s">
-        <v>906</v>
+        <v>934</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C11" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="D11" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="C12" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="D12" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C13" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D13" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="C14" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D14" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C15" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D15" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="C16" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D16" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>927</v>
+        <v>897</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>928</v>
+        <v>898</v>
       </c>
       <c r="C17" t="s">
-        <v>929</v>
+        <v>899</v>
       </c>
       <c r="D17" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>928</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>929</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>930</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>911</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
+        <v>911</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
         <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D51" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D58" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D59" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D60" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C61" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D61" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C62" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D62" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C63" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D63" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B64" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C64" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D64" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B65" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C65" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D65" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B66" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C66" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C67" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D67" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B68" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C68" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D69" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B70" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C70" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D70" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C71" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D71" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C72" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D72" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C73" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D73" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B74" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C74" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B75" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D75" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D76" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B77" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C77" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D77" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B78" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C78" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D78" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B79" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C79" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D79" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B80" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C80" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D80" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B81" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C81" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D81" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C82" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D82" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D83" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B84" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C84" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D84" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B85" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D85" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B86" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C86" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D86" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B87" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C87" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D87" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B88" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C88" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D88" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B89" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C89" t="s">
         <v>276</v>
       </c>
       <c r="D89" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B90" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C90" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D90" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B91" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C91" t="s">
         <v>283</v>
       </c>
       <c r="D91" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B92" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C92" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D92" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B93" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C93" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D93" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B94" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C94" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D94" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B95" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C95" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D95" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B96" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C96" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D96" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B97" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C97" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D97" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B98" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C98" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D98" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B99" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C99" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D99" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B100" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C100" t="s">
         <v>318</v>
       </c>
       <c r="D100" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B101" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C101" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D101" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B102" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C102" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D102" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B103" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C103" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D103" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B104" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C104" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D104" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B105" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C105" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D105" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B106" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C106" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D106" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B107" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C107" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D107" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B108" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C108" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D108" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B109" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C109" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D109" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B110" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C110" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D110" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B111" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C111" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D111" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B112" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C112" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D112" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B113" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C113" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D113" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B114" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C114" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D114" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B115" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C115" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D115" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B116" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C116" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D116" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B117" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C117" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D117" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B118" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C118" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D118" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B119" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C119" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D119" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B120" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C120" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D120" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B121" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C121" t="s">
-        <v>931</v>
+        <v>401</v>
       </c>
       <c r="D121" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B122" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C122" t="s">
-        <v>408</v>
+        <v>931</v>
       </c>
       <c r="D122" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B123" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C123" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D123" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B124" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C124" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D124" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B125" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C125" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D125" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B126" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C126" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D126" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B127" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C127" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D127" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B128" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C128" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D128" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B129" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C129" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D129" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B130" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C130" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D130" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B131" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C131" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D131" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B132" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C132" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D132" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B133" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C133" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D133" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B134" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C134" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D134" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B135" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C135" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D135" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B136" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C136" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D136" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B137" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C137" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D137" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B138" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C138" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D138" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B139" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C139" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D139" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B140" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C140" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D140" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B141" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C141" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D141" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B142" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C142" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D142" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B143" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C143" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D143" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B144" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C144" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D144" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B145" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C145" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D145" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B146" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C146" t="s">
         <v>500</v>
       </c>
       <c r="D146" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B147" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C147" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D147" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B148" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C148" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D148" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B149" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C149" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D149" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B150" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C150" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D150" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B151" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C151" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D151" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B152" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C152" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D152" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B153" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D153" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B154" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C154" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D154" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B155" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C155" t="s">
         <v>535</v>
       </c>
       <c r="D155" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B156" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C156" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D156" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B157" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C157" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D157" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B158" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C158" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D158" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B159" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C159" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D159" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B160" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C160" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D160" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B161" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C161" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D161" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B162" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C162" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D162" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B163" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C163" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D163" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B164" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C164" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D164" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B165" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C165" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D165" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B166" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C166" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D166" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B167" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C167" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D167" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B168" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C168" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D168" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B169" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C169" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D169" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B170" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C170" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D170" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B171" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C171" t="s">
         <v>598</v>
       </c>
       <c r="D171" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B172" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C172" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D172" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B173" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C173" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D173" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B174" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C174" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D174" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B175" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C175" t="s">
         <v>613</v>
       </c>
       <c r="D175" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B176" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C176" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="D176" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B177" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C177" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D177" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B178" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C178" t="s">
         <v>624</v>
       </c>
       <c r="D178" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B179" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C179" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D179" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B180" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C180" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D180" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B181" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C181" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D181" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B182" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C182" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D182" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B183" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C183" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D183" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B184" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C184" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D184" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B185" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C185" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D185" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B186" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C186" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D186" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B187" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C187" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D187" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B188" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C188" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D188" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B189" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C189" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D189" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B190" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C190" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D190" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B191" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C191" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D191" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B192" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C192" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D192" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B193" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C193" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D193" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B194" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C194" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D194" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B195" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C195" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D195" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B196" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C196" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D196" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B197" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C197" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D197" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B198" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C198" t="s">
         <v>703</v>
       </c>
       <c r="D198" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B199" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C199" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D199" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B200" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C200" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D200" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B201" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C201" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D201" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B202" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C202" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D202" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B203" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C203" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D203" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B204" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C204" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D204" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B205" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C205" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D205" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B206" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C206" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D206" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B207" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C207" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D207" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B208" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C208" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D208" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B209" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C209" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D209" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B210" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C210" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D210" t="s">
         <v>751</v>
@@ -6185,505 +6197,519 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B211" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C211" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D211" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B212" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C212" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D212" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B213" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C213" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D213" t="s">
-        <v>599</v>
+        <v>762</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B214" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C214" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D214" t="s">
-        <v>769</v>
+        <v>599</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B215" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C215" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D215" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B216" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C216" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D216" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B217" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C217" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D217" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B218" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C218" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D218" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B219" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C219" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D219" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B220" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C220" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D220" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B221" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C221" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D221" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B222" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C222" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D222" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B223" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C223" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D223" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B224" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C224" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D224" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B225" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C225" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D225" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B226" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C226" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D226" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B227" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C227" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D227" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B228" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C228" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D228" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B229" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C229" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D229" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B230" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C230" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D230" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B231" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C231" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D231" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B232" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C232" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D232" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B233" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C233" t="s">
         <v>840</v>
       </c>
       <c r="D233" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B234" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C234" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D234" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B235" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C235" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D235" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B236" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C236" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D236" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B237" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C237" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D237" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B238" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C238" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D238" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B239" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C239" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D239" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B240" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C240" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D240" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B241" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C241" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D241" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B242" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C242" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D242" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B243" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C243" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D243" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B244" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C244" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D244" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B245" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C245" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D245" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>889</v>
+      </c>
+      <c r="B246" t="s">
+        <v>890</v>
+      </c>
+      <c r="C246" t="s">
+        <v>891</v>
+      </c>
+      <c r="D246" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
         <v>893</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>894</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C247" t="s">
         <v>895</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D247" t="s">
         <v>896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 100.1 (ZA7887)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A23752-9658-426C-A74D-3D2A982C4D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B328076-EFEA-4351-909C-38D89C1F9E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="971">
   <si>
     <t>archive_id</t>
   </si>
@@ -754,9 +754,6 @@
     <t>77.1</t>
   </si>
   <si>
-    <t>February March 2012</t>
-  </si>
-  <si>
     <t>Robotics, Civil Protection, Humanitarian Aid, Smoking Habits, and Multilingualism</t>
   </si>
   <si>
@@ -790,9 +787,6 @@
     <t>76.2</t>
   </si>
   <si>
-    <t>September November 2011</t>
-  </si>
-  <si>
     <t>Employment and Social Policy, Job Security, and Active Aging</t>
   </si>
   <si>
@@ -850,9 +844,6 @@
     <t>75.1EP</t>
   </si>
   <si>
-    <t>February March 2011</t>
-  </si>
-  <si>
     <t>Women in the European Union</t>
   </si>
   <si>
@@ -892,9 +883,6 @@
     <t>74.1</t>
   </si>
   <si>
-    <t>August September 2010</t>
-  </si>
-  <si>
     <t>Poverty and Social Exclusion, Mobile Phone Use, Economic Crisis, and International Trade</t>
   </si>
   <si>
@@ -1915,9 +1903,6 @@
     <t>44.2bis</t>
   </si>
   <si>
-    <t>January March 1996</t>
-  </si>
-  <si>
     <t>Policies and Practices in Building Europe and the European Union</t>
   </si>
   <si>
@@ -1927,9 +1912,6 @@
     <t>44.2</t>
   </si>
   <si>
-    <t>November 1995- January 1996</t>
-  </si>
-  <si>
     <t>Working Conditions in the European Union; November 1995-January 1996</t>
   </si>
   <si>
@@ -2023,9 +2005,6 @@
     <t>41.1</t>
   </si>
   <si>
-    <t>June July 1994</t>
-  </si>
-  <si>
     <t>Post-European Election</t>
   </si>
   <si>
@@ -2059,9 +2038,6 @@
     <t>39.A</t>
   </si>
   <si>
-    <t>March June 1993</t>
-  </si>
-  <si>
     <t>Health and Safety Issues</t>
   </si>
   <si>
@@ -2272,9 +2248,6 @@
     <t>31A</t>
   </si>
   <si>
-    <t>June July 1989</t>
-  </si>
-  <si>
     <t>European Elections 1989</t>
   </si>
   <si>
@@ -2924,6 +2897,42 @@
   </si>
   <si>
     <t>October-November 2022</t>
+  </si>
+  <si>
+    <t>February-March 2012</t>
+  </si>
+  <si>
+    <t>September-November 2011</t>
+  </si>
+  <si>
+    <t>February-March 2011</t>
+  </si>
+  <si>
+    <t>August-September 2010</t>
+  </si>
+  <si>
+    <t>January-March 1996</t>
+  </si>
+  <si>
+    <t>November 1995-January 1996</t>
+  </si>
+  <si>
+    <t>June-July 1994</t>
+  </si>
+  <si>
+    <t>March-June 1993</t>
+  </si>
+  <si>
+    <t>June-July 1989</t>
+  </si>
+  <si>
+    <t>ZA8778</t>
+  </si>
+  <si>
+    <t>100.1</t>
+  </si>
+  <si>
+    <t>September-October 2023</t>
   </si>
 </sst>
 </file>
@@ -3258,10 +3267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:D248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,41 +3295,38 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>960</v>
+        <v>951</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
       <c r="C2" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
       <c r="D2" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>956</v>
+      <c r="A3" s="1" t="s">
+        <v>968</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>957</v>
+        <v>969</v>
       </c>
       <c r="C3" t="s">
-        <v>958</v>
-      </c>
-      <c r="D3" t="s">
-        <v>959</v>
+        <v>970</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>947</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>949</v>
-      </c>
-      <c r="C4" t="s">
-        <v>951</v>
       </c>
       <c r="D4" t="s">
         <v>950</v>
@@ -3328,3389 +3334,3403 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>964</v>
+        <v>939</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>965</v>
+        <v>940</v>
       </c>
       <c r="C5" t="s">
-        <v>967</v>
+        <v>942</v>
       </c>
       <c r="D5" t="s">
-        <v>966</v>
+        <v>941</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>944</v>
+        <v>955</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>945</v>
+        <v>956</v>
       </c>
       <c r="C6" t="s">
-        <v>947</v>
+        <v>958</v>
       </c>
       <c r="D6" t="s">
-        <v>946</v>
+        <v>957</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>952</v>
+        <v>935</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>953</v>
+        <v>936</v>
       </c>
       <c r="C7" t="s">
-        <v>954</v>
+        <v>938</v>
       </c>
       <c r="D7" t="s">
-        <v>955</v>
+        <v>937</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>938</v>
+        <v>943</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>939</v>
+        <v>944</v>
       </c>
       <c r="C8" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="D8" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>936</v>
+        <v>929</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>937</v>
+        <v>930</v>
       </c>
       <c r="C9" t="s">
-        <v>940</v>
+        <v>933</v>
       </c>
       <c r="D9" t="s">
-        <v>941</v>
+        <v>934</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>927</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="C10" t="s">
+        <v>931</v>
+      </c>
+      <c r="D10" t="s">
         <v>932</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>933</v>
-      </c>
-      <c r="C10" t="s">
-        <v>935</v>
-      </c>
-      <c r="D10" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>923</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>924</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>925</v>
       </c>
       <c r="C11" t="s">
         <v>926</v>
       </c>
       <c r="D11" t="s">
-        <v>906</v>
+        <v>925</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
       <c r="C12" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
       <c r="D12" t="s">
-        <v>923</v>
+        <v>897</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="C13" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="D13" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>916</v>
+        <v>899</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>917</v>
+        <v>900</v>
       </c>
       <c r="C14" t="s">
-        <v>918</v>
+        <v>901</v>
       </c>
       <c r="D14" t="s">
-        <v>919</v>
+        <v>897</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>900</v>
+        <v>907</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>901</v>
+        <v>908</v>
       </c>
       <c r="C15" t="s">
-        <v>902</v>
+        <v>909</v>
       </c>
       <c r="D15" t="s">
-        <v>903</v>
+        <v>910</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>904</v>
+        <v>891</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>905</v>
+        <v>892</v>
       </c>
       <c r="C16" t="s">
-        <v>907</v>
+        <v>893</v>
       </c>
       <c r="D16" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>895</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="C17" t="s">
+        <v>898</v>
+      </c>
+      <c r="D17" t="s">
         <v>897</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="C17" t="s">
-        <v>899</v>
-      </c>
-      <c r="D17" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>927</v>
+        <v>888</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>928</v>
+        <v>889</v>
       </c>
       <c r="C18" t="s">
-        <v>929</v>
+        <v>890</v>
       </c>
       <c r="D18" t="s">
-        <v>930</v>
+        <v>906</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
+        <v>918</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>919</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>920</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>921</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>911</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>913</v>
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>914</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
+        <v>902</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>904</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>905</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D42" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D46" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
         <v>121</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B54" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D54" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D55" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D56" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B57" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D60" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B61" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B62" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C62" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D62" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C63" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D63" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B64" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D64" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C65" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D65" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B66" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C66" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D66" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B67" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C67" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D67" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C68" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D68" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C69" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D69" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B70" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C70" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D70" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B71" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C71" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D71" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D72" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C73" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D73" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C74" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D74" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C75" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D75" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B77" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C77" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D77" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B79" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C79" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D79" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B80" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C80" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D80" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B81" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C81" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D81" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B82" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C82" t="s">
-        <v>248</v>
+        <v>959</v>
       </c>
       <c r="D82" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C83" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D83" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C84" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D84" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B85" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C85" t="s">
-        <v>260</v>
+        <v>960</v>
       </c>
       <c r="D85" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B86" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C86" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D86" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B87" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C87" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D87" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B88" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C88" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D88" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B89" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C89" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D89" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B90" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C90" t="s">
-        <v>276</v>
+        <v>961</v>
       </c>
       <c r="D90" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B91" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C91" t="s">
-        <v>283</v>
+        <v>961</v>
       </c>
       <c r="D91" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B92" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C92" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D92" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B93" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C93" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D93" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B94" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C94" t="s">
-        <v>294</v>
+        <v>962</v>
       </c>
       <c r="D94" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B95" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C95" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D95" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B96" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C96" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D96" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B97" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C97" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D97" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B98" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C98" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D98" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B99" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C99" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D99" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B100" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C100" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D100" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B101" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C101" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D101" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B102" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C102" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D102" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B103" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C103" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D103" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B104" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C104" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D104" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B105" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C105" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D105" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B106" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C106" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D106" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B107" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C107" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D107" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B108" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C108" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D108" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B109" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C109" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D109" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B110" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C110" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D110" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B111" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C111" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D111" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B112" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C112" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D112" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B113" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C113" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D113" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B114" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C114" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D114" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B115" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C115" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D115" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B116" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C116" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D116" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B117" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C117" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D117" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B118" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C118" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D118" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B119" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C119" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D119" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B120" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C120" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D120" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B121" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C121" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D121" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B122" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C122" t="s">
-        <v>931</v>
+        <v>397</v>
       </c>
       <c r="D122" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B123" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C123" t="s">
-        <v>408</v>
+        <v>922</v>
       </c>
       <c r="D123" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B124" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C124" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="D124" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B125" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C125" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="D125" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B126" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C126" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="D126" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B127" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C127" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="D127" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B128" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C128" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="D128" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B129" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C129" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="D129" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B130" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C130" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="D130" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B131" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C131" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="D131" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B132" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C132" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D132" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B133" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C133" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D133" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B134" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C134" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="D134" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B135" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C135" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D135" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B136" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C136" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D136" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B137" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="C137" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="D137" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B138" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="C138" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="D138" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B139" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C139" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D139" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B140" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C140" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="D140" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B141" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C141" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D141" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B142" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C142" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D142" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B143" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C143" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D143" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B144" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C144" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D144" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B145" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C145" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D145" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B146" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C146" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D146" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B147" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="C147" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D147" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B148" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C148" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="D148" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B149" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C149" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="D149" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B150" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C150" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="D150" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B151" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C151" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="D151" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B152" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C152" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D152" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B153" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C153" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="D153" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="B154" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C154" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="D154" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B155" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C155" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="D155" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="B156" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C156" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D156" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B157" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C157" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="D157" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="B158" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="C158" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="D158" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="B159" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C159" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="D159" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="B160" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="C160" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="D160" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="B161" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="C161" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="D161" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B162" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="C162" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D162" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B163" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C163" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D163" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B164" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C164" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="D164" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="B165" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="C165" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="D165" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B166" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C166" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D166" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B167" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="C167" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="D167" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B168" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="C168" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="D168" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B169" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C169" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D169" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B170" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="C170" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D170" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B171" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C171" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="D171" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="B172" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C172" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D172" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="B173" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="C173" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="D173" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="B174" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="C174" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="D174" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="B175" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="C175" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="D175" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="B176" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="C176" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D176" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="B177" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="C177" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="D177" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="B178" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="C178" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="D178" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="B179" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="C179" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D179" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="B180" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="C180" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="D180" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="B181" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="C181" t="s">
-        <v>635</v>
+        <v>963</v>
       </c>
       <c r="D181" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="B182" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="C182" t="s">
-        <v>639</v>
+        <v>964</v>
       </c>
       <c r="D182" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="B183" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="C183" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="D183" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="B184" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="C184" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="D184" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="B185" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="C185" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="D185" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B186" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="C186" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="D186" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="B187" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="C187" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="D187" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="B188" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="C188" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="D188" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="B189" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="C189" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="D189" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="B190" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="C190" t="s">
-        <v>671</v>
+        <v>965</v>
       </c>
       <c r="D190" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>673</v>
+        <v>662</v>
       </c>
       <c r="B191" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="C191" t="s">
-        <v>675</v>
+        <v>664</v>
       </c>
       <c r="D191" t="s">
-        <v>676</v>
+        <v>665</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>677</v>
+        <v>666</v>
       </c>
       <c r="B192" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
       <c r="C192" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
       <c r="D192" t="s">
-        <v>680</v>
+        <v>669</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>681</v>
+        <v>670</v>
       </c>
       <c r="B193" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
       <c r="C193" t="s">
-        <v>683</v>
+        <v>966</v>
       </c>
       <c r="D193" t="s">
-        <v>684</v>
+        <v>672</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>685</v>
+        <v>673</v>
       </c>
       <c r="B194" t="s">
-        <v>686</v>
+        <v>674</v>
       </c>
       <c r="C194" t="s">
-        <v>687</v>
+        <v>675</v>
       </c>
       <c r="D194" t="s">
-        <v>688</v>
+        <v>676</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>689</v>
+        <v>677</v>
       </c>
       <c r="B195" t="s">
-        <v>690</v>
+        <v>678</v>
       </c>
       <c r="C195" t="s">
-        <v>691</v>
+        <v>679</v>
       </c>
       <c r="D195" t="s">
-        <v>692</v>
+        <v>680</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>693</v>
+        <v>681</v>
       </c>
       <c r="B196" t="s">
-        <v>694</v>
+        <v>682</v>
       </c>
       <c r="C196" t="s">
-        <v>695</v>
+        <v>683</v>
       </c>
       <c r="D196" t="s">
-        <v>696</v>
+        <v>684</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>697</v>
+        <v>685</v>
       </c>
       <c r="B197" t="s">
-        <v>698</v>
+        <v>686</v>
       </c>
       <c r="C197" t="s">
-        <v>699</v>
+        <v>687</v>
       </c>
       <c r="D197" t="s">
-        <v>700</v>
+        <v>688</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>701</v>
+        <v>689</v>
       </c>
       <c r="B198" t="s">
-        <v>702</v>
+        <v>690</v>
       </c>
       <c r="C198" t="s">
-        <v>703</v>
+        <v>691</v>
       </c>
       <c r="D198" t="s">
-        <v>704</v>
+        <v>692</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>705</v>
+        <v>693</v>
       </c>
       <c r="B199" t="s">
-        <v>706</v>
+        <v>694</v>
       </c>
       <c r="C199" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="D199" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
       <c r="B200" t="s">
-        <v>709</v>
+        <v>698</v>
       </c>
       <c r="C200" t="s">
-        <v>710</v>
+        <v>695</v>
       </c>
       <c r="D200" t="s">
-        <v>711</v>
+        <v>699</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>712</v>
+        <v>700</v>
       </c>
       <c r="B201" t="s">
-        <v>713</v>
+        <v>701</v>
       </c>
       <c r="C201" t="s">
-        <v>714</v>
+        <v>702</v>
       </c>
       <c r="D201" t="s">
-        <v>715</v>
+        <v>703</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>716</v>
+        <v>704</v>
       </c>
       <c r="B202" t="s">
-        <v>717</v>
+        <v>705</v>
       </c>
       <c r="C202" t="s">
-        <v>718</v>
+        <v>706</v>
       </c>
       <c r="D202" t="s">
-        <v>719</v>
+        <v>707</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="B203" t="s">
-        <v>721</v>
+        <v>709</v>
       </c>
       <c r="C203" t="s">
-        <v>722</v>
+        <v>710</v>
       </c>
       <c r="D203" t="s">
-        <v>723</v>
+        <v>711</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>724</v>
+        <v>712</v>
       </c>
       <c r="B204" t="s">
-        <v>725</v>
+        <v>713</v>
       </c>
       <c r="C204" t="s">
-        <v>726</v>
+        <v>714</v>
       </c>
       <c r="D204" t="s">
-        <v>727</v>
+        <v>715</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
       <c r="B205" t="s">
-        <v>729</v>
+        <v>717</v>
       </c>
       <c r="C205" t="s">
-        <v>730</v>
+        <v>718</v>
       </c>
       <c r="D205" t="s">
-        <v>731</v>
+        <v>719</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
       <c r="B206" t="s">
-        <v>733</v>
+        <v>721</v>
       </c>
       <c r="C206" t="s">
-        <v>734</v>
+        <v>722</v>
       </c>
       <c r="D206" t="s">
-        <v>735</v>
+        <v>723</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>736</v>
+        <v>724</v>
       </c>
       <c r="B207" t="s">
-        <v>737</v>
+        <v>725</v>
       </c>
       <c r="C207" t="s">
-        <v>738</v>
+        <v>726</v>
       </c>
       <c r="D207" t="s">
-        <v>739</v>
+        <v>727</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>740</v>
+        <v>728</v>
       </c>
       <c r="B208" t="s">
-        <v>741</v>
+        <v>729</v>
       </c>
       <c r="C208" t="s">
-        <v>742</v>
+        <v>730</v>
       </c>
       <c r="D208" t="s">
-        <v>743</v>
+        <v>731</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>744</v>
+        <v>732</v>
       </c>
       <c r="B209" t="s">
-        <v>745</v>
+        <v>733</v>
       </c>
       <c r="C209" t="s">
-        <v>746</v>
+        <v>734</v>
       </c>
       <c r="D209" t="s">
-        <v>747</v>
+        <v>735</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>748</v>
+        <v>736</v>
       </c>
       <c r="B210" t="s">
-        <v>749</v>
+        <v>737</v>
       </c>
       <c r="C210" t="s">
-        <v>750</v>
+        <v>738</v>
       </c>
       <c r="D210" t="s">
-        <v>751</v>
+        <v>739</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>752</v>
+        <v>740</v>
       </c>
       <c r="B211" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="C211" t="s">
-        <v>754</v>
+        <v>967</v>
       </c>
       <c r="D211" t="s">
-        <v>751</v>
+        <v>742</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>755</v>
+        <v>743</v>
       </c>
       <c r="B212" t="s">
-        <v>756</v>
+        <v>744</v>
       </c>
       <c r="C212" t="s">
-        <v>757</v>
+        <v>745</v>
       </c>
       <c r="D212" t="s">
-        <v>758</v>
+        <v>742</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>759</v>
+        <v>746</v>
       </c>
       <c r="B213" t="s">
-        <v>760</v>
+        <v>747</v>
       </c>
       <c r="C213" t="s">
-        <v>761</v>
+        <v>748</v>
       </c>
       <c r="D213" t="s">
-        <v>762</v>
+        <v>749</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>763</v>
+        <v>750</v>
       </c>
       <c r="B214" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
       <c r="C214" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="D214" t="s">
-        <v>599</v>
+        <v>753</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>766</v>
+        <v>754</v>
       </c>
       <c r="B215" t="s">
-        <v>767</v>
+        <v>755</v>
       </c>
       <c r="C215" t="s">
-        <v>768</v>
+        <v>756</v>
       </c>
       <c r="D215" t="s">
-        <v>769</v>
+        <v>595</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="B216" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="C216" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="D216" t="s">
-        <v>773</v>
+        <v>760</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>774</v>
+        <v>761</v>
       </c>
       <c r="B217" t="s">
-        <v>775</v>
+        <v>762</v>
       </c>
       <c r="C217" t="s">
-        <v>776</v>
+        <v>763</v>
       </c>
       <c r="D217" t="s">
-        <v>777</v>
+        <v>764</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>778</v>
+        <v>765</v>
       </c>
       <c r="B218" t="s">
-        <v>779</v>
+        <v>766</v>
       </c>
       <c r="C218" t="s">
-        <v>780</v>
+        <v>767</v>
       </c>
       <c r="D218" t="s">
-        <v>781</v>
+        <v>768</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>782</v>
+        <v>769</v>
       </c>
       <c r="B219" t="s">
-        <v>783</v>
+        <v>770</v>
       </c>
       <c r="C219" t="s">
-        <v>784</v>
+        <v>771</v>
       </c>
       <c r="D219" t="s">
-        <v>785</v>
+        <v>772</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="B220" t="s">
-        <v>787</v>
+        <v>774</v>
       </c>
       <c r="C220" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
       <c r="D220" t="s">
-        <v>789</v>
+        <v>776</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>790</v>
+        <v>777</v>
       </c>
       <c r="B221" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="C221" t="s">
-        <v>792</v>
+        <v>779</v>
       </c>
       <c r="D221" t="s">
-        <v>793</v>
+        <v>780</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>794</v>
+        <v>781</v>
       </c>
       <c r="B222" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="C222" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="D222" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="B223" t="s">
-        <v>799</v>
+        <v>786</v>
       </c>
       <c r="C223" t="s">
-        <v>800</v>
+        <v>787</v>
       </c>
       <c r="D223" t="s">
-        <v>801</v>
+        <v>788</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>802</v>
+        <v>789</v>
       </c>
       <c r="B224" t="s">
-        <v>803</v>
+        <v>790</v>
       </c>
       <c r="C224" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
       <c r="D224" t="s">
-        <v>805</v>
+        <v>792</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>806</v>
+        <v>793</v>
       </c>
       <c r="B225" t="s">
-        <v>807</v>
+        <v>794</v>
       </c>
       <c r="C225" t="s">
-        <v>808</v>
+        <v>795</v>
       </c>
       <c r="D225" t="s">
-        <v>809</v>
+        <v>796</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>810</v>
+        <v>797</v>
       </c>
       <c r="B226" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="C226" t="s">
-        <v>812</v>
+        <v>799</v>
       </c>
       <c r="D226" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="B227" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="C227" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="D227" t="s">
-        <v>817</v>
+        <v>804</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>818</v>
+        <v>805</v>
       </c>
       <c r="B228" t="s">
-        <v>819</v>
+        <v>806</v>
       </c>
       <c r="C228" t="s">
-        <v>820</v>
+        <v>807</v>
       </c>
       <c r="D228" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>822</v>
+        <v>809</v>
       </c>
       <c r="B229" t="s">
-        <v>823</v>
+        <v>810</v>
       </c>
       <c r="C229" t="s">
-        <v>824</v>
+        <v>811</v>
       </c>
       <c r="D229" t="s">
-        <v>825</v>
+        <v>812</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>826</v>
+        <v>813</v>
       </c>
       <c r="B230" t="s">
-        <v>827</v>
+        <v>814</v>
       </c>
       <c r="C230" t="s">
-        <v>828</v>
+        <v>815</v>
       </c>
       <c r="D230" t="s">
-        <v>829</v>
+        <v>816</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>830</v>
+        <v>817</v>
       </c>
       <c r="B231" t="s">
-        <v>831</v>
+        <v>818</v>
       </c>
       <c r="C231" t="s">
-        <v>832</v>
+        <v>819</v>
       </c>
       <c r="D231" t="s">
-        <v>833</v>
+        <v>820</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="B232" t="s">
-        <v>835</v>
+        <v>822</v>
       </c>
       <c r="C232" t="s">
-        <v>836</v>
+        <v>823</v>
       </c>
       <c r="D232" t="s">
-        <v>837</v>
+        <v>824</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="B233" t="s">
-        <v>839</v>
+        <v>826</v>
       </c>
       <c r="C233" t="s">
-        <v>840</v>
+        <v>827</v>
       </c>
       <c r="D233" t="s">
-        <v>841</v>
+        <v>828</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>842</v>
+        <v>829</v>
       </c>
       <c r="B234" t="s">
-        <v>843</v>
+        <v>830</v>
       </c>
       <c r="C234" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="D234" t="s">
-        <v>844</v>
+        <v>832</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>845</v>
+        <v>833</v>
       </c>
       <c r="B235" t="s">
-        <v>846</v>
+        <v>834</v>
       </c>
       <c r="C235" t="s">
-        <v>847</v>
+        <v>831</v>
       </c>
       <c r="D235" t="s">
-        <v>848</v>
+        <v>835</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>849</v>
+        <v>836</v>
       </c>
       <c r="B236" t="s">
-        <v>850</v>
+        <v>837</v>
       </c>
       <c r="C236" t="s">
-        <v>851</v>
+        <v>838</v>
       </c>
       <c r="D236" t="s">
-        <v>852</v>
+        <v>839</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>853</v>
+        <v>840</v>
       </c>
       <c r="B237" t="s">
-        <v>854</v>
+        <v>841</v>
       </c>
       <c r="C237" t="s">
-        <v>855</v>
+        <v>842</v>
       </c>
       <c r="D237" t="s">
-        <v>856</v>
+        <v>843</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>857</v>
+        <v>844</v>
       </c>
       <c r="B238" t="s">
-        <v>858</v>
+        <v>845</v>
       </c>
       <c r="C238" t="s">
-        <v>859</v>
+        <v>846</v>
       </c>
       <c r="D238" t="s">
-        <v>860</v>
+        <v>847</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>861</v>
+        <v>848</v>
       </c>
       <c r="B239" t="s">
-        <v>862</v>
+        <v>849</v>
       </c>
       <c r="C239" t="s">
-        <v>863</v>
+        <v>850</v>
       </c>
       <c r="D239" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
       <c r="B240" t="s">
-        <v>866</v>
+        <v>853</v>
       </c>
       <c r="C240" t="s">
-        <v>867</v>
+        <v>854</v>
       </c>
       <c r="D240" t="s">
-        <v>868</v>
+        <v>855</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>869</v>
+        <v>856</v>
       </c>
       <c r="B241" t="s">
-        <v>870</v>
+        <v>857</v>
       </c>
       <c r="C241" t="s">
-        <v>871</v>
+        <v>858</v>
       </c>
       <c r="D241" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="B242" t="s">
-        <v>874</v>
+        <v>861</v>
       </c>
       <c r="C242" t="s">
-        <v>875</v>
+        <v>862</v>
       </c>
       <c r="D242" t="s">
-        <v>876</v>
+        <v>863</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>877</v>
+        <v>864</v>
       </c>
       <c r="B243" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="C243" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="D243" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="B244" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="C244" t="s">
-        <v>883</v>
+        <v>870</v>
       </c>
       <c r="D244" t="s">
-        <v>884</v>
+        <v>871</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>885</v>
+        <v>872</v>
       </c>
       <c r="B245" t="s">
-        <v>886</v>
+        <v>873</v>
       </c>
       <c r="C245" t="s">
-        <v>887</v>
+        <v>874</v>
       </c>
       <c r="D245" t="s">
-        <v>888</v>
+        <v>875</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>889</v>
+        <v>876</v>
       </c>
       <c r="B246" t="s">
-        <v>890</v>
+        <v>877</v>
       </c>
       <c r="C246" t="s">
-        <v>891</v>
+        <v>878</v>
       </c>
       <c r="D246" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>893</v>
+        <v>880</v>
       </c>
       <c r="B247" t="s">
-        <v>894</v>
+        <v>881</v>
       </c>
       <c r="C247" t="s">
-        <v>895</v>
+        <v>882</v>
       </c>
       <c r="D247" t="s">
-        <v>896</v>
+        <v>883</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>884</v>
+      </c>
+      <c r="B248" t="s">
+        <v>885</v>
+      </c>
+      <c r="C248" t="s">
+        <v>886</v>
+      </c>
+      <c r="D248" t="s">
+        <v>887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add EB 99.1 (ZA7954) and EB 101.1 (ZA8841)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B328076-EFEA-4351-909C-38D89C1F9E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C8E032-1565-42C0-8AE8-39BE429D8D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="980">
   <si>
     <t>archive_id</t>
   </si>
@@ -2933,6 +2933,33 @@
   </si>
   <si>
     <t>September-October 2023</t>
+  </si>
+  <si>
+    <t>ZA8841</t>
+  </si>
+  <si>
+    <t>101.1</t>
+  </si>
+  <si>
+    <t>February-March 2024</t>
+  </si>
+  <si>
+    <t>Social Europe, Disaster risk awareness and preparedness of the EU population, and Citizens’ attitudes towards corruption in the EU in 2024</t>
+  </si>
+  <si>
+    <t>99.1</t>
+  </si>
+  <si>
+    <t>The Digital Decade, and Attitudes of Europeans towards Animal Welfare</t>
+  </si>
+  <si>
+    <t>March 2023</t>
+  </si>
+  <si>
+    <t>ZA7954</t>
+  </si>
+  <si>
+    <t>Parlemeter 2023, Europeans and their languages, EU Civil Protection, and EU Humanitarian Aid</t>
   </si>
 </sst>
 </file>
@@ -3267,10 +3294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D248"/>
+  <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3295,178 +3322,181 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>971</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="C2" t="s">
+        <v>973</v>
+      </c>
+      <c r="D2" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>951</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>953</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>968</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>947</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>948</v>
-      </c>
-      <c r="C4" t="s">
-        <v>949</v>
-      </c>
       <c r="D4" t="s">
-        <v>950</v>
+        <v>979</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="C5" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="D5" t="s">
-        <v>941</v>
+        <v>950</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>955</v>
+        <v>978</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>956</v>
-      </c>
-      <c r="C6" t="s">
-        <v>958</v>
+        <v>975</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>977</v>
       </c>
       <c r="D6" t="s">
-        <v>957</v>
+        <v>976</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="C7" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="D7" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>944</v>
+        <v>956</v>
       </c>
       <c r="C8" t="s">
-        <v>945</v>
+        <v>958</v>
       </c>
       <c r="D8" t="s">
-        <v>946</v>
+        <v>957</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>929</v>
+        <v>935</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>930</v>
+        <v>936</v>
       </c>
       <c r="C9" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
       <c r="D9" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>927</v>
+        <v>943</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>928</v>
+        <v>944</v>
       </c>
       <c r="C10" t="s">
-        <v>931</v>
+        <v>945</v>
       </c>
       <c r="D10" t="s">
-        <v>932</v>
+        <v>946</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>924</v>
+        <v>930</v>
       </c>
       <c r="C11" t="s">
-        <v>926</v>
+        <v>933</v>
       </c>
       <c r="D11" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>915</v>
+        <v>927</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>916</v>
+        <v>928</v>
       </c>
       <c r="C12" t="s">
-        <v>917</v>
+        <v>931</v>
       </c>
       <c r="D12" t="s">
-        <v>897</v>
+        <v>932</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>911</v>
+        <v>923</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>912</v>
+        <v>924</v>
       </c>
       <c r="C13" t="s">
-        <v>913</v>
+        <v>926</v>
       </c>
       <c r="D13" t="s">
-        <v>914</v>
+        <v>925</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>899</v>
+        <v>915</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="C14" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="D14" t="s">
         <v>897</v>
@@ -3474,3262 +3504,3290 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c r="C15" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="D15" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>892</v>
+        <v>900</v>
       </c>
       <c r="C16" t="s">
-        <v>893</v>
+        <v>901</v>
       </c>
       <c r="D16" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>895</v>
+        <v>907</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>896</v>
+        <v>908</v>
       </c>
       <c r="C17" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
       <c r="D17" t="s">
-        <v>897</v>
+        <v>910</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="C18" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="D18" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>918</v>
+        <v>895</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>919</v>
+        <v>896</v>
       </c>
       <c r="C19" t="s">
-        <v>920</v>
+        <v>898</v>
       </c>
       <c r="D19" t="s">
-        <v>921</v>
+        <v>897</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
+        <v>888</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>889</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>890</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>906</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
+        <v>918</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>919</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>920</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>921</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>902</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>903</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>904</v>
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>905</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
+        <v>902</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>904</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>905</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
-      </c>
-      <c r="D49" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D51" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D55" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C57" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C58" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D59" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D61" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D63" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C65" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D65" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C66" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D66" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C67" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D67" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C68" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D68" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B69" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C69" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D69" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B70" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C70" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D70" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B71" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C71" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B72" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C72" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D72" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B73" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C73" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D73" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C74" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D74" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B75" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C75" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D75" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B76" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C76" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D76" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C77" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D77" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C78" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D78" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B79" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C79" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D79" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C80" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D80" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B81" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C81" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D81" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B82" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C82" t="s">
-        <v>959</v>
+        <v>236</v>
       </c>
       <c r="D82" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B83" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C83" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D83" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B84" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C84" t="s">
-        <v>251</v>
+        <v>959</v>
       </c>
       <c r="D84" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B85" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C85" t="s">
-        <v>960</v>
+        <v>247</v>
       </c>
       <c r="D85" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B86" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C86" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D86" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B87" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C87" t="s">
-        <v>262</v>
+        <v>960</v>
       </c>
       <c r="D87" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B88" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C88" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D88" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B89" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C89" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D89" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B90" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C90" t="s">
-        <v>961</v>
+        <v>266</v>
       </c>
       <c r="D90" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B91" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C91" t="s">
-        <v>961</v>
+        <v>270</v>
       </c>
       <c r="D91" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B92" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C92" t="s">
-        <v>280</v>
+        <v>961</v>
       </c>
       <c r="D92" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B93" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C93" t="s">
-        <v>280</v>
+        <v>961</v>
       </c>
       <c r="D93" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B94" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C94" t="s">
-        <v>962</v>
+        <v>280</v>
       </c>
       <c r="D94" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C95" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D95" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B96" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C96" t="s">
-        <v>294</v>
+        <v>962</v>
       </c>
       <c r="D96" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B97" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C97" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D97" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B98" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C98" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D98" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B99" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C99" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D99" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B100" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C100" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D100" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B101" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C101" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D101" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B102" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C102" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D102" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B103" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C103" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D103" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B104" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C104" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D104" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B105" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C105" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D105" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B106" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C106" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D106" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B107" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C107" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D107" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B108" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C108" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D108" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B109" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C109" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D109" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B110" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C110" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D110" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B111" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C111" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D111" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B112" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C112" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D112" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B113" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C113" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D113" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B114" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C114" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D114" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B115" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C115" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D115" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B116" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C116" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D116" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B117" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C117" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D117" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B118" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C118" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D118" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B119" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C119" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D119" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B120" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C120" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D120" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B121" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C121" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D121" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B122" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C122" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D122" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B123" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C123" t="s">
-        <v>922</v>
+        <v>393</v>
       </c>
       <c r="D123" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B124" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C124" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D124" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B125" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C125" t="s">
-        <v>408</v>
+        <v>922</v>
       </c>
       <c r="D125" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B126" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C126" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="D126" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B127" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C127" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="D127" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B128" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C128" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="D128" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B129" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C129" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="D129" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B130" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C130" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="D130" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B131" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C131" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="D131" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B132" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C132" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="D132" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B133" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C133" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="D133" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B134" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C134" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D134" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B135" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C135" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D135" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B136" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C136" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="D136" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B137" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C137" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D137" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B138" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C138" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D138" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B139" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="C139" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="D139" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B140" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="C140" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="D140" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B141" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C141" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D141" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B142" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C142" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="D142" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B143" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C143" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D143" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B144" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C144" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D144" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B145" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C145" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D145" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B146" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C146" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D146" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B147" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C147" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D147" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B148" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C148" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D148" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B149" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="C149" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="D149" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B150" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C150" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="D150" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B151" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C151" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="D151" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B152" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C152" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="D152" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B153" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C153" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="D153" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B154" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C154" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D154" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B155" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C155" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="D155" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="B156" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C156" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="D156" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B157" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C157" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D157" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="B158" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="C158" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="D158" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B159" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C159" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="D159" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="B160" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="C160" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="D160" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="B161" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C161" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="D161" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="B162" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="C162" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="D162" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="B163" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="C163" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="D163" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B164" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="C164" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D164" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B165" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C165" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D165" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B166" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C166" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="D166" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="B167" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="C167" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="D167" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B168" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C168" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D168" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B169" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="C169" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="D169" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B170" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="C170" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="D170" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B171" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C171" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D171" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B172" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="C172" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D172" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B173" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C173" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D173" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="B174" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="C174" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="D174" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="B175" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="C175" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="D175" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="B176" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="C176" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="D176" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="B177" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="C177" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D177" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="B178" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="C178" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="D178" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="B179" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="C179" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="D179" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="B180" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="C180" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D180" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="B181" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="C181" t="s">
-        <v>963</v>
+        <v>620</v>
       </c>
       <c r="D181" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B182" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="C182" t="s">
-        <v>964</v>
+        <v>620</v>
       </c>
       <c r="D182" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="B183" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="C183" t="s">
-        <v>633</v>
+        <v>963</v>
       </c>
       <c r="D183" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="B184" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="C184" t="s">
-        <v>637</v>
+        <v>964</v>
       </c>
       <c r="D184" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="B185" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="C185" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="D185" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="B186" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="C186" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="D186" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="B187" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="C187" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="D187" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="B188" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="C188" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="D188" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="B189" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="C189" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="D189" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="B190" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="C190" t="s">
-        <v>965</v>
+        <v>653</v>
       </c>
       <c r="D190" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="B191" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="C191" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="D191" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="B192" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="C192" t="s">
-        <v>668</v>
+        <v>965</v>
       </c>
       <c r="D192" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B193" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="C193" t="s">
-        <v>966</v>
+        <v>664</v>
       </c>
       <c r="D193" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="B194" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="C194" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="D194" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="B195" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="C195" t="s">
-        <v>679</v>
+        <v>966</v>
       </c>
       <c r="D195" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="B196" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="C196" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D196" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="B197" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="C197" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="D197" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B198" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="C198" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="D198" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="B199" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="C199" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="D199" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="B200" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C200" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D200" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="B201" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="C201" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="D201" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="B202" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="C202" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="D202" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="B203" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="C203" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="D203" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="B204" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="C204" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="D204" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="B205" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="C205" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="D205" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="B206" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="C206" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="D206" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="B207" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="C207" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="D207" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="B208" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="C208" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="D208" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="B209" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="C209" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="D209" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="B210" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="C210" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="D210" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="B211" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="C211" t="s">
-        <v>967</v>
+        <v>734</v>
       </c>
       <c r="D211" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="B212" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
       <c r="C212" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="D212" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="B213" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="C213" t="s">
-        <v>748</v>
+        <v>967</v>
       </c>
       <c r="D213" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
       <c r="B214" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
       <c r="C214" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="D214" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="B215" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="C215" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="D215" t="s">
-        <v>595</v>
+        <v>749</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="B216" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="C216" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="D216" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="B217" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="C217" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="D217" t="s">
-        <v>764</v>
+        <v>595</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="B218" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="C218" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="D218" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="B219" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="C219" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="D219" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="B220" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="C220" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="D220" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B221" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="C221" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="D221" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B222" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="C222" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="D222" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="B223" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="C223" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="D223" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B224" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="C224" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="D224" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B225" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="C225" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="D225" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="B226" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="C226" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="D226" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="B227" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="C227" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="D227" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="B228" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="C228" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="D228" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="B229" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="C229" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="D229" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="B230" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="C230" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="D230" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="B231" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="C231" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="D231" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="B232" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="C232" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="D232" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="B233" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="C233" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="D233" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="B234" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="C234" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D234" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="B235" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="C235" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="D235" t="s">
-        <v>835</v>
+        <v>828</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
       <c r="B236" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="C236" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="D236" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="B237" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="C237" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
       <c r="D237" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="B238" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="C238" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="D238" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="B239" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="C239" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="D239" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="B240" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="C240" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="D240" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="B241" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="C241" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="D241" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="B242" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="C242" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="D242" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="B243" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="C243" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="D243" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="B244" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="C244" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="D244" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="B245" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="C245" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="D245" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="B246" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="C246" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="D246" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="B247" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="C247" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="D247" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
+        <v>876</v>
+      </c>
+      <c r="B248" t="s">
+        <v>877</v>
+      </c>
+      <c r="C248" t="s">
+        <v>878</v>
+      </c>
+      <c r="D248" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>880</v>
+      </c>
+      <c r="B249" t="s">
+        <v>881</v>
+      </c>
+      <c r="C249" t="s">
+        <v>882</v>
+      </c>
+      <c r="D249" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
         <v>884</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B250" t="s">
         <v>885</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C250" t="s">
         <v>886</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D250" t="s">
         <v>887</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 101.3 (ZA8843) and EB 101.4 (ZA8844)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C8E032-1565-42C0-8AE8-39BE429D8D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52615E27-C10F-42AF-857C-1213A0C00555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="987">
   <si>
     <t>archive_id</t>
   </si>
@@ -2960,6 +2960,27 @@
   </si>
   <si>
     <t>Parlemeter 2023, Europeans and their languages, EU Civil Protection, and EU Humanitarian Aid</t>
+  </si>
+  <si>
+    <t>ZA8843</t>
+  </si>
+  <si>
+    <t>ZA8844</t>
+  </si>
+  <si>
+    <t>101.3</t>
+  </si>
+  <si>
+    <t>101.4</t>
+  </si>
+  <si>
+    <t>April-May 2024</t>
+  </si>
+  <si>
+    <t>Rule of law, Artificial Intelligence and the future of work, and European attitudes towards EU energy policy</t>
+  </si>
+  <si>
+    <t>Standard Eurobarometer 101</t>
   </si>
 </sst>
 </file>
@@ -3294,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D250"/>
+  <dimension ref="A1:D252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3322,209 +3343,209 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>971</v>
+        <v>981</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>972</v>
+        <v>983</v>
       </c>
       <c r="C2" t="s">
-        <v>973</v>
+        <v>984</v>
       </c>
       <c r="D2" t="s">
-        <v>974</v>
+        <v>985</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>951</v>
+        <v>980</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>952</v>
+        <v>982</v>
       </c>
       <c r="C3" t="s">
-        <v>953</v>
+        <v>984</v>
       </c>
       <c r="D3" t="s">
-        <v>954</v>
+        <v>986</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>968</v>
+      <c r="A4" t="s">
+        <v>971</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="C4" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="D4" t="s">
-        <v>979</v>
+        <v>974</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="C5" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c r="D5" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>978</v>
+      <c r="A6" s="1" t="s">
+        <v>968</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>975</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>977</v>
+        <v>969</v>
+      </c>
+      <c r="C6" t="s">
+        <v>970</v>
       </c>
       <c r="D6" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="C7" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="D7" t="s">
-        <v>941</v>
+        <v>950</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>955</v>
+        <v>978</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>956</v>
-      </c>
-      <c r="C8" t="s">
-        <v>958</v>
+        <v>975</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>977</v>
       </c>
       <c r="D8" t="s">
-        <v>957</v>
+        <v>976</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="C9" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="D9" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>944</v>
+        <v>956</v>
       </c>
       <c r="C10" t="s">
-        <v>945</v>
+        <v>958</v>
       </c>
       <c r="D10" t="s">
-        <v>946</v>
+        <v>957</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>929</v>
+        <v>935</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>930</v>
+        <v>936</v>
       </c>
       <c r="C11" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
       <c r="D11" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>927</v>
+        <v>943</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>928</v>
+        <v>944</v>
       </c>
       <c r="C12" t="s">
-        <v>931</v>
+        <v>945</v>
       </c>
       <c r="D12" t="s">
-        <v>932</v>
+        <v>946</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>924</v>
+        <v>930</v>
       </c>
       <c r="C13" t="s">
-        <v>926</v>
+        <v>933</v>
       </c>
       <c r="D13" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>915</v>
+        <v>927</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>916</v>
+        <v>928</v>
       </c>
       <c r="C14" t="s">
-        <v>917</v>
+        <v>931</v>
       </c>
       <c r="D14" t="s">
-        <v>897</v>
+        <v>932</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>911</v>
+        <v>923</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>912</v>
+        <v>924</v>
       </c>
       <c r="C15" t="s">
-        <v>913</v>
+        <v>926</v>
       </c>
       <c r="D15" t="s">
-        <v>914</v>
+        <v>925</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>899</v>
+        <v>915</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="C16" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="D16" t="s">
         <v>897</v>
@@ -3532,3262 +3553,3290 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c r="C17" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="D17" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>892</v>
+        <v>900</v>
       </c>
       <c r="C18" t="s">
-        <v>893</v>
+        <v>901</v>
       </c>
       <c r="D18" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>895</v>
+        <v>907</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>896</v>
+        <v>908</v>
       </c>
       <c r="C19" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
       <c r="D19" t="s">
-        <v>897</v>
+        <v>910</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="C20" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="D20" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>918</v>
+        <v>895</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>919</v>
+        <v>896</v>
       </c>
       <c r="C21" t="s">
-        <v>920</v>
+        <v>898</v>
       </c>
       <c r="D21" t="s">
-        <v>921</v>
+        <v>897</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
+        <v>888</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>889</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>890</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>906</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
+        <v>918</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>919</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>920</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>921</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>902</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>903</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>904</v>
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>905</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s">
-        <v>26</v>
+        <v>902</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>904</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>905</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="D49" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
-      </c>
-      <c r="D51" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D52" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D53" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D54" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C56" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D56" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C59" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D59" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C60" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D61" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C62" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D64" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C65" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B66" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C66" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D66" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D67" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C68" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D68" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B69" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C69" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C70" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D70" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B71" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C71" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D71" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B72" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C72" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D72" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B73" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C73" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D73" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B74" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C74" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D74" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B75" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C75" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C76" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D76" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B77" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C77" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D77" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C78" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D78" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B79" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C79" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D79" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C80" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D80" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B81" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C81" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D81" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B82" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C82" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D82" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B83" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C83" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D83" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B84" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C84" t="s">
-        <v>959</v>
+        <v>236</v>
       </c>
       <c r="D84" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B85" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C85" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D85" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B86" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C86" t="s">
-        <v>251</v>
+        <v>959</v>
       </c>
       <c r="D86" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C87" t="s">
-        <v>960</v>
+        <v>247</v>
       </c>
       <c r="D87" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B88" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C88" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D88" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B89" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C89" t="s">
-        <v>262</v>
+        <v>960</v>
       </c>
       <c r="D89" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B90" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C90" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D90" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B91" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C91" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D91" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B92" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C92" t="s">
-        <v>961</v>
+        <v>266</v>
       </c>
       <c r="D92" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B93" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C93" t="s">
-        <v>961</v>
+        <v>270</v>
       </c>
       <c r="D93" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B94" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C94" t="s">
-        <v>280</v>
+        <v>961</v>
       </c>
       <c r="D94" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B95" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C95" t="s">
-        <v>280</v>
+        <v>961</v>
       </c>
       <c r="D95" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B96" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C96" t="s">
-        <v>962</v>
+        <v>280</v>
       </c>
       <c r="D96" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B97" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C97" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D97" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B98" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C98" t="s">
-        <v>294</v>
+        <v>962</v>
       </c>
       <c r="D98" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B99" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C99" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D99" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B100" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C100" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D100" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B101" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C101" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D101" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B102" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C102" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D102" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B103" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C103" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D103" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B104" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C104" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D104" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B105" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C105" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D105" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C106" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D106" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B107" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C107" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D107" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B108" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C108" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D108" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B109" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C109" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D109" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B110" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C110" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D110" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B111" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C111" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D111" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B112" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C112" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D112" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B113" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C113" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D113" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B114" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C114" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D114" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B115" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C115" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D115" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B116" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C116" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D116" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B117" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C117" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D117" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B118" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C118" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D118" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B119" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C119" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D119" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B120" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C120" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D120" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B121" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C121" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D121" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B122" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C122" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D122" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B123" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C123" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D123" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B124" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C124" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D124" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B125" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C125" t="s">
-        <v>922</v>
+        <v>393</v>
       </c>
       <c r="D125" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B126" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C126" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D126" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B127" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C127" t="s">
-        <v>408</v>
+        <v>922</v>
       </c>
       <c r="D127" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B128" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C128" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="D128" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B129" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C129" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="D129" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B130" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C130" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="D130" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B131" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C131" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="D131" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B132" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C132" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="D132" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B133" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C133" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="D133" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B134" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C134" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="D134" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B135" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C135" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="D135" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B136" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C136" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D136" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B137" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C137" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D137" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B138" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C138" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="D138" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B139" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C139" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D139" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B140" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C140" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D140" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B141" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="C141" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="D141" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B142" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="C142" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="D142" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B143" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C143" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D143" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B144" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C144" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="D144" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B145" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C145" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D145" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B146" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C146" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D146" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B147" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C147" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D147" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B148" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C148" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D148" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B149" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C149" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D149" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B150" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C150" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D150" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B151" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="C151" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="D151" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B152" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C152" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="D152" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B153" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C153" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="D153" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B154" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C154" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="D154" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B155" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C155" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="D155" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B156" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C156" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D156" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B157" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C157" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="D157" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="B158" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C158" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="D158" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B159" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C159" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D159" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="B160" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="C160" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="D160" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B161" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C161" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="D161" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="B162" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="C162" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="D162" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="B163" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C163" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="D163" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="B164" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="C164" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="D164" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="B165" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="C165" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="D165" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B166" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="C166" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D166" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B167" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C167" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D167" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B168" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C168" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="D168" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="B169" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="C169" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="D169" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B170" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C170" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D170" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B171" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="C171" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="D171" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B172" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="C172" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="D172" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B173" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C173" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D173" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B174" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="C174" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D174" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B175" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C175" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D175" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="B176" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="C176" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="D176" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="B177" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="C177" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="D177" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="B178" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="C178" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="D178" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="B179" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="C179" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D179" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="B180" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="C180" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="D180" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="B181" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="C181" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="D181" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="B182" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="C182" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D182" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="B183" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="C183" t="s">
-        <v>963</v>
+        <v>620</v>
       </c>
       <c r="D183" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B184" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="C184" t="s">
-        <v>964</v>
+        <v>620</v>
       </c>
       <c r="D184" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="B185" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="C185" t="s">
-        <v>633</v>
+        <v>963</v>
       </c>
       <c r="D185" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="B186" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="C186" t="s">
-        <v>637</v>
+        <v>964</v>
       </c>
       <c r="D186" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="B187" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="C187" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="D187" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="B188" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="C188" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="D188" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="B189" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="C189" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="D189" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="B190" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="C190" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="D190" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="B191" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="C191" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="D191" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="B192" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="C192" t="s">
-        <v>965</v>
+        <v>653</v>
       </c>
       <c r="D192" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="B193" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="C193" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="D193" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="B194" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="C194" t="s">
-        <v>668</v>
+        <v>965</v>
       </c>
       <c r="D194" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B195" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="C195" t="s">
-        <v>966</v>
+        <v>664</v>
       </c>
       <c r="D195" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="B196" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="C196" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="D196" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="B197" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="C197" t="s">
-        <v>679</v>
+        <v>966</v>
       </c>
       <c r="D197" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="B198" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="C198" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D198" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="B199" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="C199" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="D199" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B200" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="C200" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="D200" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="B201" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="C201" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="D201" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="B202" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C202" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D202" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="B203" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="C203" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="D203" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="B204" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="C204" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="D204" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="B205" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="C205" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="D205" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="B206" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="C206" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="D206" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="B207" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="C207" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="D207" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="B208" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="C208" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="D208" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="B209" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="C209" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="D209" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="B210" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="C210" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="D210" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="B211" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="C211" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="D211" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="B212" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="C212" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="D212" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="B213" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="C213" t="s">
-        <v>967</v>
+        <v>734</v>
       </c>
       <c r="D213" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="B214" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
       <c r="C214" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="D214" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="B215" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="C215" t="s">
-        <v>748</v>
+        <v>967</v>
       </c>
       <c r="D215" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
       <c r="B216" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
       <c r="C216" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="D216" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="B217" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="C217" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="D217" t="s">
-        <v>595</v>
+        <v>749</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="B218" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="C218" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="D218" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="B219" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="C219" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="D219" t="s">
-        <v>764</v>
+        <v>595</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="B220" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="C220" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="D220" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="B221" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="C221" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="D221" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="B222" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="C222" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="D222" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B223" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="C223" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="D223" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B224" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="C224" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="D224" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="B225" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="C225" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="D225" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B226" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="C226" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="D226" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B227" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="C227" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="D227" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="B228" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="C228" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="D228" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="B229" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="C229" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="D229" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="B230" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="C230" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="D230" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="B231" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="C231" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="D231" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="B232" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="C232" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="D232" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="B233" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="C233" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="D233" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="B234" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="C234" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="D234" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="B235" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="C235" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="D235" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="B236" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="C236" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D236" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="B237" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="C237" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="D237" t="s">
-        <v>835</v>
+        <v>828</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
       <c r="B238" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="C238" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="D238" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="B239" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="C239" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
       <c r="D239" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="B240" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="C240" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="D240" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="B241" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="C241" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="D241" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="B242" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="C242" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="D242" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="B243" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="C243" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="D243" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="B244" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="C244" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="D244" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="B245" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="C245" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="D245" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="B246" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="C246" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="D246" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="B247" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="C247" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="D247" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="B248" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="C248" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="D248" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="B249" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="C249" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="D249" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
+        <v>876</v>
+      </c>
+      <c r="B250" t="s">
+        <v>877</v>
+      </c>
+      <c r="C250" t="s">
+        <v>878</v>
+      </c>
+      <c r="D250" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>880</v>
+      </c>
+      <c r="B251" t="s">
+        <v>881</v>
+      </c>
+      <c r="C251" t="s">
+        <v>882</v>
+      </c>
+      <c r="D251" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
         <v>884</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B252" t="s">
         <v>885</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C252" t="s">
         <v>886</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D252" t="s">
         <v>887</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add EB 101.5 (ZA8900)
</commit_message>
<xml_diff>
--- a/survey-metadata/eb_waves_filenames.xlsx
+++ b/survey-metadata/eb_waves_filenames.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\harmonization-toolbox\survey-metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MK\Documents\Work in progress\harmonization-toolbox\survey-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52615E27-C10F-42AF-857C-1213A0C00555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E00CDF-C885-4429-AD81-B5BAC5E2E110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="991">
   <si>
     <t>archive_id</t>
   </si>
@@ -2981,6 +2986,18 @@
   </si>
   <si>
     <t>Standard Eurobarometer 101</t>
+  </si>
+  <si>
+    <t>ZA8900</t>
+  </si>
+  <si>
+    <t>101.5</t>
+  </si>
+  <si>
+    <t>June-July 2024</t>
+  </si>
+  <si>
+    <t>European Parliament EU Post-Electoral Survey 2024</t>
   </si>
 </sst>
 </file>
@@ -3315,19 +3332,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D252"/>
+  <dimension ref="A1:D253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.53515625" customWidth="1"/>
+    <col min="3" max="3" width="26.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3341,3502 +3358,3516 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="C2" t="s">
+        <v>989</v>
+      </c>
+      <c r="D2" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>981</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>983</v>
-      </c>
-      <c r="C2" t="s">
-        <v>984</v>
-      </c>
-      <c r="D2" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>980</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>982</v>
       </c>
       <c r="C3" t="s">
         <v>984</v>
       </c>
       <c r="D3" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>980</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C4" t="s">
+        <v>984</v>
+      </c>
+      <c r="D4" t="s">
         <v>986</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>971</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>972</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>973</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>951</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>953</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>968</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>970</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>947</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>949</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>978</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>977</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>939</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>942</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>955</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>958</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>957</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>935</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>938</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>943</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>945</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>929</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>930</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>933</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>927</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>928</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>931</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>923</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>926</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>915</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>916</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>917</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>911</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>912</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>913</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>899</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>900</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>901</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>907</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>908</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>909</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>891</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>893</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>895</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>898</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>888</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>890</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>918</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>919</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>920</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>13</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>18</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>902</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>26</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>34</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>38</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>42</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>46</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>48</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>49</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>52</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>53</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>55</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>56</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>57</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>59</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>60</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>61</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
         <v>63</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>64</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>65</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>67</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>68</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>70</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>71</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>72</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>74</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>75</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>77</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>78</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>79</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>81</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>82</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>83</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
         <v>85</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>86</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>87</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>89</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>90</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>92</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>93</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>94</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>96</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>97</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>98</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>100</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>101</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>102</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>104</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>105</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
         <v>107</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>108</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>109</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>111</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>112</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>113</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>115</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>116</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>117</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>119</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>120</v>
-      </c>
-      <c r="C55" t="s">
-        <v>121</v>
-      </c>
-      <c r="D55" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B56" t="s">
-        <v>124</v>
       </c>
       <c r="C56" t="s">
         <v>121</v>
       </c>
       <c r="D56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
         <v>126</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>127</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>128</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>130</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>131</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>132</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
         <v>134</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>135</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>136</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
         <v>138</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>139</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>140</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>142</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>143</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>144</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>146</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>147</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>148</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>150</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>151</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>152</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
         <v>154</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>155</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>156</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
         <v>158</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>159</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>160</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
         <v>162</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>163</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>164</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
         <v>166</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>167</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>168</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
         <v>170</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>171</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>172</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
         <v>174</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>175</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>176</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
         <v>178</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>179</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>180</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
         <v>182</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>183</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>184</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
         <v>186</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>187</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>188</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
         <v>190</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>191</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>192</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
         <v>194</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>195</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>196</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
         <v>198</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>199</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>200</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
         <v>202</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>203</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>204</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
         <v>206</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>207</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>208</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
         <v>210</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>211</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>212</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
         <v>214</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>215</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>216</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
         <v>218</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>219</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>220</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
         <v>222</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>223</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>224</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
         <v>226</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>227</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>228</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
         <v>230</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>231</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>232</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
         <v>234</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>235</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>236</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
         <v>238</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>239</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>240</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
         <v>242</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>243</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>959</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
         <v>245</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>246</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>247</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
         <v>249</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>250</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>251</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
         <v>253</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>254</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>960</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
         <v>256</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>257</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>258</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
         <v>260</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>261</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>262</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
         <v>264</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>265</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>266</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
         <v>268</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>269</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>270</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
         <v>272</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>273</v>
-      </c>
-      <c r="C94" t="s">
-        <v>961</v>
-      </c>
-      <c r="D94" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>275</v>
-      </c>
-      <c r="B95" t="s">
-        <v>276</v>
       </c>
       <c r="C95" t="s">
         <v>961</v>
       </c>
       <c r="D95" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>275</v>
+      </c>
+      <c r="B96" t="s">
+        <v>276</v>
+      </c>
+      <c r="C96" t="s">
+        <v>961</v>
+      </c>
+      <c r="D96" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
         <v>278</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>279</v>
-      </c>
-      <c r="C96" t="s">
-        <v>280</v>
-      </c>
-      <c r="D96" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>282</v>
-      </c>
-      <c r="B97" t="s">
-        <v>283</v>
       </c>
       <c r="C97" t="s">
         <v>280</v>
       </c>
       <c r="D97" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
+        <v>282</v>
+      </c>
+      <c r="B98" t="s">
+        <v>283</v>
+      </c>
+      <c r="C98" t="s">
+        <v>280</v>
+      </c>
+      <c r="D98" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
         <v>285</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>286</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>962</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
         <v>288</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>289</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>290</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
         <v>292</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>293</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>294</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
         <v>296</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>297</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>298</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
         <v>300</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>301</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>302</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
         <v>304</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>305</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>306</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
         <v>308</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>309</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>310</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D105" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
         <v>312</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>313</v>
-      </c>
-      <c r="C105" t="s">
-        <v>314</v>
-      </c>
-      <c r="D105" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>316</v>
-      </c>
-      <c r="B106" t="s">
-        <v>317</v>
       </c>
       <c r="C106" t="s">
         <v>314</v>
       </c>
       <c r="D106" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
+        <v>316</v>
+      </c>
+      <c r="B107" t="s">
+        <v>317</v>
+      </c>
+      <c r="C107" t="s">
+        <v>314</v>
+      </c>
+      <c r="D107" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
         <v>319</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>320</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>321</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
         <v>323</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>324</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>325</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D109" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
         <v>327</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>328</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>329</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D110" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
         <v>331</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>332</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>333</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D111" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
         <v>335</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>336</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>337</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
         <v>339</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>340</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" t="s">
         <v>341</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D113" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
         <v>343</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>344</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>345</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
         <v>347</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>348</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>349</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D115" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
         <v>351</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>352</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" t="s">
         <v>353</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D116" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
         <v>355</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>356</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>357</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D117" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
         <v>359</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" t="s">
         <v>360</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" t="s">
         <v>361</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D118" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
         <v>363</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" t="s">
         <v>364</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>365</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D119" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
         <v>367</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>368</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>369</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D120" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
         <v>371</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" t="s">
         <v>372</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>373</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D121" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
         <v>375</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>376</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" t="s">
         <v>377</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D122" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
         <v>379</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>380</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>381</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D123" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
         <v>383</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>384</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C124" t="s">
         <v>385</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D124" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
         <v>387</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>388</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C125" t="s">
         <v>389</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D125" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
         <v>391</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>392</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>393</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D126" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
         <v>395</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" t="s">
         <v>396</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C127" t="s">
         <v>397</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D127" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
         <v>399</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" t="s">
         <v>400</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C128" t="s">
         <v>922</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D128" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
         <v>402</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>403</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>404</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
         <v>406</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>407</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C130" t="s">
         <v>408</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D130" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
         <v>410</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" t="s">
         <v>411</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>412</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A132" t="s">
         <v>414</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>415</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>416</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D132" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
         <v>418</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>419</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>420</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D133" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
         <v>422</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B134" t="s">
         <v>423</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>424</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D134" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
         <v>426</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>427</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C135" t="s">
         <v>428</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D135" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A136" t="s">
         <v>430</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B136" t="s">
         <v>431</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>432</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D136" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A137" t="s">
         <v>434</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>435</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>436</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A138" t="s">
         <v>438</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" t="s">
         <v>439</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C138" t="s">
         <v>440</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D138" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A139" t="s">
         <v>442</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>443</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C139" t="s">
         <v>444</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D139" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A140" t="s">
         <v>446</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>447</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C140" t="s">
         <v>448</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D140" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A141" t="s">
         <v>450</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B141" t="s">
         <v>451</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C141" t="s">
         <v>452</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D141" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A142" t="s">
         <v>454</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>455</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C142" t="s">
         <v>456</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D142" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
         <v>458</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B143" t="s">
         <v>459</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C143" t="s">
         <v>460</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D143" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
         <v>462</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" t="s">
         <v>463</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C144" t="s">
         <v>464</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D144" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
         <v>466</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>467</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C145" t="s">
         <v>468</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D145" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
         <v>470</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>471</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C146" t="s">
         <v>472</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D146" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A147" t="s">
         <v>474</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>475</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C147" t="s">
         <v>476</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D147" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A148" t="s">
         <v>478</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>479</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C148" t="s">
         <v>480</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D148" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A149" t="s">
         <v>482</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>483</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>484</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D149" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A150" t="s">
         <v>486</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>487</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C150" t="s">
         <v>488</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D150" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A151" t="s">
         <v>490</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>491</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C151" t="s">
         <v>492</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D151" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A152" t="s">
         <v>494</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B152" t="s">
         <v>495</v>
-      </c>
-      <c r="C151" t="s">
-        <v>496</v>
-      </c>
-      <c r="D151" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>498</v>
-      </c>
-      <c r="B152" t="s">
-        <v>499</v>
       </c>
       <c r="C152" t="s">
         <v>496</v>
       </c>
       <c r="D152" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
+        <v>498</v>
+      </c>
+      <c r="B153" t="s">
+        <v>499</v>
+      </c>
+      <c r="C153" t="s">
+        <v>496</v>
+      </c>
+      <c r="D153" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
         <v>501</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B154" t="s">
         <v>502</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C154" t="s">
         <v>503</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D154" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
         <v>505</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B155" t="s">
         <v>506</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C155" t="s">
         <v>507</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D155" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
         <v>509</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" t="s">
         <v>510</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C156" t="s">
         <v>511</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D156" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A157" t="s">
         <v>513</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" t="s">
         <v>514</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C157" t="s">
         <v>515</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D157" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A158" t="s">
         <v>517</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B158" t="s">
         <v>518</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C158" t="s">
         <v>519</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D158" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A159" t="s">
         <v>521</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B159" t="s">
         <v>522</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C159" t="s">
         <v>523</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D159" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
         <v>525</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B160" t="s">
         <v>526</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C160" t="s">
         <v>527</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D160" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
         <v>529</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" t="s">
         <v>530</v>
-      </c>
-      <c r="C160" t="s">
-        <v>531</v>
-      </c>
-      <c r="D160" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>533</v>
-      </c>
-      <c r="B161" t="s">
-        <v>534</v>
       </c>
       <c r="C161" t="s">
         <v>531</v>
       </c>
       <c r="D161" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A162" t="s">
+        <v>533</v>
+      </c>
+      <c r="B162" t="s">
+        <v>534</v>
+      </c>
+      <c r="C162" t="s">
+        <v>531</v>
+      </c>
+      <c r="D162" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
         <v>536</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" t="s">
         <v>537</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C163" t="s">
         <v>538</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D163" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
         <v>540</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B164" t="s">
         <v>541</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C164" t="s">
         <v>542</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D164" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
         <v>544</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B165" t="s">
         <v>545</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C165" t="s">
         <v>546</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D165" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
         <v>548</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>549</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C166" t="s">
         <v>550</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D166" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
         <v>552</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B167" t="s">
         <v>553</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C167" t="s">
         <v>554</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D167" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
         <v>556</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" t="s">
         <v>557</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C168" t="s">
         <v>558</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D168" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
         <v>560</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" t="s">
         <v>561</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C169" t="s">
         <v>562</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D169" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
         <v>564</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" t="s">
         <v>565</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" t="s">
         <v>566</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D170" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
         <v>568</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" t="s">
         <v>569</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C171" t="s">
         <v>570</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D171" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A172" t="s">
         <v>572</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>573</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C172" t="s">
         <v>574</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D172" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A173" t="s">
         <v>576</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B173" t="s">
         <v>577</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C173" t="s">
         <v>578</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D173" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A174" t="s">
         <v>580</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B174" t="s">
         <v>581</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" t="s">
         <v>582</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D174" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
         <v>584</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B175" t="s">
         <v>585</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C175" t="s">
         <v>586</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D175" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A176" t="s">
         <v>588</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B176" t="s">
         <v>589</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>590</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D176" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
         <v>592</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B177" t="s">
         <v>593</v>
-      </c>
-      <c r="C176" t="s">
-        <v>594</v>
-      </c>
-      <c r="D176" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
-        <v>596</v>
-      </c>
-      <c r="B177" t="s">
-        <v>597</v>
       </c>
       <c r="C177" t="s">
         <v>594</v>
       </c>
       <c r="D177" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>596</v>
+      </c>
+      <c r="B178" t="s">
+        <v>597</v>
+      </c>
+      <c r="C178" t="s">
+        <v>594</v>
+      </c>
+      <c r="D178" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A179" t="s">
         <v>599</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" t="s">
         <v>600</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C179" t="s">
         <v>601</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D179" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
         <v>603</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B180" t="s">
         <v>604</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C180" t="s">
         <v>605</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D180" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
         <v>607</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B181" t="s">
         <v>608</v>
-      </c>
-      <c r="C180" t="s">
-        <v>609</v>
-      </c>
-      <c r="D180" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
-        <v>611</v>
-      </c>
-      <c r="B181" t="s">
-        <v>612</v>
       </c>
       <c r="C181" t="s">
         <v>609</v>
       </c>
       <c r="D181" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A182" t="s">
+        <v>611</v>
+      </c>
+      <c r="B182" t="s">
+        <v>612</v>
+      </c>
+      <c r="C182" t="s">
+        <v>609</v>
+      </c>
+      <c r="D182" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
         <v>614</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B183" t="s">
         <v>615</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C183" t="s">
         <v>616</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D183" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A184" t="s">
         <v>618</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" t="s">
         <v>619</v>
-      </c>
-      <c r="C183" t="s">
-        <v>620</v>
-      </c>
-      <c r="D183" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
-        <v>622</v>
-      </c>
-      <c r="B184" t="s">
-        <v>623</v>
       </c>
       <c r="C184" t="s">
         <v>620</v>
       </c>
       <c r="D184" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>622</v>
+      </c>
+      <c r="B185" t="s">
+        <v>623</v>
+      </c>
+      <c r="C185" t="s">
+        <v>620</v>
+      </c>
+      <c r="D185" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
         <v>625</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B186" t="s">
         <v>626</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C186" t="s">
         <v>963</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D186" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
         <v>628</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B187" t="s">
         <v>629</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C187" t="s">
         <v>964</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D187" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A188" t="s">
         <v>631</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B188" t="s">
         <v>632</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C188" t="s">
         <v>633</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D188" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A189" t="s">
         <v>635</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B189" t="s">
         <v>636</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C189" t="s">
         <v>637</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D189" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A190" t="s">
         <v>639</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B190" t="s">
         <v>640</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C190" t="s">
         <v>641</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D190" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A191" t="s">
         <v>643</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B191" t="s">
         <v>644</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C191" t="s">
         <v>645</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D191" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A192" t="s">
         <v>647</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B192" t="s">
         <v>648</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C192" t="s">
         <v>649</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D192" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
         <v>651</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" t="s">
         <v>652</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C193" t="s">
         <v>653</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D193" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A194" t="s">
         <v>655</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B194" t="s">
         <v>656</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C194" t="s">
         <v>657</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D194" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A195" t="s">
         <v>659</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B195" t="s">
         <v>660</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C195" t="s">
         <v>965</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D195" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A196" t="s">
         <v>662</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B196" t="s">
         <v>663</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C196" t="s">
         <v>664</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D196" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A197" t="s">
         <v>666</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B197" t="s">
         <v>667</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C197" t="s">
         <v>668</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D197" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
         <v>670</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B198" t="s">
         <v>671</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C198" t="s">
         <v>966</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D198" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A199" t="s">
         <v>673</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B199" t="s">
         <v>674</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C199" t="s">
         <v>675</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D199" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A200" t="s">
         <v>677</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B200" t="s">
         <v>678</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C200" t="s">
         <v>679</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D200" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A201" t="s">
         <v>681</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>682</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C201" t="s">
         <v>683</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D201" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
         <v>685</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>686</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C202" t="s">
         <v>687</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D202" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A203" t="s">
         <v>689</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B203" t="s">
         <v>690</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C203" t="s">
         <v>691</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D203" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A204" t="s">
         <v>693</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B204" t="s">
         <v>694</v>
-      </c>
-      <c r="C203" t="s">
-        <v>695</v>
-      </c>
-      <c r="D203" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
-        <v>697</v>
-      </c>
-      <c r="B204" t="s">
-        <v>698</v>
       </c>
       <c r="C204" t="s">
         <v>695</v>
       </c>
       <c r="D204" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A205" t="s">
+        <v>697</v>
+      </c>
+      <c r="B205" t="s">
+        <v>698</v>
+      </c>
+      <c r="C205" t="s">
+        <v>695</v>
+      </c>
+      <c r="D205" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A206" t="s">
         <v>700</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" t="s">
         <v>701</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C206" t="s">
         <v>702</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D206" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A207" t="s">
         <v>704</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B207" t="s">
         <v>705</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C207" t="s">
         <v>706</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D207" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A208" t="s">
         <v>708</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B208" t="s">
         <v>709</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C208" t="s">
         <v>710</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D208" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A209" t="s">
         <v>712</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B209" t="s">
         <v>713</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C209" t="s">
         <v>714</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D209" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A210" t="s">
         <v>716</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B210" t="s">
         <v>717</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C210" t="s">
         <v>718</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D210" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A210" t="s">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A211" t="s">
         <v>720</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B211" t="s">
         <v>721</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C211" t="s">
         <v>722</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D211" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A212" t="s">
         <v>724</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" t="s">
         <v>725</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C212" t="s">
         <v>726</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D212" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A213" t="s">
         <v>728</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B213" t="s">
         <v>729</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C213" t="s">
         <v>730</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D213" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A213" t="s">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A214" t="s">
         <v>732</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" t="s">
         <v>733</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C214" t="s">
         <v>734</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D214" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A214" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A215" t="s">
         <v>736</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B215" t="s">
         <v>737</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C215" t="s">
         <v>738</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D215" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A215" t="s">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A216" t="s">
         <v>740</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B216" t="s">
         <v>741</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C216" t="s">
         <v>967</v>
-      </c>
-      <c r="D215" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A216" t="s">
-        <v>743</v>
-      </c>
-      <c r="B216" t="s">
-        <v>744</v>
-      </c>
-      <c r="C216" t="s">
-        <v>745</v>
       </c>
       <c r="D216" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A217" t="s">
+        <v>743</v>
+      </c>
+      <c r="B217" t="s">
+        <v>744</v>
+      </c>
+      <c r="C217" t="s">
+        <v>745</v>
+      </c>
+      <c r="D217" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A218" t="s">
         <v>746</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B218" t="s">
         <v>747</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C218" t="s">
         <v>748</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D218" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
         <v>750</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B219" t="s">
         <v>751</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C219" t="s">
         <v>752</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D219" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A219" t="s">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A220" t="s">
         <v>754</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B220" t="s">
         <v>755</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C220" t="s">
         <v>756</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D220" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A221" t="s">
         <v>757</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B221" t="s">
         <v>758</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C221" t="s">
         <v>759</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D221" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A221" t="s">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A222" t="s">
         <v>761</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>762</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C222" t="s">
         <v>763</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D222" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A222" t="s">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A223" t="s">
         <v>765</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B223" t="s">
         <v>766</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C223" t="s">
         <v>767</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D223" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A223" t="s">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A224" t="s">
         <v>769</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B224" t="s">
         <v>770</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C224" t="s">
         <v>771</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D224" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A224" t="s">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A225" t="s">
         <v>773</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B225" t="s">
         <v>774</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C225" t="s">
         <v>775</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D225" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A225" t="s">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A226" t="s">
         <v>777</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B226" t="s">
         <v>778</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C226" t="s">
         <v>779</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D226" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A226" t="s">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A227" t="s">
         <v>781</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B227" t="s">
         <v>782</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C227" t="s">
         <v>783</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D227" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A227" t="s">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A228" t="s">
         <v>785</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B228" t="s">
         <v>786</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C228" t="s">
         <v>787</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D228" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A228" t="s">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A229" t="s">
         <v>789</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B229" t="s">
         <v>790</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C229" t="s">
         <v>791</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D229" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A229" t="s">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A230" t="s">
         <v>793</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B230" t="s">
         <v>794</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C230" t="s">
         <v>795</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D230" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A230" t="s">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A231" t="s">
         <v>797</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>798</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C231" t="s">
         <v>799</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D231" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
         <v>801</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>802</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C232" t="s">
         <v>803</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D232" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A232" t="s">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A233" t="s">
         <v>805</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>806</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C233" t="s">
         <v>807</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D233" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A233" t="s">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A234" t="s">
         <v>809</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>810</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C234" t="s">
         <v>811</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D234" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A234" t="s">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A235" t="s">
         <v>813</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>814</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C235" t="s">
         <v>815</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D235" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A236" t="s">
         <v>817</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B236" t="s">
         <v>818</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C236" t="s">
         <v>819</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D236" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A237" t="s">
         <v>821</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B237" t="s">
         <v>822</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C237" t="s">
         <v>823</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D237" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A237" t="s">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A238" t="s">
         <v>825</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B238" t="s">
         <v>826</v>
       </c>
-      <c r="C237" t="s">
+      <c r="C238" t="s">
         <v>827</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D238" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A239" t="s">
         <v>829</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B239" t="s">
         <v>830</v>
-      </c>
-      <c r="C238" t="s">
-        <v>831</v>
-      </c>
-      <c r="D238" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
-        <v>833</v>
-      </c>
-      <c r="B239" t="s">
-        <v>834</v>
       </c>
       <c r="C239" t="s">
         <v>831</v>
       </c>
       <c r="D239" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A240" t="s">
+        <v>833</v>
+      </c>
+      <c r="B240" t="s">
+        <v>834</v>
+      </c>
+      <c r="C240" t="s">
+        <v>831</v>
+      </c>
+      <c r="D240" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A241" t="s">
         <v>836</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B241" t="s">
         <v>837</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C241" t="s">
         <v>838</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D241" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A242" t="s">
         <v>840</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B242" t="s">
         <v>841</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C242" t="s">
         <v>842</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D242" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A243" t="s">
         <v>844</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>845</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C243" t="s">
         <v>846</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D243" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A244" t="s">
         <v>848</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B244" t="s">
         <v>849</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C244" t="s">
         <v>850</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D244" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A245" t="s">
         <v>852</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B245" t="s">
         <v>853</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C245" t="s">
         <v>854</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D245" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A246" t="s">
         <v>856</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B246" t="s">
         <v>857</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C246" t="s">
         <v>858</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D246" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A247" t="s">
         <v>860</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>861</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C247" t="s">
         <v>862</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D247" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A248" t="s">
         <v>864</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B248" t="s">
         <v>865</v>
       </c>
-      <c r="C247" t="s">
+      <c r="C248" t="s">
         <v>866</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D248" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A249" t="s">
         <v>868</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B249" t="s">
         <v>869</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C249" t="s">
         <v>870</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D249" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A250" t="s">
         <v>872</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B250" t="s">
         <v>873</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C250" t="s">
         <v>874</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D250" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A251" t="s">
         <v>876</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B251" t="s">
         <v>877</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C251" t="s">
         <v>878</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D251" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A252" t="s">
         <v>880</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B252" t="s">
         <v>881</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C252" t="s">
         <v>882</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D252" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A252" t="s">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A253" t="s">
         <v>884</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B253" t="s">
         <v>885</v>
       </c>
-      <c r="C252" t="s">
+      <c r="C253" t="s">
         <v>886</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D253" t="s">
         <v>887</v>
       </c>
     </row>

</xml_diff>